<commit_message>
Add new quant metrics, remodelled main.py
</commit_message>
<xml_diff>
--- a/output/stock_analysis_scores.xlsx
+++ b/output/stock_analysis_scores.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK27"/>
+  <dimension ref="A1:BA27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -496,120 +496,200 @@
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
+          <t>pe_ratio</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>ps_ratio</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>pb_ratio</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>ev_ebitda</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>beta</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>scaled_vol</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>accrual_rat</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>cash_conv_rat</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
           <t>Quant Score</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>revenue_growth_rank</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>eps_growth_rank</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>fcf_growth_rank</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>net_margin_avg_rank</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>gross_margin_avg_rank</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>net_margin_avg_rank</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>fcf_growth_rank</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>d_e_ratio_rank</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>curr_ratio_rank</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>quick_ratio_rank</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="AE1" s="1" t="inlineStr">
         <is>
           <t>z_score_rank</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="AF1" s="1" t="inlineStr">
         <is>
           <t>no_y_pos_eps_rank</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AG1" s="1" t="inlineStr">
         <is>
           <t>no_y_pos_fcf_rank</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="AH1" s="1" t="inlineStr">
         <is>
           <t>shares_chg_rank</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>pe_ratio_rank</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>ps_ratio_rank</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>pb_ratio_rank</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>ev_ebitda_rank</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>beta_rank</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>scaled_vol_rank</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>accrual_rat_rank</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>cash_conv_rat_rank</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
         <is>
           <t>Quant Score_rank</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="AR1" s="1" t="inlineStr">
         <is>
           <t>MOAT Text Score</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="AS1" s="1" t="inlineStr">
         <is>
           <t>MOAT Quant Score</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="AT1" s="1" t="inlineStr">
         <is>
           <t>Management Score</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="AU1" s="1" t="inlineStr">
         <is>
           <t>Sentiment Score</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>Qual Score</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>External Rating Score</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>Quant Rank</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>Qual Rank</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>Final Rank</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>External Rating Rank</t>
         </is>
@@ -646,7 +726,7 @@
         <v>13.46804231755159</v>
       </c>
       <c r="J2" t="n">
-        <v>10.04559993226093</v>
+        <v>10.00165548536846</v>
       </c>
       <c r="K2" t="n">
         <v>40</v>
@@ -658,34 +738,34 @@
         <v>0.8404482390608314</v>
       </c>
       <c r="N2" t="n">
-        <v>20.91453633014669</v>
+        <v>-34.051506</v>
       </c>
       <c r="O2" t="n">
+        <v>-13.431593</v>
+      </c>
+      <c r="P2" t="n">
+        <v>-11.017878</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-24.295</v>
+      </c>
+      <c r="R2" t="n">
+        <v>-104</v>
+      </c>
+      <c r="S2" t="n">
+        <v>-14.82592935155069</v>
+      </c>
+      <c r="T2" t="n">
+        <v>5.546015124320884</v>
+      </c>
+      <c r="U2" t="n">
+        <v>13.3712389032917</v>
+      </c>
+      <c r="V2" t="n">
+        <v>15.68985484006297</v>
+      </c>
+      <c r="W2" t="n">
         <v>12</v>
-      </c>
-      <c r="P2" t="n">
-        <v>11</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>8</v>
-      </c>
-      <c r="R2" t="n">
-        <v>3</v>
-      </c>
-      <c r="S2" t="n">
-        <v>10</v>
-      </c>
-      <c r="T2" t="n">
-        <v>7</v>
-      </c>
-      <c r="U2" t="n">
-        <v>18</v>
-      </c>
-      <c r="V2" t="n">
-        <v>16</v>
-      </c>
-      <c r="W2" t="n">
-        <v>10</v>
       </c>
       <c r="X2" t="n">
         <v>11</v>
@@ -694,39 +774,87 @@
         <v>10</v>
       </c>
       <c r="Z2" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="AA2" t="n">
         <v>8</v>
       </c>
       <c r="AB2" t="n">
+        <v>7</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>18</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>16</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>10</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>11</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>15</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>18</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>22</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>16</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>16</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>11</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>5</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>12</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>13</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>9</v>
+      </c>
+      <c r="AR2" t="n">
         <v>3</v>
       </c>
-      <c r="AC2" t="n">
-        <v>10</v>
-      </c>
-      <c r="AD2" t="n">
+      <c r="AS2" t="n">
+        <v>10</v>
+      </c>
+      <c r="AT2" t="n">
         <v>8</v>
       </c>
-      <c r="AE2" t="n">
+      <c r="AU2" t="n">
         <v>8.360000000000001</v>
       </c>
-      <c r="AF2" t="n">
+      <c r="AV2" t="n">
         <v>7.354000000000001</v>
       </c>
-      <c r="AG2" t="n">
+      <c r="AW2" t="n">
         <v>0</v>
       </c>
-      <c r="AH2" t="n">
-        <v>8</v>
-      </c>
-      <c r="AI2" t="n">
+      <c r="AX2" t="n">
+        <v>9</v>
+      </c>
+      <c r="AY2" t="n">
         <v>6</v>
       </c>
-      <c r="AJ2" t="n">
-        <v>8.833333333333334</v>
-      </c>
-      <c r="AK2" t="n">
+      <c r="AZ2" t="n">
+        <v>9.166666666666666</v>
+      </c>
+      <c r="BA2" t="n">
         <v>12.5</v>
       </c>
     </row>
@@ -761,7 +889,7 @@
         <v>8.260068483831466</v>
       </c>
       <c r="J3" t="n">
-        <v>9.435932938400249</v>
+        <v>9.307753432726127</v>
       </c>
       <c r="K3" t="n">
         <v>40</v>
@@ -773,75 +901,123 @@
         <v>8.128057551544575</v>
       </c>
       <c r="N3" t="n">
-        <v>12.93529328914392</v>
+        <v>-30.27557</v>
       </c>
       <c r="O3" t="n">
+        <v>-9.137214</v>
+      </c>
+      <c r="P3" t="n">
+        <v>-56.779503</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>-26.974</v>
+      </c>
+      <c r="R3" t="n">
+        <v>-110.9</v>
+      </c>
+      <c r="S3" t="n">
+        <v>-3.393508415778721</v>
+      </c>
+      <c r="T3" t="n">
+        <v>6.717628363197983</v>
+      </c>
+      <c r="U3" t="n">
+        <v>12.61564393616113</v>
+      </c>
+      <c r="V3" t="n">
+        <v>8.806003258094938</v>
+      </c>
+      <c r="W3" t="n">
         <v>20</v>
       </c>
-      <c r="P3" t="n">
+      <c r="X3" t="n">
         <v>17</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="Y3" t="n">
+        <v>8</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>8</v>
+      </c>
+      <c r="AA3" t="n">
         <v>19</v>
       </c>
-      <c r="R3" t="n">
+      <c r="AB3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>23</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>12</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>11</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>4</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>12</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>16</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>24</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>17</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>12</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>7</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>16</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>17</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AT3" t="n">
         <v>8</v>
       </c>
-      <c r="S3" t="n">
-        <v>8</v>
-      </c>
-      <c r="T3" t="n">
-        <v>23</v>
-      </c>
-      <c r="U3" t="n">
-        <v>23</v>
-      </c>
-      <c r="V3" t="n">
-        <v>23</v>
-      </c>
-      <c r="W3" t="n">
-        <v>12</v>
-      </c>
-      <c r="X3" t="n">
-        <v>11</v>
-      </c>
-      <c r="Y3" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z3" t="n">
-        <v>4</v>
-      </c>
-      <c r="AA3" t="n">
-        <v>18</v>
-      </c>
-      <c r="AB3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC3" t="n">
-        <v>10</v>
-      </c>
-      <c r="AD3" t="n">
-        <v>8</v>
-      </c>
-      <c r="AE3" t="n">
+      <c r="AU3" t="n">
         <v>7.359999999999999</v>
       </c>
-      <c r="AF3" t="n">
+      <c r="AV3" t="n">
         <v>6.604</v>
       </c>
-      <c r="AG3" t="n">
+      <c r="AW3" t="n">
         <v>-1</v>
       </c>
-      <c r="AH3" t="n">
-        <v>18</v>
-      </c>
-      <c r="AI3" t="n">
-        <v>10</v>
-      </c>
-      <c r="AJ3" t="n">
-        <v>14.5</v>
-      </c>
-      <c r="AK3" t="n">
+      <c r="AX3" t="n">
+        <v>17</v>
+      </c>
+      <c r="AY3" t="n">
+        <v>10</v>
+      </c>
+      <c r="AZ3" t="n">
+        <v>14.16666666666667</v>
+      </c>
+      <c r="BA3" t="n">
         <v>15.5</v>
       </c>
     </row>
@@ -876,7 +1052,7 @@
         <v>18.36931397410292</v>
       </c>
       <c r="J4" t="n">
-        <v>17.26638005613679</v>
+        <v>17.00455522292808</v>
       </c>
       <c r="K4" t="n">
         <v>40</v>
@@ -888,75 +1064,123 @@
         <v>7.743578222122371</v>
       </c>
       <c r="N4" t="n">
-        <v>20.12825941708499</v>
+        <v>-27.662947</v>
       </c>
       <c r="O4" t="n">
+        <v>-8.080947</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-8.266685000000001</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-21.23</v>
+      </c>
+      <c r="R4" t="n">
+        <v>-101.1</v>
+      </c>
+      <c r="S4" t="n">
+        <v>-21.22957880377664</v>
+      </c>
+      <c r="T4" t="n">
+        <v>5.592596211932767</v>
+      </c>
+      <c r="U4" t="n">
+        <v>12.51513214407</v>
+      </c>
+      <c r="V4" t="n">
+        <v>15.49746343477449</v>
+      </c>
+      <c r="W4" t="n">
         <v>15</v>
       </c>
-      <c r="P4" t="n">
-        <v>10</v>
-      </c>
-      <c r="Q4" t="n">
+      <c r="X4" t="n">
+        <v>10</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>11</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>9</v>
+      </c>
+      <c r="AA4" t="n">
         <v>12</v>
       </c>
-      <c r="R4" t="n">
-        <v>9</v>
-      </c>
-      <c r="S4" t="n">
+      <c r="AB4" t="n">
+        <v>4</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>13</v>
+      </c>
+      <c r="AD4" t="n">
         <v>11</v>
       </c>
-      <c r="T4" t="n">
-        <v>4</v>
-      </c>
-      <c r="U4" t="n">
+      <c r="AE4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>11</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>5</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>10</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>12</v>
+      </c>
+      <c r="AK4" t="n">
         <v>13</v>
       </c>
-      <c r="V4" t="n">
+      <c r="AL4" t="n">
+        <v>15</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>10</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>7</v>
+      </c>
+      <c r="AO4" t="n">
         <v>11</v>
       </c>
-      <c r="W4" t="n">
+      <c r="AP4" t="n">
+        <v>18</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>10</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>8</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>10</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>7</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>9.24</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>8.836</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>2</v>
+      </c>
+      <c r="AX4" t="n">
+        <v>10</v>
+      </c>
+      <c r="AY4" t="n">
+        <v>3</v>
+      </c>
+      <c r="AZ4" t="n">
         <v>5</v>
       </c>
-      <c r="X4" t="n">
-        <v>11</v>
-      </c>
-      <c r="Y4" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z4" t="n">
-        <v>5</v>
-      </c>
-      <c r="AA4" t="n">
-        <v>10</v>
-      </c>
-      <c r="AB4" t="n">
-        <v>8</v>
-      </c>
-      <c r="AC4" t="n">
-        <v>10</v>
-      </c>
-      <c r="AD4" t="n">
-        <v>7</v>
-      </c>
-      <c r="AE4" t="n">
-        <v>9.24</v>
-      </c>
-      <c r="AF4" t="n">
-        <v>8.836</v>
-      </c>
-      <c r="AG4" t="n">
-        <v>2</v>
-      </c>
-      <c r="AH4" t="n">
-        <v>10</v>
-      </c>
-      <c r="AI4" t="n">
-        <v>3</v>
-      </c>
-      <c r="AJ4" t="n">
-        <v>5</v>
-      </c>
-      <c r="AK4" t="n">
+      <c r="BA4" t="n">
         <v>2</v>
       </c>
     </row>
@@ -991,7 +1215,7 @@
         <v>8.730542659852533</v>
       </c>
       <c r="J5" t="n">
-        <v>6.010969638090832</v>
+        <v>5.965168148784675</v>
       </c>
       <c r="K5" t="n">
         <v>30</v>
@@ -1003,75 +1227,123 @@
         <v>-3.488142292490126</v>
       </c>
       <c r="N5" t="n">
-        <v>14.01001538300497</v>
+        <v>-35.826828</v>
       </c>
       <c r="O5" t="n">
+        <v>-3.5070446</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-7.036984</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-18.084</v>
+      </c>
+      <c r="R5" t="n">
+        <v>-130.9</v>
+      </c>
+      <c r="S5" t="n">
+        <v>-69.34157182553139</v>
+      </c>
+      <c r="T5" t="n">
+        <v>9.062176945209908</v>
+      </c>
+      <c r="U5" t="n">
+        <v>19.55795976235485</v>
+      </c>
+      <c r="V5" t="n">
+        <v>9.234561844679448</v>
+      </c>
+      <c r="W5" t="n">
         <v>16</v>
       </c>
-      <c r="P5" t="n">
+      <c r="X5" t="n">
         <v>8</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="Y5" t="n">
+        <v>7</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>23</v>
+      </c>
+      <c r="AA5" t="n">
         <v>18</v>
       </c>
-      <c r="R5" t="n">
-        <v>23</v>
-      </c>
-      <c r="S5" t="n">
-        <v>7</v>
-      </c>
-      <c r="T5" t="n">
+      <c r="AB5" t="n">
         <v>15</v>
       </c>
-      <c r="U5" t="n">
+      <c r="AC5" t="n">
         <v>22</v>
       </c>
-      <c r="V5" t="n">
+      <c r="AD5" t="n">
         <v>22</v>
       </c>
-      <c r="W5" t="n">
+      <c r="AE5" t="n">
         <v>15</v>
       </c>
-      <c r="X5" t="n">
+      <c r="AF5" t="n">
         <v>23.5</v>
       </c>
-      <c r="Y5" t="n">
+      <c r="AG5" t="n">
         <v>24</v>
       </c>
-      <c r="Z5" t="n">
+      <c r="AH5" t="n">
         <v>22</v>
       </c>
-      <c r="AA5" t="n">
-        <v>16</v>
-      </c>
-      <c r="AB5" t="n">
+      <c r="AI5" t="n">
+        <v>20</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>8</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>12</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>10</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>19</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>22</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>5</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>5</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>15</v>
+      </c>
+      <c r="AR5" t="n">
         <v>6</v>
       </c>
-      <c r="AC5" t="n">
-        <v>10</v>
-      </c>
-      <c r="AD5" t="n">
+      <c r="AS5" t="n">
+        <v>10</v>
+      </c>
+      <c r="AT5" t="n">
         <v>6</v>
       </c>
-      <c r="AE5" t="n">
+      <c r="AU5" t="n">
         <v>7.039999999999999</v>
       </c>
-      <c r="AF5" t="n">
+      <c r="AV5" t="n">
         <v>7.755999999999999</v>
       </c>
-      <c r="AG5" t="n">
+      <c r="AW5" t="n">
         <v>1</v>
       </c>
-      <c r="AH5" t="n">
-        <v>16</v>
-      </c>
-      <c r="AI5" t="n">
+      <c r="AX5" t="n">
+        <v>15</v>
+      </c>
+      <c r="AY5" t="n">
         <v>5</v>
       </c>
-      <c r="AJ5" t="n">
-        <v>9.333333333333334</v>
-      </c>
-      <c r="AK5" t="n">
+      <c r="AZ5" t="n">
+        <v>9</v>
+      </c>
+      <c r="BA5" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1106,7 +1378,7 @@
         <v>16.07959473994657</v>
       </c>
       <c r="J6" t="n">
-        <v>19.67523838109184</v>
+        <v>20.01240789638013</v>
       </c>
       <c r="K6" t="n">
         <v>40</v>
@@ -1118,75 +1390,123 @@
         <v>-8.685366677931739</v>
       </c>
       <c r="N6" t="n">
-        <v>15.29794720116778</v>
+        <v>-136.73456</v>
       </c>
       <c r="O6" t="n">
-        <v>4</v>
+        <v>-15.88771</v>
       </c>
       <c r="P6" t="n">
-        <v>16</v>
+        <v>-18.473791</v>
       </c>
       <c r="Q6" t="n">
-        <v>24</v>
+        <v>-118.065</v>
       </c>
       <c r="R6" t="n">
-        <v>19</v>
+        <v>-206.5</v>
       </c>
       <c r="S6" t="n">
-        <v>13</v>
+        <v>-37.20220408485095</v>
       </c>
       <c r="T6" t="n">
-        <v>8</v>
+        <v>6.384041943147374</v>
       </c>
       <c r="U6" t="n">
-        <v>11</v>
+        <v>20.92987377279102</v>
       </c>
       <c r="V6" t="n">
-        <v>13</v>
+        <v>8.419891177867408</v>
       </c>
       <c r="W6" t="n">
         <v>4</v>
       </c>
       <c r="X6" t="n">
+        <v>16</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>13</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>19</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>24</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>8</v>
+      </c>
+      <c r="AC6" t="n">
         <v>11</v>
       </c>
-      <c r="Y6" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z6" t="n">
+      <c r="AD6" t="n">
+        <v>13</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>4</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>11</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH6" t="n">
         <v>24</v>
       </c>
-      <c r="AA6" t="n">
-        <v>15</v>
-      </c>
-      <c r="AB6" t="n">
+      <c r="AI6" t="n">
+        <v>25</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>23</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>17</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>24</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>23</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>19</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>8</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>4</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>19</v>
+      </c>
+      <c r="AR6" t="n">
         <v>0</v>
       </c>
-      <c r="AC6" t="n">
+      <c r="AS6" t="n">
         <v>0</v>
       </c>
-      <c r="AD6" t="n">
+      <c r="AT6" t="n">
         <v>1</v>
       </c>
-      <c r="AE6" t="n">
+      <c r="AU6" t="n">
         <v>8.4</v>
       </c>
-      <c r="AF6" t="n">
+      <c r="AV6" t="n">
         <v>1.41</v>
       </c>
-      <c r="AG6" t="n">
+      <c r="AW6" t="n">
         <v>1</v>
       </c>
-      <c r="AH6" t="n">
-        <v>15</v>
-      </c>
-      <c r="AI6" t="n">
+      <c r="AX6" t="n">
+        <v>19</v>
+      </c>
+      <c r="AY6" t="n">
         <v>26</v>
       </c>
-      <c r="AJ6" t="n">
-        <v>16</v>
-      </c>
-      <c r="AK6" t="n">
+      <c r="AZ6" t="n">
+        <v>17.33333333333333</v>
+      </c>
+      <c r="BA6" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1221,7 +1541,7 @@
         <v>38.81309913004932</v>
       </c>
       <c r="J7" t="n">
-        <v>86.8669294592883</v>
+        <v>85.35672854818958</v>
       </c>
       <c r="K7" t="n">
         <v>40</v>
@@ -1233,75 +1553,123 @@
         <v>1.622596153846156</v>
       </c>
       <c r="N7" t="n">
-        <v>58.44630688698005</v>
+        <v>-42.99272</v>
       </c>
       <c r="O7" t="n">
+        <v>-26.10174</v>
+      </c>
+      <c r="P7" t="n">
+        <v>-43.06589</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>-43.647</v>
+      </c>
+      <c r="R7" t="n">
+        <v>-210.2</v>
+      </c>
+      <c r="S7" t="n">
+        <v>-92.64562915219895</v>
+      </c>
+      <c r="T7" t="n">
+        <v>-7.87716955941255</v>
+      </c>
+      <c r="U7" t="n">
+        <v>8.793770581778265</v>
+      </c>
+      <c r="V7" t="n">
+        <v>45.289502693801</v>
+      </c>
+      <c r="W7" t="n">
         <v>1</v>
       </c>
-      <c r="P7" t="n">
+      <c r="X7" t="n">
         <v>1</v>
       </c>
-      <c r="Q7" t="n">
+      <c r="Y7" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>2</v>
+      </c>
+      <c r="AA7" t="n">
         <v>9</v>
       </c>
-      <c r="R7" t="n">
+      <c r="AB7" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>5</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>5</v>
+      </c>
+      <c r="AE7" t="n">
         <v>2</v>
       </c>
-      <c r="S7" t="n">
+      <c r="AF7" t="n">
+        <v>11</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH7" t="n">
+        <v>14</v>
+      </c>
+      <c r="AI7" t="n">
+        <v>22</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>24</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>23</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>21</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>24</v>
+      </c>
+      <c r="AN7" t="n">
+        <v>23</v>
+      </c>
+      <c r="AO7" t="n">
+        <v>26</v>
+      </c>
+      <c r="AP7" t="n">
+        <v>20</v>
+      </c>
+      <c r="AQ7" t="n">
         <v>1</v>
       </c>
-      <c r="T7" t="n">
-        <v>6</v>
-      </c>
-      <c r="U7" t="n">
-        <v>5</v>
-      </c>
-      <c r="V7" t="n">
-        <v>5</v>
-      </c>
-      <c r="W7" t="n">
-        <v>2</v>
-      </c>
-      <c r="X7" t="n">
+      <c r="AR7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>10</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>8</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>5.28</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>6.292</v>
+      </c>
+      <c r="AW7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AY7" t="n">
         <v>11</v>
       </c>
-      <c r="Y7" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z7" t="n">
-        <v>14</v>
-      </c>
-      <c r="AA7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC7" t="n">
-        <v>10</v>
-      </c>
-      <c r="AD7" t="n">
-        <v>8</v>
-      </c>
-      <c r="AE7" t="n">
-        <v>5.28</v>
-      </c>
-      <c r="AF7" t="n">
-        <v>6.292</v>
-      </c>
-      <c r="AG7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AI7" t="n">
-        <v>11</v>
-      </c>
-      <c r="AJ7" t="n">
+      <c r="AZ7" t="n">
         <v>6.333333333333333</v>
       </c>
-      <c r="AK7" t="n">
+      <c r="BA7" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1336,7 +1704,7 @@
         <v>29.77884271937135</v>
       </c>
       <c r="J8" t="n">
-        <v>14.60188966620858</v>
+        <v>14.47797340017563</v>
       </c>
       <c r="K8" t="n">
         <v>40</v>
@@ -1348,75 +1716,123 @@
         <v>9.982238010657197</v>
       </c>
       <c r="N8" t="n">
-        <v>25.84180955885967</v>
+        <v>-29.935375</v>
       </c>
       <c r="O8" t="n">
+        <v>-10.642643</v>
+      </c>
+      <c r="P8" t="n">
+        <v>-9.768418</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>-20.154</v>
+      </c>
+      <c r="R8" t="n">
+        <v>-124.2</v>
+      </c>
+      <c r="S8" t="n">
+        <v>-36.88491163783526</v>
+      </c>
+      <c r="T8" t="n">
+        <v>10.49359907844118</v>
+      </c>
+      <c r="U8" t="n">
+        <v>14.64528543938422</v>
+      </c>
+      <c r="V8" t="n">
+        <v>19.90705863728995</v>
+      </c>
+      <c r="W8" t="n">
         <v>13</v>
       </c>
-      <c r="P8" t="n">
+      <c r="X8" t="n">
         <v>7</v>
       </c>
-      <c r="Q8" t="n">
+      <c r="Y8" t="n">
+        <v>6</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>6</v>
+      </c>
+      <c r="AA8" t="n">
         <v>4</v>
       </c>
-      <c r="R8" t="n">
+      <c r="AB8" t="n">
+        <v>13</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>7</v>
+      </c>
+      <c r="AD8" t="n">
         <v>6</v>
       </c>
-      <c r="S8" t="n">
+      <c r="AE8" t="n">
         <v>6</v>
       </c>
-      <c r="T8" t="n">
-        <v>13</v>
-      </c>
-      <c r="U8" t="n">
+      <c r="AF8" t="n">
+        <v>11</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH8" t="n">
+        <v>3</v>
+      </c>
+      <c r="AI8" t="n">
+        <v>11</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>18</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>14</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>14</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>16</v>
+      </c>
+      <c r="AN8" t="n">
+        <v>18</v>
+      </c>
+      <c r="AO8" t="n">
+        <v>3</v>
+      </c>
+      <c r="AP8" t="n">
+        <v>11</v>
+      </c>
+      <c r="AQ8" t="n">
+        <v>4</v>
+      </c>
+      <c r="AR8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS8" t="n">
+        <v>10</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>10</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>9.16</v>
+      </c>
+      <c r="AV8" t="n">
+        <v>7.174</v>
+      </c>
+      <c r="AW8" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX8" t="n">
+        <v>4</v>
+      </c>
+      <c r="AY8" t="n">
         <v>7</v>
       </c>
-      <c r="V8" t="n">
+      <c r="AZ8" t="n">
         <v>6</v>
       </c>
-      <c r="W8" t="n">
-        <v>6</v>
-      </c>
-      <c r="X8" t="n">
-        <v>11</v>
-      </c>
-      <c r="Y8" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z8" t="n">
-        <v>3</v>
-      </c>
-      <c r="AA8" t="n">
-        <v>5</v>
-      </c>
-      <c r="AB8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC8" t="n">
-        <v>10</v>
-      </c>
-      <c r="AD8" t="n">
-        <v>10</v>
-      </c>
-      <c r="AE8" t="n">
-        <v>9.16</v>
-      </c>
-      <c r="AF8" t="n">
-        <v>7.174</v>
-      </c>
-      <c r="AG8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH8" t="n">
-        <v>5</v>
-      </c>
-      <c r="AI8" t="n">
-        <v>7</v>
-      </c>
-      <c r="AJ8" t="n">
-        <v>6.333333333333333</v>
-      </c>
-      <c r="AK8" t="n">
+      <c r="BA8" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1451,7 +1867,7 @@
         <v>9.897513390586193</v>
       </c>
       <c r="J9" t="n">
-        <v>9.537272529310465</v>
+        <v>9.313204647585749</v>
       </c>
       <c r="K9" t="n">
         <v>40</v>
@@ -1463,75 +1879,123 @@
         <v>4.026354319180092</v>
       </c>
       <c r="N9" t="n">
-        <v>18.07779598170917</v>
+        <v>-35.505615</v>
       </c>
       <c r="O9" t="n">
+        <v>-11.589415</v>
+      </c>
+      <c r="P9" t="n">
+        <v>-20.845243</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>-30.576</v>
+      </c>
+      <c r="R9" t="n">
+        <v>-124.9</v>
+      </c>
+      <c r="S9" t="n">
+        <v>-14.10708087100158</v>
+      </c>
+      <c r="T9" t="n">
+        <v>7.397879381596062</v>
+      </c>
+      <c r="U9" t="n">
+        <v>14.74747741560568</v>
+      </c>
+      <c r="V9" t="n">
+        <v>13.24433837017594</v>
+      </c>
+      <c r="W9" t="n">
         <v>8</v>
       </c>
-      <c r="P9" t="n">
+      <c r="X9" t="n">
         <v>13</v>
       </c>
-      <c r="Q9" t="n">
+      <c r="Y9" t="n">
         <v>14</v>
       </c>
-      <c r="R9" t="n">
+      <c r="Z9" t="n">
         <v>7</v>
       </c>
-      <c r="S9" t="n">
+      <c r="AA9" t="n">
         <v>14</v>
       </c>
-      <c r="T9" t="n">
+      <c r="AB9" t="n">
         <v>12</v>
       </c>
-      <c r="U9" t="n">
+      <c r="AC9" t="n">
         <v>16</v>
       </c>
-      <c r="V9" t="n">
+      <c r="AD9" t="n">
         <v>18</v>
       </c>
-      <c r="W9" t="n">
+      <c r="AE9" t="n">
         <v>11</v>
       </c>
-      <c r="X9" t="n">
+      <c r="AF9" t="n">
         <v>11</v>
       </c>
-      <c r="Y9" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z9" t="n">
-        <v>10</v>
-      </c>
-      <c r="AA9" t="n">
+      <c r="AG9" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH9" t="n">
+        <v>10</v>
+      </c>
+      <c r="AI9" t="n">
+        <v>19</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>19</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>18</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>19</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>17</v>
+      </c>
+      <c r="AN9" t="n">
+        <v>3</v>
+      </c>
+      <c r="AO9" t="n">
+        <v>6</v>
+      </c>
+      <c r="AP9" t="n">
+        <v>10</v>
+      </c>
+      <c r="AQ9" t="n">
         <v>12</v>
       </c>
-      <c r="AB9" t="n">
+      <c r="AR9" t="n">
         <v>1</v>
       </c>
-      <c r="AC9" t="n">
-        <v>10</v>
-      </c>
-      <c r="AD9" t="n">
+      <c r="AS9" t="n">
+        <v>10</v>
+      </c>
+      <c r="AT9" t="n">
         <v>7</v>
       </c>
-      <c r="AE9" t="n">
+      <c r="AU9" t="n">
         <v>10.68</v>
       </c>
-      <c r="AF9" t="n">
+      <c r="AV9" t="n">
         <v>6.951999999999999</v>
       </c>
-      <c r="AG9" t="n">
+      <c r="AW9" t="n">
         <v>2</v>
       </c>
-      <c r="AH9" t="n">
+      <c r="AX9" t="n">
         <v>12</v>
       </c>
-      <c r="AI9" t="n">
+      <c r="AY9" t="n">
         <v>8</v>
       </c>
-      <c r="AJ9" t="n">
+      <c r="AZ9" t="n">
         <v>7.333333333333333</v>
       </c>
-      <c r="AK9" t="n">
+      <c r="BA9" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1566,7 +2030,7 @@
         <v>18.28732316989424</v>
       </c>
       <c r="J10" t="n">
-        <v>14.16476589378486</v>
+        <v>14.2470358351127</v>
       </c>
       <c r="K10" t="n">
         <v>40</v>
@@ -1578,75 +2042,123 @@
         <v>-33.55317394888706</v>
       </c>
       <c r="N10" t="n">
-        <v>9.687913393370906</v>
+        <v>-31.74804</v>
       </c>
       <c r="O10" t="n">
+        <v>-8.876296999999999</v>
+      </c>
+      <c r="P10" t="n">
+        <v>-4.401658</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>-47.03</v>
+      </c>
+      <c r="R10" t="n">
+        <v>-191.6</v>
+      </c>
+      <c r="S10" t="n">
+        <v>-64.31920397517369</v>
+      </c>
+      <c r="T10" t="n">
+        <v>2.022361540461676</v>
+      </c>
+      <c r="U10" t="n">
+        <v>18.53138330286411</v>
+      </c>
+      <c r="V10" t="n">
+        <v>4.661921586891281</v>
+      </c>
+      <c r="W10" t="n">
         <v>6</v>
       </c>
-      <c r="P10" t="n">
+      <c r="X10" t="n">
         <v>26</v>
       </c>
-      <c r="Q10" t="n">
+      <c r="Y10" t="n">
+        <v>16</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>22</v>
+      </c>
+      <c r="AA10" t="n">
         <v>17</v>
       </c>
-      <c r="R10" t="n">
+      <c r="AB10" t="n">
+        <v>1</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>9</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>12</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>7</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>11</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH10" t="n">
+        <v>26</v>
+      </c>
+      <c r="AI10" t="n">
+        <v>15</v>
+      </c>
+      <c r="AJ10" t="n">
+        <v>15</v>
+      </c>
+      <c r="AK10" t="n">
+        <v>10</v>
+      </c>
+      <c r="AL10" t="n">
         <v>22</v>
       </c>
-      <c r="S10" t="n">
-        <v>16</v>
-      </c>
-      <c r="T10" t="n">
-        <v>1</v>
-      </c>
-      <c r="U10" t="n">
-        <v>9</v>
-      </c>
-      <c r="V10" t="n">
-        <v>12</v>
-      </c>
-      <c r="W10" t="n">
-        <v>7</v>
-      </c>
-      <c r="X10" t="n">
-        <v>11</v>
-      </c>
-      <c r="Y10" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z10" t="n">
-        <v>26</v>
-      </c>
-      <c r="AA10" t="n">
-        <v>21</v>
-      </c>
-      <c r="AB10" t="n">
+      <c r="AM10" t="n">
+        <v>22</v>
+      </c>
+      <c r="AN10" t="n">
+        <v>20</v>
+      </c>
+      <c r="AO10" t="n">
+        <v>18</v>
+      </c>
+      <c r="AP10" t="n">
+        <v>6</v>
+      </c>
+      <c r="AQ10" t="n">
+        <v>22</v>
+      </c>
+      <c r="AR10" t="n">
         <v>0</v>
       </c>
-      <c r="AC10" t="n">
+      <c r="AS10" t="n">
         <v>5</v>
       </c>
-      <c r="AD10" t="n">
+      <c r="AT10" t="n">
         <v>18</v>
       </c>
-      <c r="AE10" t="n">
+      <c r="AU10" t="n">
         <v>7.880000000000001</v>
       </c>
-      <c r="AF10" t="n">
+      <c r="AV10" t="n">
         <v>5.882</v>
       </c>
-      <c r="AG10" t="n">
+      <c r="AW10" t="n">
         <v>2</v>
       </c>
-      <c r="AH10" t="n">
-        <v>21</v>
-      </c>
-      <c r="AI10" t="n">
+      <c r="AX10" t="n">
+        <v>22</v>
+      </c>
+      <c r="AY10" t="n">
         <v>14</v>
       </c>
-      <c r="AJ10" t="n">
-        <v>12.33333333333333</v>
-      </c>
-      <c r="AK10" t="n">
+      <c r="AZ10" t="n">
+        <v>12.66666666666667</v>
+      </c>
+      <c r="BA10" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1681,7 +2193,7 @@
         <v>51.99138858988159</v>
       </c>
       <c r="J11" t="n">
-        <v>45.56803282316724</v>
+        <v>45.94760462249834</v>
       </c>
       <c r="K11" t="n">
         <v>40</v>
@@ -1693,75 +2205,123 @@
         <v>-2.333709923984806</v>
       </c>
       <c r="N11" t="n">
-        <v>28.74769207516695</v>
+        <v>-70.519424</v>
       </c>
       <c r="O11" t="n">
+        <v>-37.34028</v>
+      </c>
+      <c r="P11" t="n">
+        <v>-21.954058</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>-155.87</v>
+      </c>
+      <c r="R11" t="n">
+        <v>-418.3</v>
+      </c>
+      <c r="S11" t="n">
+        <v>-30.41114133027265</v>
+      </c>
+      <c r="T11" t="n">
+        <v>-4.42230183609494</v>
+      </c>
+      <c r="U11" t="n">
+        <v>5.012626262626263</v>
+      </c>
+      <c r="V11" t="n">
+        <v>17.05137071206019</v>
+      </c>
+      <c r="W11" t="n">
         <v>9</v>
       </c>
-      <c r="P11" t="n">
+      <c r="X11" t="n">
         <v>12</v>
       </c>
-      <c r="Q11" t="n">
+      <c r="Y11" t="n">
+        <v>24</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>16</v>
+      </c>
+      <c r="AA11" t="n">
         <v>1</v>
       </c>
-      <c r="R11" t="n">
-        <v>16</v>
-      </c>
-      <c r="S11" t="n">
-        <v>24</v>
-      </c>
-      <c r="T11" t="n">
+      <c r="AB11" t="n">
         <v>3</v>
       </c>
-      <c r="U11" t="n">
+      <c r="AC11" t="n">
         <v>4</v>
       </c>
-      <c r="V11" t="n">
+      <c r="AD11" t="n">
         <v>4</v>
       </c>
-      <c r="W11" t="n">
+      <c r="AE11" t="n">
         <v>3</v>
       </c>
-      <c r="X11" t="n">
+      <c r="AF11" t="n">
         <v>11</v>
       </c>
-      <c r="Y11" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z11" t="n">
+      <c r="AG11" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH11" t="n">
         <v>21</v>
-      </c>
-      <c r="AA11" t="n">
-        <v>3</v>
-      </c>
-      <c r="AB11" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC11" t="n">
-        <v>5</v>
-      </c>
-      <c r="AD11" t="n">
-        <v>1</v>
-      </c>
-      <c r="AE11" t="n">
-        <v>8.279999999999999</v>
-      </c>
-      <c r="AF11" t="n">
-        <v>3.691999999999999</v>
-      </c>
-      <c r="AG11" t="n">
-        <v>-1</v>
-      </c>
-      <c r="AH11" t="n">
-        <v>3</v>
       </c>
       <c r="AI11" t="n">
         <v>24</v>
       </c>
       <c r="AJ11" t="n">
-        <v>14.16666666666667</v>
+        <v>25</v>
       </c>
       <c r="AK11" t="n">
+        <v>20</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>25</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>26</v>
+      </c>
+      <c r="AN11" t="n">
+        <v>12</v>
+      </c>
+      <c r="AO11" t="n">
+        <v>25</v>
+      </c>
+      <c r="AP11" t="n">
+        <v>22</v>
+      </c>
+      <c r="AQ11" t="n">
+        <v>6</v>
+      </c>
+      <c r="AR11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS11" t="n">
+        <v>5</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>1</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>8.279999999999999</v>
+      </c>
+      <c r="AV11" t="n">
+        <v>3.691999999999999</v>
+      </c>
+      <c r="AW11" t="n">
+        <v>-1</v>
+      </c>
+      <c r="AX11" t="n">
+        <v>6</v>
+      </c>
+      <c r="AY11" t="n">
+        <v>24</v>
+      </c>
+      <c r="AZ11" t="n">
+        <v>15.16666666666667</v>
+      </c>
+      <c r="BA11" t="n">
         <v>15.5</v>
       </c>
     </row>
@@ -1796,7 +2356,7 @@
         <v>72.79053896859247</v>
       </c>
       <c r="J12" t="n">
-        <v>0.3716290218173907</v>
+        <v>0.3705569817803875</v>
       </c>
       <c r="K12" t="n">
         <v>40</v>
@@ -1808,75 +2368,123 @@
         <v>4.884990898560315</v>
       </c>
       <c r="N12" t="n">
-        <v>20.85245465669282</v>
+        <v>-18.703888</v>
       </c>
       <c r="O12" t="n">
+        <v>-5.257813</v>
+      </c>
+      <c r="P12" t="n">
+        <v>-2.5556931</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>-3.102</v>
+      </c>
+      <c r="R12" t="n">
+        <v>-112.9</v>
+      </c>
+      <c r="S12" t="n">
+        <v>-17.22958222926846</v>
+      </c>
+      <c r="T12" t="n">
+        <v>-2.510308997620174</v>
+      </c>
+      <c r="U12" t="n">
+        <v>-7.185100306134665</v>
+      </c>
+      <c r="V12" t="n">
+        <v>16.71516538989576</v>
+      </c>
+      <c r="W12" t="n">
         <v>14</v>
       </c>
-      <c r="P12" t="n">
+      <c r="X12" t="n">
         <v>15</v>
       </c>
-      <c r="Q12" t="n">
+      <c r="Y12" t="n">
+        <v>19</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>4</v>
+      </c>
+      <c r="AA12" t="n">
         <v>22</v>
       </c>
-      <c r="R12" t="n">
-        <v>4</v>
-      </c>
-      <c r="S12" t="n">
-        <v>19</v>
-      </c>
-      <c r="T12" t="n">
+      <c r="AB12" t="n">
         <v>21</v>
       </c>
-      <c r="U12" t="n">
+      <c r="AC12" t="n">
         <v>1</v>
       </c>
-      <c r="V12" t="n">
+      <c r="AD12" t="n">
         <v>1</v>
       </c>
-      <c r="W12" t="n">
+      <c r="AE12" t="n">
         <v>24</v>
       </c>
-      <c r="X12" t="n">
+      <c r="AF12" t="n">
         <v>11</v>
       </c>
-      <c r="Y12" t="n">
+      <c r="AG12" t="n">
         <v>21</v>
-      </c>
-      <c r="Z12" t="n">
-        <v>9</v>
-      </c>
-      <c r="AA12" t="n">
-        <v>9</v>
-      </c>
-      <c r="AB12" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC12" t="n">
-        <v>5</v>
-      </c>
-      <c r="AD12" t="n">
-        <v>7</v>
-      </c>
-      <c r="AE12" t="n">
-        <v>6.879999999999999</v>
-      </c>
-      <c r="AF12" t="n">
-        <v>4.082</v>
-      </c>
-      <c r="AG12" t="n">
-        <v>-2</v>
       </c>
       <c r="AH12" t="n">
         <v>9</v>
       </c>
       <c r="AI12" t="n">
+        <v>6</v>
+      </c>
+      <c r="AJ12" t="n">
+        <v>11</v>
+      </c>
+      <c r="AK12" t="n">
+        <v>9</v>
+      </c>
+      <c r="AL12" t="n">
+        <v>4</v>
+      </c>
+      <c r="AM12" t="n">
+        <v>13</v>
+      </c>
+      <c r="AN12" t="n">
+        <v>6</v>
+      </c>
+      <c r="AO12" t="n">
+        <v>24</v>
+      </c>
+      <c r="AP12" t="n">
+        <v>24</v>
+      </c>
+      <c r="AQ12" t="n">
+        <v>7</v>
+      </c>
+      <c r="AR12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AS12" t="n">
+        <v>5</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>7</v>
+      </c>
+      <c r="AU12" t="n">
+        <v>6.879999999999999</v>
+      </c>
+      <c r="AV12" t="n">
+        <v>4.082</v>
+      </c>
+      <c r="AW12" t="n">
+        <v>-2</v>
+      </c>
+      <c r="AX12" t="n">
+        <v>7</v>
+      </c>
+      <c r="AY12" t="n">
         <v>20</v>
       </c>
-      <c r="AJ12" t="n">
-        <v>16.83333333333333</v>
-      </c>
-      <c r="AK12" t="n">
+      <c r="AZ12" t="n">
+        <v>16.16666666666667</v>
+      </c>
+      <c r="BA12" t="n">
         <v>21.5</v>
       </c>
     </row>
@@ -1911,7 +2519,7 @@
         <v>20.09313206214689</v>
       </c>
       <c r="J13" t="n">
-        <v>0.2939479743696643</v>
+        <v>0.2907138303612626</v>
       </c>
       <c r="K13" t="n">
         <v>40</v>
@@ -1923,75 +2531,123 @@
         <v>5.337563823861091</v>
       </c>
       <c r="N13" t="n">
-        <v>5.486147152601344</v>
+        <v>-19.151106</v>
       </c>
       <c r="O13" t="n">
+        <v>-4.397229</v>
+      </c>
+      <c r="P13" t="n">
+        <v>-2.3133376</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>-0.36</v>
+      </c>
+      <c r="R13" t="n">
+        <v>-140.2</v>
+      </c>
+      <c r="S13" t="n">
+        <v>-36.1665165785675</v>
+      </c>
+      <c r="T13" t="n">
+        <v>-1.640122866014468</v>
+      </c>
+      <c r="U13" t="n">
+        <v>-9.254693191370132</v>
+      </c>
+      <c r="V13" t="n">
+        <v>1.921076849380055</v>
+      </c>
+      <c r="W13" t="n">
         <v>24</v>
       </c>
-      <c r="P13" t="n">
+      <c r="X13" t="n">
         <v>22</v>
       </c>
-      <c r="Q13" t="n">
+      <c r="Y13" t="n">
+        <v>19</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>11</v>
+      </c>
+      <c r="AA13" t="n">
         <v>23</v>
       </c>
-      <c r="R13" t="n">
+      <c r="AB13" t="n">
+        <v>25</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>12</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>10</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>25</v>
+      </c>
+      <c r="AF13" t="n">
         <v>11</v>
       </c>
-      <c r="S13" t="n">
-        <v>19</v>
-      </c>
-      <c r="T13" t="n">
+      <c r="AG13" t="n">
+        <v>24</v>
+      </c>
+      <c r="AH13" t="n">
+        <v>8</v>
+      </c>
+      <c r="AI13" t="n">
+        <v>7</v>
+      </c>
+      <c r="AJ13" t="n">
+        <v>10</v>
+      </c>
+      <c r="AK13" t="n">
+        <v>8</v>
+      </c>
+      <c r="AL13" t="n">
+        <v>2</v>
+      </c>
+      <c r="AM13" t="n">
+        <v>21</v>
+      </c>
+      <c r="AN13" t="n">
+        <v>17</v>
+      </c>
+      <c r="AO13" t="n">
+        <v>22</v>
+      </c>
+      <c r="AP13" t="n">
         <v>25</v>
       </c>
-      <c r="U13" t="n">
-        <v>12</v>
-      </c>
-      <c r="V13" t="n">
-        <v>10</v>
-      </c>
-      <c r="W13" t="n">
+      <c r="AQ13" t="n">
         <v>25</v>
       </c>
-      <c r="X13" t="n">
-        <v>11</v>
-      </c>
-      <c r="Y13" t="n">
-        <v>24</v>
-      </c>
-      <c r="Z13" t="n">
-        <v>8</v>
-      </c>
-      <c r="AA13" t="n">
+      <c r="AR13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT13" t="n">
+        <v>17</v>
+      </c>
+      <c r="AU13" t="n">
+        <v>8.119999999999999</v>
+      </c>
+      <c r="AV13" t="n">
+        <v>4.068</v>
+      </c>
+      <c r="AW13" t="n">
+        <v>-2</v>
+      </c>
+      <c r="AX13" t="n">
         <v>25</v>
       </c>
-      <c r="AB13" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD13" t="n">
-        <v>17</v>
-      </c>
-      <c r="AE13" t="n">
-        <v>8.119999999999999</v>
-      </c>
-      <c r="AF13" t="n">
-        <v>4.068</v>
-      </c>
-      <c r="AG13" t="n">
-        <v>-2</v>
-      </c>
-      <c r="AH13" t="n">
-        <v>25</v>
-      </c>
-      <c r="AI13" t="n">
+      <c r="AY13" t="n">
         <v>21</v>
       </c>
-      <c r="AJ13" t="n">
+      <c r="AZ13" t="n">
         <v>22.5</v>
       </c>
-      <c r="AK13" t="n">
+      <c r="BA13" t="n">
         <v>21.5</v>
       </c>
     </row>
@@ -2026,7 +2682,7 @@
         <v>13.60366441658631</v>
       </c>
       <c r="J14" t="n">
-        <v>8.607759009226037</v>
+        <v>8.544378348743662</v>
       </c>
       <c r="K14" t="n">
         <v>40</v>
@@ -2038,75 +2694,123 @@
         <v>-0</v>
       </c>
       <c r="N14" t="n">
-        <v>22.5379248419639</v>
+        <v>-31.144402</v>
       </c>
       <c r="O14" t="n">
-        <v>10</v>
+        <v>-10.250537</v>
       </c>
       <c r="P14" t="n">
+        <v>-9.80471</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>-100</v>
+      </c>
+      <c r="R14" t="n">
+        <v>-126</v>
+      </c>
+      <c r="S14" t="n">
+        <v>-24.35856634276198</v>
+      </c>
+      <c r="T14" t="n">
+        <v>6.326099897180583</v>
+      </c>
+      <c r="U14" t="n">
+        <v>16.04290514344792</v>
+      </c>
+      <c r="V14" t="n">
+        <v>16.3239528247262</v>
+      </c>
+      <c r="W14" t="n">
+        <v>10</v>
+      </c>
+      <c r="X14" t="n">
         <v>6</v>
       </c>
-      <c r="Q14" t="n">
+      <c r="Y14" t="n">
+        <v>5</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>15</v>
+      </c>
+      <c r="AA14" t="n">
         <v>7</v>
       </c>
-      <c r="R14" t="n">
+      <c r="AB14" t="n">
+        <v>14</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>17</v>
+      </c>
+      <c r="AD14" t="n">
         <v>15</v>
       </c>
-      <c r="S14" t="n">
+      <c r="AE14" t="n">
+        <v>13</v>
+      </c>
+      <c r="AF14" t="n">
+        <v>11</v>
+      </c>
+      <c r="AG14" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH14" t="n">
+        <v>17</v>
+      </c>
+      <c r="AI14" t="n">
+        <v>14</v>
+      </c>
+      <c r="AJ14" t="n">
+        <v>17</v>
+      </c>
+      <c r="AK14" t="n">
+        <v>15</v>
+      </c>
+      <c r="AL14" t="n">
+        <v>23</v>
+      </c>
+      <c r="AM14" t="n">
+        <v>18</v>
+      </c>
+      <c r="AN14" t="n">
+        <v>10</v>
+      </c>
+      <c r="AO14" t="n">
+        <v>9</v>
+      </c>
+      <c r="AP14" t="n">
+        <v>7</v>
+      </c>
+      <c r="AQ14" t="n">
+        <v>8</v>
+      </c>
+      <c r="AR14" t="n">
         <v>5</v>
       </c>
-      <c r="T14" t="n">
-        <v>14</v>
-      </c>
-      <c r="U14" t="n">
-        <v>17</v>
-      </c>
-      <c r="V14" t="n">
-        <v>15</v>
-      </c>
-      <c r="W14" t="n">
-        <v>13</v>
-      </c>
-      <c r="X14" t="n">
-        <v>11</v>
-      </c>
-      <c r="Y14" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z14" t="n">
-        <v>17</v>
-      </c>
-      <c r="AA14" t="n">
-        <v>6</v>
-      </c>
-      <c r="AB14" t="n">
-        <v>5</v>
-      </c>
-      <c r="AC14" t="n">
-        <v>10</v>
-      </c>
-      <c r="AD14" t="n">
+      <c r="AS14" t="n">
+        <v>10</v>
+      </c>
+      <c r="AT14" t="n">
         <v>9</v>
       </c>
-      <c r="AE14" t="n">
+      <c r="AU14" t="n">
         <v>9.800000000000001</v>
       </c>
-      <c r="AF14" t="n">
+      <c r="AV14" t="n">
         <v>8.32</v>
       </c>
-      <c r="AG14" t="n">
+      <c r="AW14" t="n">
         <v>0</v>
       </c>
-      <c r="AH14" t="n">
-        <v>6</v>
-      </c>
-      <c r="AI14" t="n">
+      <c r="AX14" t="n">
+        <v>8</v>
+      </c>
+      <c r="AY14" t="n">
         <v>4</v>
       </c>
-      <c r="AJ14" t="n">
-        <v>7.5</v>
-      </c>
-      <c r="AK14" t="n">
+      <c r="AZ14" t="n">
+        <v>8.166666666666666</v>
+      </c>
+      <c r="BA14" t="n">
         <v>12.5</v>
       </c>
     </row>
@@ -2141,7 +2845,7 @@
         <v>21.39969185176944</v>
       </c>
       <c r="J15" t="n">
-        <v>4.208888033649355</v>
+        <v>4.182676905433154</v>
       </c>
       <c r="K15" t="n">
         <v>40</v>
@@ -2153,49 +2857,49 @@
         <v>0.01089070040624085</v>
       </c>
       <c r="N15" t="n">
-        <v>26.39897823844397</v>
+        <v>-30.338762</v>
       </c>
       <c r="O15" t="n">
+        <v>-2.2724824</v>
+      </c>
+      <c r="P15" t="n">
+        <v>-1.0544966</v>
+      </c>
+      <c r="Q15" t="n">
+        <v>-1.386</v>
+      </c>
+      <c r="R15" t="n">
+        <v>-119.9</v>
+      </c>
+      <c r="S15" t="n">
+        <v>-23.6604978211487</v>
+      </c>
+      <c r="T15" t="n">
+        <v>9.979384062921399</v>
+      </c>
+      <c r="U15" t="n">
+        <v>15.7649198423799</v>
+      </c>
+      <c r="V15" t="n">
+        <v>21.2269055030331</v>
+      </c>
+      <c r="W15" t="n">
         <v>3</v>
       </c>
-      <c r="P15" t="n">
+      <c r="X15" t="n">
         <v>4</v>
       </c>
-      <c r="Q15" t="n">
+      <c r="Y15" t="n">
+        <v>3</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA15" t="n">
         <v>13</v>
       </c>
-      <c r="R15" t="n">
-        <v>1</v>
-      </c>
-      <c r="S15" t="n">
-        <v>3</v>
-      </c>
-      <c r="T15" t="n">
-        <v>10</v>
-      </c>
-      <c r="U15" t="n">
-        <v>10</v>
-      </c>
-      <c r="V15" t="n">
-        <v>9</v>
-      </c>
-      <c r="W15" t="n">
-        <v>16</v>
-      </c>
-      <c r="X15" t="n">
-        <v>11</v>
-      </c>
-      <c r="Y15" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z15" t="n">
-        <v>16</v>
-      </c>
-      <c r="AA15" t="n">
-        <v>4</v>
-      </c>
       <c r="AB15" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="AC15" t="n">
         <v>10</v>
@@ -2204,24 +2908,72 @@
         <v>9</v>
       </c>
       <c r="AE15" t="n">
+        <v>16</v>
+      </c>
+      <c r="AF15" t="n">
+        <v>11</v>
+      </c>
+      <c r="AG15" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH15" t="n">
+        <v>16</v>
+      </c>
+      <c r="AI15" t="n">
+        <v>13</v>
+      </c>
+      <c r="AJ15" t="n">
+        <v>4</v>
+      </c>
+      <c r="AK15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AL15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AM15" t="n">
+        <v>14</v>
+      </c>
+      <c r="AN15" t="n">
+        <v>9</v>
+      </c>
+      <c r="AO15" t="n">
+        <v>4</v>
+      </c>
+      <c r="AP15" t="n">
+        <v>8</v>
+      </c>
+      <c r="AQ15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AR15" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS15" t="n">
+        <v>10</v>
+      </c>
+      <c r="AT15" t="n">
+        <v>9</v>
+      </c>
+      <c r="AU15" t="n">
         <v>7.359999999999999</v>
       </c>
-      <c r="AF15" t="n">
+      <c r="AV15" t="n">
         <v>6.754</v>
       </c>
-      <c r="AG15" t="n">
+      <c r="AW15" t="n">
         <v>1</v>
       </c>
-      <c r="AH15" t="n">
-        <v>4</v>
-      </c>
-      <c r="AI15" t="n">
+      <c r="AX15" t="n">
+        <v>3</v>
+      </c>
+      <c r="AY15" t="n">
         <v>9</v>
       </c>
-      <c r="AJ15" t="n">
-        <v>6.666666666666667</v>
-      </c>
-      <c r="AK15" t="n">
+      <c r="AZ15" t="n">
+        <v>6.333333333333333</v>
+      </c>
+      <c r="BA15" t="n">
         <v>7</v>
       </c>
     </row>
@@ -2256,7 +3008,7 @@
         <v>26.36943414195747</v>
       </c>
       <c r="J16" t="n">
-        <v>11.16892808080251</v>
+        <v>10.92217941192822</v>
       </c>
       <c r="K16" t="n">
         <v>40</v>
@@ -2268,75 +3020,123 @@
         <v>2.549797772789864</v>
       </c>
       <c r="N16" t="n">
-        <v>22.29568920351538</v>
+        <v>-50.22718</v>
       </c>
       <c r="O16" t="n">
+        <v>-12.242119</v>
+      </c>
+      <c r="P16" t="n">
+        <v>-24.086199</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>-37.983</v>
+      </c>
+      <c r="R16" t="n">
+        <v>-69.89999999999999</v>
+      </c>
+      <c r="S16" t="n">
+        <v>-24.9593083635035</v>
+      </c>
+      <c r="T16" t="n">
+        <v>4.262112007122982</v>
+      </c>
+      <c r="U16" t="n">
+        <v>12.65973531369487</v>
+      </c>
+      <c r="V16" t="n">
+        <v>17.3577666158993</v>
+      </c>
+      <c r="W16" t="n">
         <v>7</v>
       </c>
-      <c r="P16" t="n">
+      <c r="X16" t="n">
         <v>5</v>
       </c>
-      <c r="Q16" t="n">
+      <c r="Y16" t="n">
+        <v>4</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>13</v>
+      </c>
+      <c r="AA16" t="n">
         <v>16</v>
       </c>
-      <c r="R16" t="n">
+      <c r="AB16" t="n">
+        <v>19</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>6</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>7</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>8</v>
+      </c>
+      <c r="AF16" t="n">
+        <v>11</v>
+      </c>
+      <c r="AG16" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH16" t="n">
+        <v>12</v>
+      </c>
+      <c r="AI16" t="n">
+        <v>23</v>
+      </c>
+      <c r="AJ16" t="n">
+        <v>20</v>
+      </c>
+      <c r="AK16" t="n">
+        <v>21</v>
+      </c>
+      <c r="AL16" t="n">
+        <v>20</v>
+      </c>
+      <c r="AM16" t="n">
+        <v>7</v>
+      </c>
+      <c r="AN16" t="n">
+        <v>11</v>
+      </c>
+      <c r="AO16" t="n">
         <v>13</v>
       </c>
-      <c r="S16" t="n">
+      <c r="AP16" t="n">
+        <v>15</v>
+      </c>
+      <c r="AQ16" t="n">
+        <v>5</v>
+      </c>
+      <c r="AR16" t="n">
+        <v>16</v>
+      </c>
+      <c r="AS16" t="n">
+        <v>10</v>
+      </c>
+      <c r="AT16" t="n">
         <v>4</v>
       </c>
-      <c r="T16" t="n">
-        <v>19</v>
-      </c>
-      <c r="U16" t="n">
-        <v>6</v>
-      </c>
-      <c r="V16" t="n">
-        <v>7</v>
-      </c>
-      <c r="W16" t="n">
-        <v>8</v>
-      </c>
-      <c r="X16" t="n">
-        <v>11</v>
-      </c>
-      <c r="Y16" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z16" t="n">
-        <v>12</v>
-      </c>
-      <c r="AA16" t="n">
-        <v>7</v>
-      </c>
-      <c r="AB16" t="n">
-        <v>16</v>
-      </c>
-      <c r="AC16" t="n">
-        <v>10</v>
-      </c>
-      <c r="AD16" t="n">
-        <v>4</v>
-      </c>
-      <c r="AE16" t="n">
+      <c r="AU16" t="n">
         <v>9.119999999999999</v>
       </c>
-      <c r="AF16" t="n">
+      <c r="AV16" t="n">
         <v>10.768</v>
       </c>
-      <c r="AG16" t="n">
+      <c r="AW16" t="n">
         <v>1</v>
       </c>
-      <c r="AH16" t="n">
-        <v>7</v>
-      </c>
-      <c r="AI16" t="n">
+      <c r="AX16" t="n">
+        <v>5</v>
+      </c>
+      <c r="AY16" t="n">
         <v>1</v>
       </c>
-      <c r="AJ16" t="n">
-        <v>5</v>
-      </c>
-      <c r="AK16" t="n">
+      <c r="AZ16" t="n">
+        <v>4.333333333333333</v>
+      </c>
+      <c r="BA16" t="n">
         <v>7</v>
       </c>
     </row>
@@ -2371,7 +3171,7 @@
         <v>59.58013810995384</v>
       </c>
       <c r="J17" t="n">
-        <v>208.270543968919</v>
+        <v>203.9996630653805</v>
       </c>
       <c r="K17" t="n">
         <v>20</v>
@@ -2383,75 +3183,123 @@
         <v>-16.975624565597</v>
       </c>
       <c r="N17" t="n">
-        <v>46.14093174419554</v>
+        <v>-379.34042</v>
       </c>
       <c r="O17" t="n">
+        <v>-122.933945</v>
+      </c>
+      <c r="P17" t="n">
+        <v>-71.315994</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>-714.972</v>
+      </c>
+      <c r="R17" t="n">
+        <v>-259.2</v>
+      </c>
+      <c r="S17" t="n">
+        <v>-103.4381263528082</v>
+      </c>
+      <c r="T17" t="n">
+        <v>10.9081793642653</v>
+      </c>
+      <c r="U17" t="n">
+        <v>24.96516584088794</v>
+      </c>
+      <c r="V17" t="n">
+        <v>23.11117995228029</v>
+      </c>
+      <c r="W17" t="n">
         <v>2</v>
       </c>
-      <c r="P17" t="n">
+      <c r="X17" t="n">
         <v>14</v>
       </c>
-      <c r="Q17" t="n">
+      <c r="Y17" t="n">
+        <v>2</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>24</v>
+      </c>
+      <c r="AA17" t="n">
         <v>5</v>
       </c>
-      <c r="R17" t="n">
+      <c r="AB17" t="n">
+        <v>2</v>
+      </c>
+      <c r="AC17" t="n">
+        <v>2</v>
+      </c>
+      <c r="AD17" t="n">
+        <v>2</v>
+      </c>
+      <c r="AE17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AF17" t="n">
+        <v>26</v>
+      </c>
+      <c r="AG17" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH17" t="n">
+        <v>25</v>
+      </c>
+      <c r="AI17" t="n">
+        <v>26</v>
+      </c>
+      <c r="AJ17" t="n">
+        <v>26</v>
+      </c>
+      <c r="AK17" t="n">
+        <v>25</v>
+      </c>
+      <c r="AL17" t="n">
+        <v>26</v>
+      </c>
+      <c r="AM17" t="n">
+        <v>25</v>
+      </c>
+      <c r="AN17" t="n">
         <v>24</v>
       </c>
-      <c r="S17" t="n">
+      <c r="AO17" t="n">
         <v>2</v>
       </c>
-      <c r="T17" t="n">
+      <c r="AP17" t="n">
         <v>2</v>
       </c>
-      <c r="U17" t="n">
+      <c r="AQ17" t="n">
         <v>2</v>
       </c>
-      <c r="V17" t="n">
+      <c r="AR17" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS17" t="n">
+        <v>5</v>
+      </c>
+      <c r="AT17" t="n">
+        <v>5</v>
+      </c>
+      <c r="AU17" t="n">
+        <v>5.08</v>
+      </c>
+      <c r="AV17" t="n">
+        <v>3.812</v>
+      </c>
+      <c r="AW17" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX17" t="n">
         <v>2</v>
       </c>
-      <c r="W17" t="n">
-        <v>1</v>
-      </c>
-      <c r="X17" t="n">
-        <v>26</v>
-      </c>
-      <c r="Y17" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z17" t="n">
-        <v>25</v>
-      </c>
-      <c r="AA17" t="n">
-        <v>2</v>
-      </c>
-      <c r="AB17" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC17" t="n">
-        <v>5</v>
-      </c>
-      <c r="AD17" t="n">
-        <v>5</v>
-      </c>
-      <c r="AE17" t="n">
-        <v>5.08</v>
-      </c>
-      <c r="AF17" t="n">
-        <v>3.812</v>
-      </c>
-      <c r="AG17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AH17" t="n">
-        <v>2</v>
-      </c>
-      <c r="AI17" t="n">
+      <c r="AY17" t="n">
         <v>23</v>
       </c>
-      <c r="AJ17" t="n">
+      <c r="AZ17" t="n">
         <v>12.5</v>
       </c>
-      <c r="AK17" t="n">
+      <c r="BA17" t="n">
         <v>12.5</v>
       </c>
     </row>
@@ -2486,7 +3334,7 @@
         <v>8.863112564577856</v>
       </c>
       <c r="J18" t="n">
-        <v>7.671781199656317</v>
+        <v>7.610184785468961</v>
       </c>
       <c r="K18" t="n">
         <v>40</v>
@@ -2498,75 +3346,123 @@
         <v>5.884215747237198</v>
       </c>
       <c r="N18" t="n">
-        <v>17.61231817603731</v>
+        <v>-32.602825</v>
       </c>
       <c r="O18" t="n">
+        <v>-12.435372</v>
+      </c>
+      <c r="P18" t="n">
+        <v>-36.259144</v>
+      </c>
+      <c r="Q18" t="n">
+        <v>-28.541</v>
+      </c>
+      <c r="R18" t="n">
+        <v>-46.5</v>
+      </c>
+      <c r="S18" t="n">
+        <v>-33.17948947479677</v>
+      </c>
+      <c r="T18" t="n">
+        <v>-2.251289146019368</v>
+      </c>
+      <c r="U18" t="n">
+        <v>8.326628895184136</v>
+      </c>
+      <c r="V18" t="n">
+        <v>11.94022055861703</v>
+      </c>
+      <c r="W18" t="n">
         <v>5</v>
       </c>
-      <c r="P18" t="n">
+      <c r="X18" t="n">
         <v>3</v>
       </c>
-      <c r="Q18" t="n">
+      <c r="Y18" t="n">
+        <v>26</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>14</v>
+      </c>
+      <c r="AA18" t="n">
         <v>6</v>
       </c>
-      <c r="R18" t="n">
+      <c r="AB18" t="n">
+        <v>24</v>
+      </c>
+      <c r="AC18" t="n">
+        <v>20</v>
+      </c>
+      <c r="AD18" t="n">
+        <v>21</v>
+      </c>
+      <c r="AE18" t="n">
         <v>14</v>
       </c>
-      <c r="S18" t="n">
-        <v>26</v>
-      </c>
-      <c r="T18" t="n">
-        <v>24</v>
-      </c>
-      <c r="U18" t="n">
-        <v>20</v>
-      </c>
-      <c r="V18" t="n">
+      <c r="AF18" t="n">
+        <v>11</v>
+      </c>
+      <c r="AG18" t="n">
         <v>21</v>
       </c>
-      <c r="W18" t="n">
+      <c r="AH18" t="n">
+        <v>7</v>
+      </c>
+      <c r="AI18" t="n">
+        <v>17</v>
+      </c>
+      <c r="AJ18" t="n">
+        <v>21</v>
+      </c>
+      <c r="AK18" t="n">
+        <v>22</v>
+      </c>
+      <c r="AL18" t="n">
+        <v>18</v>
+      </c>
+      <c r="AM18" t="n">
+        <v>5</v>
+      </c>
+      <c r="AN18" t="n">
         <v>14</v>
       </c>
-      <c r="X18" t="n">
+      <c r="AO18" t="n">
+        <v>23</v>
+      </c>
+      <c r="AP18" t="n">
+        <v>21</v>
+      </c>
+      <c r="AQ18" t="n">
+        <v>14</v>
+      </c>
+      <c r="AR18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS18" t="n">
+        <v>10</v>
+      </c>
+      <c r="AT18" t="n">
+        <v>6</v>
+      </c>
+      <c r="AU18" t="n">
+        <v>6.719999999999999</v>
+      </c>
+      <c r="AV18" t="n">
+        <v>6.207999999999999</v>
+      </c>
+      <c r="AW18" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX18" t="n">
+        <v>14</v>
+      </c>
+      <c r="AY18" t="n">
+        <v>12</v>
+      </c>
+      <c r="AZ18" t="n">
         <v>11</v>
       </c>
-      <c r="Y18" t="n">
-        <v>21</v>
-      </c>
-      <c r="Z18" t="n">
-        <v>7</v>
-      </c>
-      <c r="AA18" t="n">
-        <v>13</v>
-      </c>
-      <c r="AB18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC18" t="n">
-        <v>10</v>
-      </c>
-      <c r="AD18" t="n">
-        <v>6</v>
-      </c>
-      <c r="AE18" t="n">
-        <v>6.719999999999999</v>
-      </c>
-      <c r="AF18" t="n">
-        <v>6.207999999999999</v>
-      </c>
-      <c r="AG18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AH18" t="n">
-        <v>13</v>
-      </c>
-      <c r="AI18" t="n">
-        <v>12</v>
-      </c>
-      <c r="AJ18" t="n">
-        <v>10.66666666666667</v>
-      </c>
-      <c r="AK18" t="n">
+      <c r="BA18" t="n">
         <v>7</v>
       </c>
     </row>
@@ -2601,7 +3497,7 @@
         <v>23.53980811311227</v>
       </c>
       <c r="J19" t="n">
-        <v>11.03907072417057</v>
+        <v>10.88205819350233</v>
       </c>
       <c r="K19" t="n">
         <v>30</v>
@@ -2613,75 +3509,123 @@
         <v>-0.07760962359333323</v>
       </c>
       <c r="N19" t="n">
-        <v>18.22105312983866</v>
+        <v>-20.007193</v>
       </c>
       <c r="O19" t="n">
+        <v>-8.432029999999999</v>
+      </c>
+      <c r="P19" t="n">
+        <v>-5.6037455</v>
+      </c>
+      <c r="Q19" t="n">
+        <v>-19.265</v>
+      </c>
+      <c r="R19" t="n">
+        <v>-43.9</v>
+      </c>
+      <c r="S19" t="n">
+        <v>-66.87507419383033</v>
+      </c>
+      <c r="T19" t="n">
+        <v>0.1908295315356896</v>
+      </c>
+      <c r="U19" t="n">
+        <v>9.197162061239732</v>
+      </c>
+      <c r="V19" t="n">
+        <v>12.98702941412517</v>
+      </c>
+      <c r="W19" t="n">
         <v>11</v>
       </c>
-      <c r="P19" t="n">
+      <c r="X19" t="n">
         <v>20.5</v>
       </c>
-      <c r="Q19" t="n">
+      <c r="Y19" t="n">
+        <v>19</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>10</v>
+      </c>
+      <c r="AA19" t="n">
         <v>2</v>
       </c>
-      <c r="R19" t="n">
-        <v>10</v>
-      </c>
-      <c r="S19" t="n">
+      <c r="AB19" t="n">
+        <v>5</v>
+      </c>
+      <c r="AC19" t="n">
+        <v>8</v>
+      </c>
+      <c r="AD19" t="n">
+        <v>8</v>
+      </c>
+      <c r="AE19" t="n">
+        <v>9</v>
+      </c>
+      <c r="AF19" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="AG19" t="n">
+        <v>21</v>
+      </c>
+      <c r="AH19" t="n">
+        <v>18</v>
+      </c>
+      <c r="AI19" t="n">
+        <v>8</v>
+      </c>
+      <c r="AJ19" t="n">
+        <v>13</v>
+      </c>
+      <c r="AK19" t="n">
+        <v>11</v>
+      </c>
+      <c r="AL19" t="n">
+        <v>13</v>
+      </c>
+      <c r="AM19" t="n">
+        <v>4</v>
+      </c>
+      <c r="AN19" t="n">
+        <v>21</v>
+      </c>
+      <c r="AO19" t="n">
+        <v>20</v>
+      </c>
+      <c r="AP19" t="n">
         <v>19</v>
       </c>
-      <c r="T19" t="n">
+      <c r="AQ19" t="n">
+        <v>13</v>
+      </c>
+      <c r="AR19" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS19" t="n">
         <v>5</v>
       </c>
-      <c r="U19" t="n">
-        <v>8</v>
-      </c>
-      <c r="V19" t="n">
-        <v>8</v>
-      </c>
-      <c r="W19" t="n">
+      <c r="AT19" t="n">
         <v>9</v>
       </c>
-      <c r="X19" t="n">
-        <v>23.5</v>
-      </c>
-      <c r="Y19" t="n">
-        <v>21</v>
-      </c>
-      <c r="Z19" t="n">
-        <v>18</v>
-      </c>
-      <c r="AA19" t="n">
-        <v>11</v>
-      </c>
-      <c r="AB19" t="n">
-        <v>3</v>
-      </c>
-      <c r="AC19" t="n">
-        <v>5</v>
-      </c>
-      <c r="AD19" t="n">
-        <v>9</v>
-      </c>
-      <c r="AE19" t="n">
+      <c r="AU19" t="n">
         <v>6.959999999999999</v>
       </c>
-      <c r="AF19" t="n">
+      <c r="AV19" t="n">
         <v>5.294</v>
       </c>
-      <c r="AG19" t="n">
+      <c r="AW19" t="n">
         <v>-2</v>
       </c>
-      <c r="AH19" t="n">
-        <v>11</v>
-      </c>
-      <c r="AI19" t="n">
+      <c r="AX19" t="n">
+        <v>13</v>
+      </c>
+      <c r="AY19" t="n">
         <v>15</v>
       </c>
-      <c r="AJ19" t="n">
-        <v>15.83333333333333</v>
-      </c>
-      <c r="AK19" t="n">
+      <c r="AZ19" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="BA19" t="n">
         <v>21.5</v>
       </c>
     </row>
@@ -2716,7 +3660,7 @@
         <v>3.85414624583415</v>
       </c>
       <c r="J20" t="n">
-        <v>1.090352630653325</v>
+        <v>1.098445183005373</v>
       </c>
       <c r="K20" t="n">
         <v>40</v>
@@ -2728,75 +3672,123 @@
         <v>2.030008826125329</v>
       </c>
       <c r="N20" t="n">
-        <v>11.60538451619294</v>
+        <v>-22.035713</v>
       </c>
       <c r="O20" t="n">
-        <v>23</v>
+        <v>-3.8634846</v>
       </c>
       <c r="P20" t="n">
-        <v>9</v>
+        <v>-2.0051274</v>
       </c>
       <c r="Q20" t="n">
-        <v>15</v>
+        <v>-14.146</v>
       </c>
       <c r="R20" t="n">
-        <v>18</v>
+        <v>-81.8</v>
       </c>
       <c r="S20" t="n">
-        <v>23</v>
+        <v>-14.6143510056393</v>
       </c>
       <c r="T20" t="n">
-        <v>20</v>
+        <v>4.23207808758245</v>
       </c>
       <c r="U20" t="n">
-        <v>25</v>
+        <v>21.56525066972828</v>
       </c>
       <c r="V20" t="n">
-        <v>25</v>
+        <v>8.642770463208505</v>
       </c>
       <c r="W20" t="n">
         <v>23</v>
       </c>
       <c r="X20" t="n">
+        <v>9</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>23</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>18</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>15</v>
+      </c>
+      <c r="AB20" t="n">
+        <v>20</v>
+      </c>
+      <c r="AC20" t="n">
+        <v>25</v>
+      </c>
+      <c r="AD20" t="n">
+        <v>25</v>
+      </c>
+      <c r="AE20" t="n">
+        <v>23</v>
+      </c>
+      <c r="AF20" t="n">
         <v>11</v>
       </c>
-      <c r="Y20" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z20" t="n">
+      <c r="AG20" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH20" t="n">
         <v>13</v>
       </c>
-      <c r="AA20" t="n">
-        <v>19</v>
-      </c>
-      <c r="AB20" t="n">
+      <c r="AI20" t="n">
+        <v>9</v>
+      </c>
+      <c r="AJ20" t="n">
+        <v>9</v>
+      </c>
+      <c r="AK20" t="n">
+        <v>6</v>
+      </c>
+      <c r="AL20" t="n">
+        <v>7</v>
+      </c>
+      <c r="AM20" t="n">
+        <v>8</v>
+      </c>
+      <c r="AN20" t="n">
+        <v>4</v>
+      </c>
+      <c r="AO20" t="n">
+        <v>14</v>
+      </c>
+      <c r="AP20" t="n">
         <v>3</v>
       </c>
-      <c r="AC20" t="n">
+      <c r="AQ20" t="n">
+        <v>18</v>
+      </c>
+      <c r="AR20" t="n">
+        <v>3</v>
+      </c>
+      <c r="AS20" t="n">
         <v>5</v>
       </c>
-      <c r="AD20" t="n">
+      <c r="AT20" t="n">
         <v>1</v>
       </c>
-      <c r="AE20" t="n">
+      <c r="AU20" t="n">
         <v>7.92</v>
       </c>
-      <c r="AF20" t="n">
+      <c r="AV20" t="n">
         <v>4.238</v>
       </c>
-      <c r="AG20" t="n">
+      <c r="AW20" t="n">
         <v>-2</v>
       </c>
-      <c r="AH20" t="n">
-        <v>19</v>
-      </c>
-      <c r="AI20" t="n">
+      <c r="AX20" t="n">
+        <v>18</v>
+      </c>
+      <c r="AY20" t="n">
         <v>17</v>
       </c>
-      <c r="AJ20" t="n">
-        <v>19.16666666666667</v>
-      </c>
-      <c r="AK20" t="n">
+      <c r="AZ20" t="n">
+        <v>18.83333333333333</v>
+      </c>
+      <c r="BA20" t="n">
         <v>21.5</v>
       </c>
     </row>
@@ -2831,7 +3823,7 @@
         <v>57.01102979074322</v>
       </c>
       <c r="J21" t="n">
-        <v>0.2382001836300649</v>
+        <v>0.2366152385206008</v>
       </c>
       <c r="K21" t="n">
         <v>40</v>
@@ -2843,75 +3835,123 @@
         <v>6.473192326610921</v>
       </c>
       <c r="N21" t="n">
-        <v>9.900858274619116</v>
+        <v>-14.171155</v>
       </c>
       <c r="O21" t="n">
+        <v>-2.575629</v>
+      </c>
+      <c r="P21" t="n">
+        <v>-0.95275617</v>
+      </c>
+      <c r="Q21" t="n">
+        <v>0.073</v>
+      </c>
+      <c r="R21" t="n">
+        <v>-140</v>
+      </c>
+      <c r="S21" t="n">
+        <v>-35.06301256914385</v>
+      </c>
+      <c r="T21" t="n">
+        <v>-1.374915265762693</v>
+      </c>
+      <c r="U21" t="n">
+        <v>-15.50938337801609</v>
+      </c>
+      <c r="V21" t="n">
+        <v>6.681589930541358</v>
+      </c>
+      <c r="W21" t="n">
         <v>19</v>
       </c>
-      <c r="P21" t="n">
+      <c r="X21" t="n">
         <v>23</v>
       </c>
-      <c r="Q21" t="n">
+      <c r="Y21" t="n">
+        <v>19</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>17</v>
+      </c>
+      <c r="AA21" t="n">
         <v>25</v>
       </c>
-      <c r="R21" t="n">
-        <v>17</v>
-      </c>
-      <c r="S21" t="n">
-        <v>19</v>
-      </c>
-      <c r="T21" t="n">
+      <c r="AB21" t="n">
         <v>22</v>
       </c>
-      <c r="U21" t="n">
+      <c r="AC21" t="n">
         <v>3</v>
       </c>
-      <c r="V21" t="n">
+      <c r="AD21" t="n">
         <v>3</v>
       </c>
-      <c r="W21" t="n">
+      <c r="AE21" t="n">
         <v>26</v>
       </c>
-      <c r="X21" t="n">
+      <c r="AF21" t="n">
         <v>11</v>
       </c>
-      <c r="Y21" t="n">
+      <c r="AG21" t="n">
         <v>24</v>
       </c>
-      <c r="Z21" t="n">
+      <c r="AH21" t="n">
         <v>6</v>
       </c>
-      <c r="AA21" t="n">
+      <c r="AI21" t="n">
+        <v>3</v>
+      </c>
+      <c r="AJ21" t="n">
+        <v>5</v>
+      </c>
+      <c r="AK21" t="n">
+        <v>2</v>
+      </c>
+      <c r="AL21" t="n">
+        <v>1</v>
+      </c>
+      <c r="AM21" t="n">
         <v>20</v>
       </c>
-      <c r="AB21" t="n">
+      <c r="AN21" t="n">
+        <v>15</v>
+      </c>
+      <c r="AO21" t="n">
+        <v>21</v>
+      </c>
+      <c r="AP21" t="n">
+        <v>26</v>
+      </c>
+      <c r="AQ21" t="n">
+        <v>20</v>
+      </c>
+      <c r="AR21" t="n">
         <v>5</v>
       </c>
-      <c r="AC21" t="n">
+      <c r="AS21" t="n">
         <v>0</v>
       </c>
-      <c r="AD21" t="n">
+      <c r="AT21" t="n">
         <v>12</v>
       </c>
-      <c r="AE21" t="n">
+      <c r="AU21" t="n">
         <v>8.92</v>
       </c>
-      <c r="AF21" t="n">
+      <c r="AV21" t="n">
         <v>4.638</v>
       </c>
-      <c r="AG21" t="n">
+      <c r="AW21" t="n">
         <v>-2</v>
       </c>
-      <c r="AH21" t="n">
+      <c r="AX21" t="n">
         <v>20</v>
       </c>
-      <c r="AI21" t="n">
+      <c r="AY21" t="n">
         <v>16</v>
       </c>
-      <c r="AJ21" t="n">
+      <c r="AZ21" t="n">
         <v>19.16666666666667</v>
       </c>
-      <c r="AK21" t="n">
+      <c r="BA21" t="n">
         <v>21.5</v>
       </c>
     </row>
@@ -2946,7 +3986,7 @@
         <v>9.848595300846746</v>
       </c>
       <c r="J22" t="n">
-        <v>1.435752144752943</v>
+        <v>1.463938293126425</v>
       </c>
       <c r="K22" t="n">
         <v>30</v>
@@ -2958,75 +3998,123 @@
         <v>-5.444690810544461</v>
       </c>
       <c r="N22" t="n">
-        <v>2.31309870506679</v>
+        <v>-31.762783</v>
       </c>
       <c r="O22" t="n">
+        <v>-2.7113304</v>
+      </c>
+      <c r="P22" t="n">
+        <v>-1.3777176</v>
+      </c>
+      <c r="Q22" t="n">
+        <v>-18.024</v>
+      </c>
+      <c r="R22" t="n">
+        <v>-123</v>
+      </c>
+      <c r="S22" t="n">
+        <v>-115.4777074378162</v>
+      </c>
+      <c r="T22" t="n">
+        <v>13.763900552205</v>
+      </c>
+      <c r="U22" t="n">
+        <v>-4.418852633823843</v>
+      </c>
+      <c r="V22" t="n">
+        <v>-1.915161541857004</v>
+      </c>
+      <c r="W22" t="n">
         <v>26</v>
       </c>
-      <c r="P22" t="n">
+      <c r="X22" t="n">
         <v>20.5</v>
       </c>
-      <c r="Q22" t="n">
+      <c r="Y22" t="n">
+        <v>19</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>26</v>
+      </c>
+      <c r="AA22" t="n">
         <v>20</v>
       </c>
-      <c r="R22" t="n">
+      <c r="AB22" t="n">
+        <v>16</v>
+      </c>
+      <c r="AC22" t="n">
+        <v>19</v>
+      </c>
+      <c r="AD22" t="n">
+        <v>19</v>
+      </c>
+      <c r="AE22" t="n">
+        <v>21</v>
+      </c>
+      <c r="AF22" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="AG22" t="n">
         <v>26</v>
       </c>
-      <c r="S22" t="n">
-        <v>19</v>
-      </c>
-      <c r="T22" t="n">
+      <c r="AH22" t="n">
+        <v>23</v>
+      </c>
+      <c r="AI22" t="n">
         <v>16</v>
       </c>
-      <c r="U22" t="n">
-        <v>19</v>
-      </c>
-      <c r="V22" t="n">
-        <v>19</v>
-      </c>
-      <c r="W22" t="n">
-        <v>21</v>
-      </c>
-      <c r="X22" t="n">
-        <v>23.5</v>
-      </c>
-      <c r="Y22" t="n">
+      <c r="AJ22" t="n">
+        <v>6</v>
+      </c>
+      <c r="AK22" t="n">
+        <v>4</v>
+      </c>
+      <c r="AL22" t="n">
+        <v>9</v>
+      </c>
+      <c r="AM22" t="n">
+        <v>15</v>
+      </c>
+      <c r="AN22" t="n">
         <v>26</v>
       </c>
-      <c r="Z22" t="n">
+      <c r="AO22" t="n">
+        <v>1</v>
+      </c>
+      <c r="AP22" t="n">
         <v>23</v>
       </c>
-      <c r="AA22" t="n">
+      <c r="AQ22" t="n">
         <v>26</v>
       </c>
-      <c r="AB22" t="n">
+      <c r="AR22" t="n">
         <v>0</v>
       </c>
-      <c r="AC22" t="n">
+      <c r="AS22" t="n">
         <v>0</v>
       </c>
-      <c r="AD22" t="n">
+      <c r="AT22" t="n">
         <v>9</v>
       </c>
-      <c r="AE22" t="n">
+      <c r="AU22" t="n">
         <v>7.080000000000001</v>
       </c>
-      <c r="AF22" t="n">
+      <c r="AV22" t="n">
         <v>2.412</v>
       </c>
-      <c r="AG22" t="n">
+      <c r="AW22" t="n">
         <v>-2</v>
       </c>
-      <c r="AH22" t="n">
+      <c r="AX22" t="n">
         <v>26</v>
       </c>
-      <c r="AI22" t="n">
+      <c r="AY22" t="n">
         <v>25</v>
       </c>
-      <c r="AJ22" t="n">
+      <c r="AZ22" t="n">
         <v>24.16666666666667</v>
       </c>
-      <c r="AK22" t="n">
+      <c r="BA22" t="n">
         <v>21.5</v>
       </c>
     </row>
@@ -3061,7 +4149,7 @@
         <v>15.04922521396774</v>
       </c>
       <c r="J23" t="n">
-        <v>1.850434833301343</v>
+        <v>1.871579964907891</v>
       </c>
       <c r="K23" t="n">
         <v>40</v>
@@ -3073,75 +4161,123 @@
         <v>12.83514240653122</v>
       </c>
       <c r="N23" t="n">
-        <v>17.0160278732489</v>
+        <v>-17.86221</v>
       </c>
       <c r="O23" t="n">
+        <v>-0.42557862</v>
+      </c>
+      <c r="P23" t="n">
+        <v>-0.40371707</v>
+      </c>
+      <c r="Q23" t="n">
+        <v>-15.904</v>
+      </c>
+      <c r="R23" t="n">
+        <v>-10</v>
+      </c>
+      <c r="S23" t="n">
+        <v>-36.0547333105999</v>
+      </c>
+      <c r="T23" t="n">
+        <v>1.851208301394448</v>
+      </c>
+      <c r="U23" t="n">
+        <v>12.567078372749</v>
+      </c>
+      <c r="V23" t="n">
+        <v>14.07464531357968</v>
+      </c>
+      <c r="W23" t="n">
         <v>18</v>
       </c>
-      <c r="P23" t="n">
+      <c r="X23" t="n">
         <v>2</v>
       </c>
-      <c r="Q23" t="n">
+      <c r="Y23" t="n">
+        <v>15</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>20</v>
+      </c>
+      <c r="AA23" t="n">
         <v>21</v>
       </c>
-      <c r="R23" t="n">
+      <c r="AB23" t="n">
+        <v>9</v>
+      </c>
+      <c r="AC23" t="n">
+        <v>15</v>
+      </c>
+      <c r="AD23" t="n">
+        <v>14</v>
+      </c>
+      <c r="AE23" t="n">
         <v>20</v>
       </c>
-      <c r="S23" t="n">
-        <v>15</v>
-      </c>
-      <c r="T23" t="n">
-        <v>9</v>
-      </c>
-      <c r="U23" t="n">
-        <v>15</v>
-      </c>
-      <c r="V23" t="n">
-        <v>14</v>
-      </c>
-      <c r="W23" t="n">
-        <v>20</v>
-      </c>
-      <c r="X23" t="n">
+      <c r="AF23" t="n">
         <v>11</v>
       </c>
-      <c r="Y23" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z23" t="n">
+      <c r="AG23" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH23" t="n">
         <v>2</v>
       </c>
-      <c r="AA23" t="n">
-        <v>14</v>
-      </c>
-      <c r="AB23" t="n">
+      <c r="AI23" t="n">
+        <v>5</v>
+      </c>
+      <c r="AJ23" t="n">
         <v>1</v>
       </c>
-      <c r="AC23" t="n">
+      <c r="AK23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AL23" t="n">
+        <v>8</v>
+      </c>
+      <c r="AM23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AN23" t="n">
+        <v>16</v>
+      </c>
+      <c r="AO23" t="n">
+        <v>19</v>
+      </c>
+      <c r="AP23" t="n">
+        <v>17</v>
+      </c>
+      <c r="AQ23" t="n">
+        <v>11</v>
+      </c>
+      <c r="AR23" t="n">
+        <v>1</v>
+      </c>
+      <c r="AS23" t="n">
         <v>0</v>
       </c>
-      <c r="AD23" t="n">
+      <c r="AT23" t="n">
         <v>16</v>
       </c>
-      <c r="AE23" t="n">
+      <c r="AU23" t="n">
         <v>9.960000000000001</v>
       </c>
-      <c r="AF23" t="n">
+      <c r="AV23" t="n">
         <v>4.194</v>
       </c>
-      <c r="AG23" t="n">
+      <c r="AW23" t="n">
         <v>0</v>
       </c>
-      <c r="AH23" t="n">
-        <v>14</v>
-      </c>
-      <c r="AI23" t="n">
+      <c r="AX23" t="n">
+        <v>11</v>
+      </c>
+      <c r="AY23" t="n">
         <v>18</v>
       </c>
-      <c r="AJ23" t="n">
-        <v>14.83333333333333</v>
-      </c>
-      <c r="AK23" t="n">
+      <c r="AZ23" t="n">
+        <v>13.83333333333333</v>
+      </c>
+      <c r="BA23" t="n">
         <v>12.5</v>
       </c>
     </row>
@@ -3176,7 +4312,7 @@
         <v>11.2918334326833</v>
       </c>
       <c r="J24" t="n">
-        <v>3.100091378094315</v>
+        <v>3.127922830386768</v>
       </c>
       <c r="K24" t="n">
         <v>40</v>
@@ -3188,75 +4324,123 @@
         <v>-0.2904102817597565</v>
       </c>
       <c r="N24" t="n">
-        <v>8.813281749305151</v>
+        <v>-9.404692000000001</v>
       </c>
       <c r="O24" t="n">
+        <v>-1.9280291</v>
+      </c>
+      <c r="P24" t="n">
+        <v>-1.7894207</v>
+      </c>
+      <c r="Q24" t="n">
+        <v>-6.662</v>
+      </c>
+      <c r="R24" t="n">
+        <v>-62.6</v>
+      </c>
+      <c r="S24" t="n">
+        <v>-31.43509248397971</v>
+      </c>
+      <c r="T24" t="n">
+        <v>3.937306637090654</v>
+      </c>
+      <c r="U24" t="n">
+        <v>13.50328947368421</v>
+      </c>
+      <c r="V24" t="n">
+        <v>6.031961772324975</v>
+      </c>
+      <c r="W24" t="n">
         <v>25</v>
       </c>
-      <c r="P24" t="n">
+      <c r="X24" t="n">
         <v>24</v>
       </c>
-      <c r="Q24" t="n">
+      <c r="Y24" t="n">
+        <v>25</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>12</v>
+      </c>
+      <c r="AA24" t="n">
         <v>11</v>
       </c>
-      <c r="R24" t="n">
+      <c r="AB24" t="n">
+        <v>11</v>
+      </c>
+      <c r="AC24" t="n">
+        <v>14</v>
+      </c>
+      <c r="AD24" t="n">
+        <v>17</v>
+      </c>
+      <c r="AE24" t="n">
+        <v>18</v>
+      </c>
+      <c r="AF24" t="n">
+        <v>11</v>
+      </c>
+      <c r="AG24" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH24" t="n">
+        <v>19</v>
+      </c>
+      <c r="AI24" t="n">
+        <v>2</v>
+      </c>
+      <c r="AJ24" t="n">
+        <v>3</v>
+      </c>
+      <c r="AK24" t="n">
+        <v>5</v>
+      </c>
+      <c r="AL24" t="n">
+        <v>5</v>
+      </c>
+      <c r="AM24" t="n">
+        <v>6</v>
+      </c>
+      <c r="AN24" t="n">
+        <v>13</v>
+      </c>
+      <c r="AO24" t="n">
+        <v>15</v>
+      </c>
+      <c r="AP24" t="n">
         <v>12</v>
       </c>
-      <c r="S24" t="n">
-        <v>25</v>
-      </c>
-      <c r="T24" t="n">
-        <v>11</v>
-      </c>
-      <c r="U24" t="n">
-        <v>14</v>
-      </c>
-      <c r="V24" t="n">
-        <v>17</v>
-      </c>
-      <c r="W24" t="n">
-        <v>18</v>
-      </c>
-      <c r="X24" t="n">
-        <v>11</v>
-      </c>
-      <c r="Y24" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z24" t="n">
-        <v>19</v>
-      </c>
-      <c r="AA24" t="n">
-        <v>22</v>
-      </c>
-      <c r="AB24" t="n">
+      <c r="AQ24" t="n">
+        <v>21</v>
+      </c>
+      <c r="AR24" t="n">
         <v>0</v>
       </c>
-      <c r="AC24" t="n">
-        <v>10</v>
-      </c>
-      <c r="AD24" t="n">
+      <c r="AS24" t="n">
+        <v>10</v>
+      </c>
+      <c r="AT24" t="n">
         <v>5</v>
       </c>
-      <c r="AE24" t="n">
+      <c r="AU24" t="n">
         <v>7.759999999999999</v>
       </c>
-      <c r="AF24" t="n">
+      <c r="AV24" t="n">
         <v>5.914</v>
       </c>
-      <c r="AG24" t="n">
+      <c r="AW24" t="n">
         <v>-2</v>
       </c>
-      <c r="AH24" t="n">
-        <v>22</v>
-      </c>
-      <c r="AI24" t="n">
+      <c r="AX24" t="n">
+        <v>21</v>
+      </c>
+      <c r="AY24" t="n">
         <v>13</v>
       </c>
-      <c r="AJ24" t="n">
-        <v>18.83333333333333</v>
-      </c>
-      <c r="AK24" t="n">
+      <c r="AZ24" t="n">
+        <v>18.5</v>
+      </c>
+      <c r="BA24" t="n">
         <v>21.5</v>
       </c>
     </row>
@@ -3291,7 +4475,7 @@
         <v>1.633187042671735</v>
       </c>
       <c r="J25" t="n">
-        <v>2.070590706659692</v>
+        <v>2.072377747003896</v>
       </c>
       <c r="K25" t="n">
         <v>40</v>
@@ -3303,75 +4487,123 @@
         <v>-1.327330652992109</v>
       </c>
       <c r="N25" t="n">
-        <v>13.16083757257699</v>
+        <v>-38.603546</v>
       </c>
       <c r="O25" t="n">
+        <v>-8.432829999999999</v>
+      </c>
+      <c r="P25" t="n">
+        <v>-2.2554884</v>
+      </c>
+      <c r="Q25" t="n">
+        <v>-18.443</v>
+      </c>
+      <c r="R25" t="n">
+        <v>-94</v>
+      </c>
+      <c r="S25" t="n">
+        <v>-22.30591767442485</v>
+      </c>
+      <c r="T25" t="n">
+        <v>2.581220394797471</v>
+      </c>
+      <c r="U25" t="n">
+        <v>15.19173494517928</v>
+      </c>
+      <c r="V25" t="n">
+        <v>8.946967212645861</v>
+      </c>
+      <c r="W25" t="n">
         <v>17</v>
       </c>
-      <c r="P25" t="n">
+      <c r="X25" t="n">
         <v>19</v>
       </c>
-      <c r="Q25" t="n">
-        <v>10</v>
-      </c>
-      <c r="R25" t="n">
+      <c r="Y25" t="n">
+        <v>9</v>
+      </c>
+      <c r="Z25" t="n">
         <v>5</v>
       </c>
-      <c r="S25" t="n">
+      <c r="AA25" t="n">
+        <v>10</v>
+      </c>
+      <c r="AB25" t="n">
+        <v>18</v>
+      </c>
+      <c r="AC25" t="n">
+        <v>26</v>
+      </c>
+      <c r="AD25" t="n">
+        <v>26</v>
+      </c>
+      <c r="AE25" t="n">
+        <v>19</v>
+      </c>
+      <c r="AF25" t="n">
+        <v>11</v>
+      </c>
+      <c r="AG25" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH25" t="n">
+        <v>20</v>
+      </c>
+      <c r="AI25" t="n">
+        <v>21</v>
+      </c>
+      <c r="AJ25" t="n">
+        <v>14</v>
+      </c>
+      <c r="AK25" t="n">
+        <v>7</v>
+      </c>
+      <c r="AL25" t="n">
+        <v>11</v>
+      </c>
+      <c r="AM25" t="n">
         <v>9</v>
       </c>
-      <c r="T25" t="n">
-        <v>18</v>
-      </c>
-      <c r="U25" t="n">
-        <v>26</v>
-      </c>
-      <c r="V25" t="n">
-        <v>26</v>
-      </c>
-      <c r="W25" t="n">
-        <v>19</v>
-      </c>
-      <c r="X25" t="n">
-        <v>11</v>
-      </c>
-      <c r="Y25" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z25" t="n">
-        <v>20</v>
-      </c>
-      <c r="AA25" t="n">
+      <c r="AN25" t="n">
+        <v>8</v>
+      </c>
+      <c r="AO25" t="n">
         <v>17</v>
       </c>
-      <c r="AB25" t="n">
+      <c r="AP25" t="n">
+        <v>9</v>
+      </c>
+      <c r="AQ25" t="n">
+        <v>16</v>
+      </c>
+      <c r="AR25" t="n">
         <v>1</v>
       </c>
-      <c r="AC25" t="n">
+      <c r="AS25" t="n">
         <v>5</v>
       </c>
-      <c r="AD25" t="n">
+      <c r="AT25" t="n">
         <v>3</v>
       </c>
-      <c r="AE25" t="n">
+      <c r="AU25" t="n">
         <v>8.44</v>
       </c>
-      <c r="AF25" t="n">
+      <c r="AV25" t="n">
         <v>4.016</v>
       </c>
-      <c r="AG25" t="n">
+      <c r="AW25" t="n">
         <v>-2</v>
       </c>
-      <c r="AH25" t="n">
-        <v>17</v>
-      </c>
-      <c r="AI25" t="n">
+      <c r="AX25" t="n">
+        <v>16</v>
+      </c>
+      <c r="AY25" t="n">
         <v>22</v>
       </c>
-      <c r="AJ25" t="n">
-        <v>20.16666666666667</v>
-      </c>
-      <c r="AK25" t="n">
+      <c r="AZ25" t="n">
+        <v>19.83333333333333</v>
+      </c>
+      <c r="BA25" t="n">
         <v>21.5</v>
       </c>
     </row>
@@ -3406,7 +4638,7 @@
         <v>9.461894953656024</v>
       </c>
       <c r="J26" t="n">
-        <v>3.495138873517946</v>
+        <v>3.509094495042173</v>
       </c>
       <c r="K26" t="n">
         <v>40</v>
@@ -3418,75 +4650,123 @@
         <v>13.78437047756874</v>
       </c>
       <c r="N26" t="n">
-        <v>5.60088810210565</v>
+        <v>-17.303806</v>
       </c>
       <c r="O26" t="n">
+        <v>-1.5806433</v>
+      </c>
+      <c r="P26" t="n">
+        <v>-21.15654</v>
+      </c>
+      <c r="Q26" t="n">
+        <v>-18.622</v>
+      </c>
+      <c r="R26" t="n">
+        <v>-26.2</v>
+      </c>
+      <c r="S26" t="n">
+        <v>-9.885073471050896</v>
+      </c>
+      <c r="T26" t="n">
+        <v>2.941546649405757</v>
+      </c>
+      <c r="U26" t="n">
+        <v>13.06596701649175</v>
+      </c>
+      <c r="V26" t="n">
+        <v>4.243071781557444</v>
+      </c>
+      <c r="W26" t="n">
         <v>21</v>
       </c>
-      <c r="P26" t="n">
+      <c r="X26" t="n">
         <v>18</v>
       </c>
-      <c r="Q26" t="n">
+      <c r="Y26" t="n">
+        <v>22</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>21</v>
+      </c>
+      <c r="AA26" t="n">
         <v>26</v>
       </c>
-      <c r="R26" t="n">
+      <c r="AB26" t="n">
+        <v>26</v>
+      </c>
+      <c r="AC26" t="n">
         <v>21</v>
       </c>
-      <c r="S26" t="n">
-        <v>22</v>
-      </c>
-      <c r="T26" t="n">
-        <v>26</v>
-      </c>
-      <c r="U26" t="n">
-        <v>21</v>
-      </c>
-      <c r="V26" t="n">
+      <c r="AD26" t="n">
         <v>20</v>
       </c>
-      <c r="W26" t="n">
+      <c r="AE26" t="n">
         <v>17</v>
       </c>
-      <c r="X26" t="n">
+      <c r="AF26" t="n">
         <v>11</v>
       </c>
-      <c r="Y26" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z26" t="n">
+      <c r="AG26" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH26" t="n">
         <v>1</v>
       </c>
-      <c r="AA26" t="n">
-        <v>24</v>
-      </c>
-      <c r="AB26" t="n">
+      <c r="AI26" t="n">
+        <v>4</v>
+      </c>
+      <c r="AJ26" t="n">
+        <v>2</v>
+      </c>
+      <c r="AK26" t="n">
+        <v>19</v>
+      </c>
+      <c r="AL26" t="n">
+        <v>12</v>
+      </c>
+      <c r="AM26" t="n">
+        <v>3</v>
+      </c>
+      <c r="AN26" t="n">
+        <v>2</v>
+      </c>
+      <c r="AO26" t="n">
+        <v>16</v>
+      </c>
+      <c r="AP26" t="n">
+        <v>14</v>
+      </c>
+      <c r="AQ26" t="n">
+        <v>23</v>
+      </c>
+      <c r="AR26" t="n">
         <v>0</v>
       </c>
-      <c r="AC26" t="n">
+      <c r="AS26" t="n">
         <v>5</v>
       </c>
-      <c r="AD26" t="n">
+      <c r="AT26" t="n">
         <v>8</v>
       </c>
-      <c r="AE26" t="n">
+      <c r="AU26" t="n">
         <v>6.2</v>
       </c>
-      <c r="AF26" t="n">
+      <c r="AV26" t="n">
         <v>4.13</v>
       </c>
-      <c r="AG26" t="n">
+      <c r="AW26" t="n">
         <v>-2</v>
       </c>
-      <c r="AH26" t="n">
-        <v>24</v>
-      </c>
-      <c r="AI26" t="n">
+      <c r="AX26" t="n">
+        <v>23</v>
+      </c>
+      <c r="AY26" t="n">
         <v>19</v>
       </c>
-      <c r="AJ26" t="n">
-        <v>21.5</v>
-      </c>
-      <c r="AK26" t="n">
+      <c r="AZ26" t="n">
+        <v>21.16666666666667</v>
+      </c>
+      <c r="BA26" t="n">
         <v>21.5</v>
       </c>
     </row>
@@ -3521,7 +4801,7 @@
         <v>5.163527717014352</v>
       </c>
       <c r="J27" t="n">
-        <v>1.372017380596165</v>
+        <v>1.367606298185855</v>
       </c>
       <c r="K27" t="n">
         <v>30</v>
@@ -3533,75 +4813,123 @@
         <v>3.191954525579366</v>
       </c>
       <c r="N27" t="n">
-        <v>8.542189320018256</v>
+        <v>-0.10475781</v>
       </c>
       <c r="O27" t="n">
-        <v>22</v>
+        <v>-3.3193715</v>
       </c>
       <c r="P27" t="n">
-        <v>25</v>
+        <v>-189.10521</v>
       </c>
       <c r="Q27" t="n">
-        <v>3</v>
+        <v>-9.476000000000001</v>
       </c>
       <c r="R27" t="n">
-        <v>25</v>
+        <v>-15.9</v>
       </c>
       <c r="S27" t="n">
-        <v>12</v>
+        <v>-113.6662432659112</v>
       </c>
       <c r="T27" t="n">
-        <v>17</v>
+        <v>5.93528961555606</v>
       </c>
       <c r="U27" t="n">
-        <v>24</v>
+        <v>33.0019556714472</v>
       </c>
       <c r="V27" t="n">
-        <v>24</v>
+        <v>3.387334335792863</v>
       </c>
       <c r="W27" t="n">
         <v>22</v>
       </c>
       <c r="X27" t="n">
+        <v>25</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>12</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>25</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>3</v>
+      </c>
+      <c r="AB27" t="n">
+        <v>17</v>
+      </c>
+      <c r="AC27" t="n">
+        <v>24</v>
+      </c>
+      <c r="AD27" t="n">
+        <v>24</v>
+      </c>
+      <c r="AE27" t="n">
+        <v>22</v>
+      </c>
+      <c r="AF27" t="n">
         <v>23.5</v>
       </c>
-      <c r="Y27" t="n">
-        <v>10</v>
-      </c>
-      <c r="Z27" t="n">
+      <c r="AG27" t="n">
+        <v>10</v>
+      </c>
+      <c r="AH27" t="n">
         <v>11</v>
       </c>
-      <c r="AA27" t="n">
-        <v>23</v>
-      </c>
-      <c r="AB27" t="n">
+      <c r="AI27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AJ27" t="n">
+        <v>7</v>
+      </c>
+      <c r="AK27" t="n">
+        <v>26</v>
+      </c>
+      <c r="AL27" t="n">
+        <v>6</v>
+      </c>
+      <c r="AM27" t="n">
+        <v>2</v>
+      </c>
+      <c r="AN27" t="n">
+        <v>25</v>
+      </c>
+      <c r="AO27" t="n">
+        <v>10</v>
+      </c>
+      <c r="AP27" t="n">
+        <v>1</v>
+      </c>
+      <c r="AQ27" t="n">
+        <v>24</v>
+      </c>
+      <c r="AR27" t="n">
         <v>16</v>
       </c>
-      <c r="AC27" t="n">
+      <c r="AS27" t="n">
         <v>5</v>
       </c>
-      <c r="AD27" t="n">
+      <c r="AT27" t="n">
         <v>18</v>
       </c>
-      <c r="AE27" t="n">
+      <c r="AU27" t="n">
         <v>8.120000000000001</v>
       </c>
-      <c r="AF27" t="n">
+      <c r="AV27" t="n">
         <v>10.718</v>
       </c>
-      <c r="AG27" t="n">
+      <c r="AW27" t="n">
         <v>-2</v>
       </c>
-      <c r="AH27" t="n">
-        <v>23</v>
-      </c>
-      <c r="AI27" t="n">
+      <c r="AX27" t="n">
+        <v>24</v>
+      </c>
+      <c r="AY27" t="n">
         <v>2</v>
       </c>
-      <c r="AJ27" t="n">
-        <v>15.5</v>
-      </c>
-      <c r="AK27" t="n">
+      <c r="AZ27" t="n">
+        <v>15.83333333333333</v>
+      </c>
+      <c r="BA27" t="n">
         <v>21.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added data preprocessing module, metric normalization
</commit_message>
<xml_diff>
--- a/output/stock_analysis_scores.xlsx
+++ b/output/stock_analysis_scores.xlsx
@@ -646,22 +646,22 @@
       </c>
       <c r="AR1" s="1" t="inlineStr">
         <is>
-          <t>MOAT Text Score</t>
+          <t>MOAT_TEXT</t>
         </is>
       </c>
       <c r="AS1" s="1" t="inlineStr">
         <is>
-          <t>MOAT Quant Score</t>
+          <t>MOAT_QUANT</t>
         </is>
       </c>
       <c r="AT1" s="1" t="inlineStr">
         <is>
-          <t>Management Score</t>
+          <t>MANAGEMENT</t>
         </is>
       </c>
       <c r="AU1" s="1" t="inlineStr">
         <is>
-          <t>Sentiment Score</t>
+          <t>SENTIMENT</t>
         </is>
       </c>
       <c r="AV1" s="1" t="inlineStr">
@@ -702,73 +702,73 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>12.42311465286305</v>
+        <v>0.3040976384676057</v>
       </c>
       <c r="C2" t="n">
-        <v>12.19743910249467</v>
+        <v>0.5060987195512474</v>
       </c>
       <c r="D2" t="n">
-        <v>69.16942403254254</v>
+        <v>0.6813239154170486</v>
       </c>
       <c r="E2" t="n">
-        <v>35.4160753571489</v>
+        <v>0.8806946560763196</v>
       </c>
       <c r="F2" t="n">
-        <v>3.202605420584792</v>
+        <v>0.5016013027102924</v>
       </c>
       <c r="G2" t="n">
-        <v>-1.763950634536609</v>
+        <v>0.9563696614683402</v>
       </c>
       <c r="H2" t="n">
-        <v>13.53446444504242</v>
+        <v>0.1672529553202128</v>
       </c>
       <c r="I2" t="n">
-        <v>13.46804231755159</v>
+        <v>0.1663195011416484</v>
       </c>
       <c r="J2" t="n">
-        <v>10.00165548536846</v>
+        <v>0.04717297044309587</v>
       </c>
       <c r="K2" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="L2" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="M2" t="n">
-        <v>0.8404482390608314</v>
+        <v>0.7265611810807434</v>
       </c>
       <c r="N2" t="n">
-        <v>-34.051506</v>
+        <v>0.9109327977518669</v>
       </c>
       <c r="O2" t="n">
-        <v>-13.431593</v>
+        <v>0.8943858253170122</v>
       </c>
       <c r="P2" t="n">
-        <v>-11.017878</v>
+        <v>0.9441324103030683</v>
       </c>
       <c r="Q2" t="n">
-        <v>-24.295</v>
+        <v>0.9652381284191277</v>
       </c>
       <c r="R2" t="n">
-        <v>-104</v>
+        <v>0.7697771246632378</v>
       </c>
       <c r="S2" t="n">
-        <v>-14.82592935155069</v>
+        <v>0.8980014932031215</v>
       </c>
       <c r="T2" t="n">
-        <v>5.546015124320884</v>
+        <v>0.6202643683746248</v>
       </c>
       <c r="U2" t="n">
-        <v>13.3712389032917</v>
+        <v>0.5953375612217265</v>
       </c>
       <c r="V2" t="n">
-        <v>15.68985484006297</v>
+        <v>0.5631956754380434</v>
       </c>
       <c r="W2" t="n">
         <v>12</v>
       </c>
       <c r="X2" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Y2" t="n">
         <v>10</v>
@@ -825,31 +825,31 @@
         <v>13</v>
       </c>
       <c r="AQ2" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AR2" t="n">
-        <v>3</v>
+        <v>0.1875</v>
       </c>
       <c r="AS2" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AT2" t="n">
-        <v>8</v>
+        <v>0.4117647058823529</v>
       </c>
       <c r="AU2" t="n">
-        <v>8.360000000000001</v>
+        <v>0.5857142857142862</v>
       </c>
       <c r="AV2" t="n">
-        <v>7.354000000000001</v>
+        <v>0.605871848739496</v>
       </c>
       <c r="AW2" t="n">
         <v>0</v>
       </c>
       <c r="AX2" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="AY2" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AZ2" t="n">
         <v>9.166666666666666</v>
@@ -865,67 +865,67 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>2.247001899501888</v>
+        <v>0.1794912288728406</v>
       </c>
       <c r="C3" t="n">
-        <v>2.522546249796354</v>
+        <v>0.5012612731248982</v>
       </c>
       <c r="D3" t="n">
-        <v>44.54903665126719</v>
+        <v>0.389841288930731</v>
       </c>
       <c r="E3" t="n">
-        <v>24.86237691315463</v>
+        <v>0.6589466170082152</v>
       </c>
       <c r="F3" t="n">
-        <v>5.389612680192757</v>
+        <v>0.5026948063400963</v>
       </c>
       <c r="G3" t="n">
-        <v>-18.72326602282704</v>
+        <v>0.4200678305604184</v>
       </c>
       <c r="H3" t="n">
-        <v>8.673125765340831</v>
+        <v>0.09893480479709411</v>
       </c>
       <c r="I3" t="n">
-        <v>8.260068483831466</v>
+        <v>0.09312996144177385</v>
       </c>
       <c r="J3" t="n">
-        <v>9.307753432726127</v>
+        <v>0.04380607548732765</v>
       </c>
       <c r="K3" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="L3" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="M3" t="n">
-        <v>8.128057551544575</v>
+        <v>0.8805110616835674</v>
       </c>
       <c r="N3" t="n">
-        <v>-30.27557</v>
+        <v>0.9207813685041114</v>
       </c>
       <c r="O3" t="n">
-        <v>-9.137214</v>
+        <v>0.929210906502052</v>
       </c>
       <c r="P3" t="n">
-        <v>-56.779503</v>
+        <v>0.7030576364069231</v>
       </c>
       <c r="Q3" t="n">
-        <v>-26.974</v>
+        <v>0.9618053136105278</v>
       </c>
       <c r="R3" t="n">
-        <v>-110.9</v>
+        <v>0.7528777859417095</v>
       </c>
       <c r="S3" t="n">
-        <v>-3.393508415778721</v>
+        <v>1</v>
       </c>
       <c r="T3" t="n">
-        <v>6.717628363197983</v>
+        <v>0.6744027835654773</v>
       </c>
       <c r="U3" t="n">
-        <v>12.61564393616113</v>
+        <v>0.5797619250522088</v>
       </c>
       <c r="V3" t="n">
-        <v>8.806003258094938</v>
+        <v>0.468088314943601</v>
       </c>
       <c r="W3" t="n">
         <v>20</v>
@@ -982,40 +982,40 @@
         <v>1</v>
       </c>
       <c r="AO3" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AP3" t="n">
         <v>16</v>
       </c>
       <c r="AQ3" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AR3" t="n">
-        <v>1</v>
+        <v>0.0625</v>
       </c>
       <c r="AS3" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AT3" t="n">
-        <v>8</v>
+        <v>0.4117647058823529</v>
       </c>
       <c r="AU3" t="n">
-        <v>7.359999999999999</v>
+        <v>0.4071428571428572</v>
       </c>
       <c r="AV3" t="n">
-        <v>6.604</v>
+        <v>0.5415861344537816</v>
       </c>
       <c r="AW3" t="n">
         <v>-1</v>
       </c>
       <c r="AX3" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AY3" t="n">
         <v>10</v>
       </c>
       <c r="AZ3" t="n">
-        <v>14.16666666666667</v>
+        <v>14.5</v>
       </c>
       <c r="BA3" t="n">
         <v>15.5</v>
@@ -1028,73 +1028,73 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>10.75433024222652</v>
+        <v>0.2836633882939869</v>
       </c>
       <c r="C4" t="n">
-        <v>12.60500501426027</v>
+        <v>0.5063025025071302</v>
       </c>
       <c r="D4" t="n">
-        <v>56.73497529799424</v>
+        <v>0.5341115373205079</v>
       </c>
       <c r="E4" t="n">
-        <v>24.60470947035482</v>
+        <v>0.6535326618458841</v>
       </c>
       <c r="F4" t="n">
-        <v>2.783009197173469</v>
+        <v>0.5013915045985867</v>
       </c>
       <c r="G4" t="n">
-        <v>-0.7832129541903016</v>
+        <v>0.9755099098559328</v>
       </c>
       <c r="H4" t="n">
-        <v>18.36931397410292</v>
+        <v>0.3112363605144653</v>
       </c>
       <c r="I4" t="n">
-        <v>18.36931397410292</v>
+        <v>0.3058218618737277</v>
       </c>
       <c r="J4" t="n">
-        <v>17.00455522292808</v>
+        <v>0.09369783883611271</v>
       </c>
       <c r="K4" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="L4" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="M4" t="n">
-        <v>7.743578222122371</v>
+        <v>0.8723889815444184</v>
       </c>
       <c r="N4" t="n">
-        <v>-27.662947</v>
+        <v>0.9280590770221323</v>
       </c>
       <c r="O4" t="n">
-        <v>-8.080947</v>
+        <v>0.9381715388346016</v>
       </c>
       <c r="P4" t="n">
-        <v>-8.266685000000001</v>
+        <v>0.9588308050046499</v>
       </c>
       <c r="Q4" t="n">
-        <v>-21.23</v>
+        <v>0.9702095951013421</v>
       </c>
       <c r="R4" t="n">
-        <v>-101.1</v>
+        <v>0.7768797452853293</v>
       </c>
       <c r="S4" t="n">
-        <v>-21.22957880377664</v>
+        <v>0.8408690025568093</v>
       </c>
       <c r="T4" t="n">
-        <v>5.592596211932767</v>
+        <v>0.6825488437978666</v>
       </c>
       <c r="U4" t="n">
-        <v>12.51513214407</v>
+        <v>0.5776900013729086</v>
       </c>
       <c r="V4" t="n">
-        <v>15.49746343477449</v>
+        <v>0.5646952859791136</v>
       </c>
       <c r="W4" t="n">
         <v>15</v>
       </c>
       <c r="X4" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Y4" t="n">
         <v>11</v>
@@ -1106,13 +1106,13 @@
         <v>12</v>
       </c>
       <c r="AB4" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AC4" t="n">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="AD4" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AE4" t="n">
         <v>5</v>
@@ -1145,40 +1145,40 @@
         <v>7</v>
       </c>
       <c r="AO4" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="AP4" t="n">
         <v>18</v>
       </c>
       <c r="AQ4" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="AR4" t="n">
-        <v>8</v>
+        <v>0.5</v>
       </c>
       <c r="AS4" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AT4" t="n">
-        <v>7</v>
+        <v>0.3529411764705883</v>
       </c>
       <c r="AU4" t="n">
-        <v>9.24</v>
+        <v>0.7428571428571432</v>
       </c>
       <c r="AV4" t="n">
-        <v>8.836</v>
+        <v>0.7143697478991597</v>
       </c>
       <c r="AW4" t="n">
         <v>2</v>
       </c>
       <c r="AX4" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="AY4" t="n">
         <v>3</v>
       </c>
       <c r="AZ4" t="n">
-        <v>5</v>
+        <v>3.666666666666667</v>
       </c>
       <c r="BA4" t="n">
         <v>2</v>
@@ -1191,76 +1191,76 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10.73539855959649</v>
+        <v>0.2834315700096095</v>
       </c>
       <c r="C5" t="n">
-        <v>19.72603312568742</v>
+        <v>0.5098630165628437</v>
       </c>
       <c r="D5" t="n">
-        <v>46.54727409482788</v>
+        <v>0.4134985730088584</v>
       </c>
       <c r="E5" t="n">
-        <v>4.683603757580885</v>
+        <v>0.2349622288059056</v>
       </c>
       <c r="F5" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G5" t="n">
-        <v>-4.577403224114418</v>
+        <v>0.8674002814894169</v>
       </c>
       <c r="H5" t="n">
-        <v>10.63734806137178</v>
+        <v>0.1265387310656802</v>
       </c>
       <c r="I5" t="n">
-        <v>8.730542659852533</v>
+        <v>0.09974170517994529</v>
       </c>
       <c r="J5" t="n">
-        <v>5.965168148784675</v>
+        <v>0.02739625053119859</v>
       </c>
       <c r="K5" t="n">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="L5" t="n">
-        <v>20</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="M5" t="n">
-        <v>-3.488142292490126</v>
+        <v>0.6351202205493853</v>
       </c>
       <c r="N5" t="n">
-        <v>-35.826828</v>
+        <v>0.9065269436419175</v>
       </c>
       <c r="O5" t="n">
-        <v>-3.5070446</v>
+        <v>0.9750716264593272</v>
       </c>
       <c r="P5" t="n">
-        <v>-7.036984</v>
+        <v>0.9651841491541497</v>
       </c>
       <c r="Q5" t="n">
-        <v>-18.084</v>
+        <v>0.9741884749002081</v>
       </c>
       <c r="R5" t="n">
-        <v>-130.9</v>
+        <v>0.7038941954445259</v>
       </c>
       <c r="S5" t="n">
-        <v>-69.34157182553139</v>
+        <v>0.41162033555875</v>
       </c>
       <c r="T5" t="n">
-        <v>9.062176945209908</v>
+        <v>0.7827407063169638</v>
       </c>
       <c r="U5" t="n">
-        <v>19.55795976235485</v>
+        <v>0.722868999856208</v>
       </c>
       <c r="V5" t="n">
-        <v>9.234561844679448</v>
+        <v>0.4394651701670539</v>
       </c>
       <c r="W5" t="n">
         <v>16</v>
       </c>
       <c r="X5" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Y5" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="Z5" t="n">
         <v>23</v>
@@ -1299,7 +1299,7 @@
         <v>12</v>
       </c>
       <c r="AL5" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AM5" t="n">
         <v>19</v>
@@ -1314,34 +1314,34 @@
         <v>5</v>
       </c>
       <c r="AQ5" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="AR5" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>0.2941176470588235</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>0.35</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>0.6091176470588234</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>20</v>
+      </c>
+      <c r="AY5" t="n">
         <v>6</v>
       </c>
-      <c r="AS5" t="n">
-        <v>10</v>
-      </c>
-      <c r="AT5" t="n">
-        <v>6</v>
-      </c>
-      <c r="AU5" t="n">
-        <v>7.039999999999999</v>
-      </c>
-      <c r="AV5" t="n">
-        <v>7.755999999999999</v>
-      </c>
-      <c r="AW5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX5" t="n">
-        <v>15</v>
-      </c>
-      <c r="AY5" t="n">
-        <v>5</v>
-      </c>
       <c r="AZ5" t="n">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="BA5" t="n">
         <v>7</v>
@@ -1354,67 +1354,67 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>21.98152809039133</v>
+        <v>0.4211403254680378</v>
       </c>
       <c r="C6" t="n">
-        <v>6.044403165851664</v>
+        <v>0.5030222015829258</v>
       </c>
       <c r="D6" t="n">
-        <v>20.56998564943704</v>
+        <v>0.1059514922990762</v>
       </c>
       <c r="E6" t="n">
-        <v>12.7480737548154</v>
+        <v>0.4044080792345729</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9292274122154387</v>
+        <v>0.5004646137061077</v>
       </c>
       <c r="G6" t="n">
-        <v>-1.868391096237982</v>
+        <v>0.9530669567571589</v>
       </c>
       <c r="H6" t="n">
-        <v>20.24912390270983</v>
+        <v>0.2616164929720607</v>
       </c>
       <c r="I6" t="n">
-        <v>16.07959473994657</v>
+        <v>0.2030205917768616</v>
       </c>
       <c r="J6" t="n">
-        <v>20.01240789638013</v>
+        <v>0.09584913851042939</v>
       </c>
       <c r="K6" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="L6" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="M6" t="n">
-        <v>-8.685366677931739</v>
+        <v>0.5253294730906513</v>
       </c>
       <c r="N6" t="n">
-        <v>-136.73456</v>
+        <v>0.6424594952765212</v>
       </c>
       <c r="O6" t="n">
-        <v>-15.88771</v>
+        <v>0.8747767539664674</v>
       </c>
       <c r="P6" t="n">
-        <v>-18.473791</v>
+        <v>0.9051464262448219</v>
       </c>
       <c r="Q6" t="n">
-        <v>-118.065</v>
+        <v>0.8251625041061528</v>
       </c>
       <c r="R6" t="n">
-        <v>-206.5</v>
+        <v>0.5187362233651727</v>
       </c>
       <c r="S6" t="n">
-        <v>-37.20220408485095</v>
+        <v>0.6983634092578479</v>
       </c>
       <c r="T6" t="n">
-        <v>6.384041943147374</v>
+        <v>0.6589882768737989</v>
       </c>
       <c r="U6" t="n">
-        <v>20.92987377279102</v>
+        <v>0.7511492748871105</v>
       </c>
       <c r="V6" t="n">
-        <v>8.419891177867408</v>
+        <v>0.4969180586672016</v>
       </c>
       <c r="W6" t="n">
         <v>4</v>
@@ -1435,7 +1435,7 @@
         <v>8</v>
       </c>
       <c r="AC6" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AD6" t="n">
         <v>13</v>
@@ -1471,13 +1471,13 @@
         <v>19</v>
       </c>
       <c r="AO6" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AP6" t="n">
         <v>4</v>
       </c>
       <c r="AQ6" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="AR6" t="n">
         <v>0</v>
@@ -1486,25 +1486,25 @@
         <v>0</v>
       </c>
       <c r="AT6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU6" t="n">
-        <v>8.4</v>
+        <v>0.5928571428571431</v>
       </c>
       <c r="AV6" t="n">
-        <v>1.41</v>
+        <v>0.08892857142857145</v>
       </c>
       <c r="AW6" t="n">
         <v>1</v>
       </c>
       <c r="AX6" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="AY6" t="n">
         <v>26</v>
       </c>
       <c r="AZ6" t="n">
-        <v>17.33333333333333</v>
+        <v>15.33333333333333</v>
       </c>
       <c r="BA6" t="n">
         <v>7</v>
@@ -1517,76 +1517,76 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>69.25470878444982</v>
+        <v>1</v>
       </c>
       <c r="C7" t="n">
-        <v>96.57422131180678</v>
+        <v>0.5482871106559034</v>
       </c>
       <c r="D7" t="n">
-        <v>68.21172161319939</v>
+        <v>0.6699856041118923</v>
       </c>
       <c r="E7" t="n">
-        <v>40.29691563315185</v>
+        <v>0.9832479710068011</v>
       </c>
       <c r="F7" t="n">
-        <v>95.59670802594465</v>
+        <v>0.5477983540129723</v>
       </c>
       <c r="G7" t="n">
-        <v>-1.294641168832806</v>
+        <v>0.9712105627639874</v>
       </c>
       <c r="H7" t="n">
-        <v>44.39851498864077</v>
+        <v>0.6009966193021126</v>
       </c>
       <c r="I7" t="n">
-        <v>38.81309913004932</v>
+        <v>0.5225027503283737</v>
       </c>
       <c r="J7" t="n">
-        <v>85.35672854818958</v>
+        <v>0.4141298953939992</v>
       </c>
       <c r="K7" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="L7" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="M7" t="n">
-        <v>1.622596153846156</v>
+        <v>0.7430839628232666</v>
       </c>
       <c r="N7" t="n">
-        <v>-42.99272</v>
+        <v>0.8878134281190538</v>
       </c>
       <c r="O7" t="n">
-        <v>-26.10174</v>
+        <v>0.7921107719388552</v>
       </c>
       <c r="P7" t="n">
-        <v>-43.06589</v>
+        <v>0.7761404879876588</v>
       </c>
       <c r="Q7" t="n">
-        <v>-43.647</v>
+        <v>0.9382932340556843</v>
       </c>
       <c r="R7" t="n">
-        <v>-210.2</v>
+        <v>0.5096742591231938</v>
       </c>
       <c r="S7" t="n">
-        <v>-92.64562915219895</v>
+        <v>0.2037047013301856</v>
       </c>
       <c r="T7" t="n">
-        <v>-7.87716955941255</v>
+        <v>0</v>
       </c>
       <c r="U7" t="n">
-        <v>8.793770581778265</v>
+        <v>0.5009788316709686</v>
       </c>
       <c r="V7" t="n">
-        <v>45.289502693801</v>
+        <v>0.7172734282580814</v>
       </c>
       <c r="W7" t="n">
         <v>1</v>
       </c>
       <c r="X7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z7" t="n">
         <v>2</v>
@@ -1643,19 +1643,19 @@
         <v>1</v>
       </c>
       <c r="AR7" t="n">
-        <v>1</v>
+        <v>0.0625</v>
       </c>
       <c r="AS7" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AT7" t="n">
-        <v>8</v>
+        <v>0.4117647058823529</v>
       </c>
       <c r="AU7" t="n">
-        <v>5.28</v>
+        <v>0.03571428571428576</v>
       </c>
       <c r="AV7" t="n">
-        <v>6.292</v>
+        <v>0.4858718487394958</v>
       </c>
       <c r="AW7" t="n">
         <v>1</v>
@@ -1664,10 +1664,10 @@
         <v>1</v>
       </c>
       <c r="AY7" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="AZ7" t="n">
-        <v>6.333333333333333</v>
+        <v>7</v>
       </c>
       <c r="BA7" t="n">
         <v>7</v>
@@ -1680,76 +1680,76 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>11.73330424169203</v>
+        <v>0.2956509161562085</v>
       </c>
       <c r="C8" t="n">
-        <v>20.71594348627375</v>
+        <v>0.5103579717431368</v>
       </c>
       <c r="D8" t="n">
-        <v>80.2565322169655</v>
+        <v>0.8125850269376321</v>
       </c>
       <c r="E8" t="n">
-        <v>28.92888438600457</v>
+        <v>0.7443896550811303</v>
       </c>
       <c r="F8" t="n">
-        <v>11.51379467515707</v>
+        <v>0.5057568973375786</v>
       </c>
       <c r="G8" t="n">
-        <v>-2.686202686202686</v>
+        <v>0.9272054262063081</v>
       </c>
       <c r="H8" t="n">
-        <v>29.77884271937135</v>
+        <v>0.3955410778355132</v>
       </c>
       <c r="I8" t="n">
-        <v>29.77884271937135</v>
+        <v>0.3955410778355132</v>
       </c>
       <c r="J8" t="n">
-        <v>14.47797340017563</v>
+        <v>0.06917132465993209</v>
       </c>
       <c r="K8" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="L8" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="M8" t="n">
-        <v>9.982238010657197</v>
+        <v>0.9196804035152566</v>
       </c>
       <c r="N8" t="n">
-        <v>-29.935375</v>
+        <v>0.9215579366909874</v>
       </c>
       <c r="O8" t="n">
-        <v>-10.642643</v>
+        <v>0.9168614577123432</v>
       </c>
       <c r="P8" t="n">
-        <v>-9.768418</v>
+        <v>0.9505942384385307</v>
       </c>
       <c r="Q8" t="n">
-        <v>-20.154</v>
+        <v>0.9709874533036222</v>
       </c>
       <c r="R8" t="n">
-        <v>-124.2</v>
+        <v>0.7203036982610824</v>
       </c>
       <c r="S8" t="n">
-        <v>-36.88491163783526</v>
+        <v>0.7011942493743331</v>
       </c>
       <c r="T8" t="n">
-        <v>10.49359907844118</v>
+        <v>0.848884484136104</v>
       </c>
       <c r="U8" t="n">
-        <v>14.64528543938422</v>
+        <v>0.6216004218447548</v>
       </c>
       <c r="V8" t="n">
-        <v>19.90705863728995</v>
+        <v>0.602203408587734</v>
       </c>
       <c r="W8" t="n">
         <v>13</v>
       </c>
       <c r="X8" t="n">
+        <v>8</v>
+      </c>
+      <c r="Y8" t="n">
         <v>7</v>
-      </c>
-      <c r="Y8" t="n">
-        <v>6</v>
       </c>
       <c r="Z8" t="n">
         <v>6</v>
@@ -1806,19 +1806,19 @@
         <v>4</v>
       </c>
       <c r="AR8" t="n">
-        <v>1</v>
+        <v>0.0625</v>
       </c>
       <c r="AS8" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AT8" t="n">
-        <v>10</v>
+        <v>0.5294117647058824</v>
       </c>
       <c r="AU8" t="n">
-        <v>9.16</v>
+        <v>0.7285714285714289</v>
       </c>
       <c r="AV8" t="n">
-        <v>7.174</v>
+        <v>0.6074474789915967</v>
       </c>
       <c r="AW8" t="n">
         <v>1</v>
@@ -1843,73 +1843,73 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>14.9429496088632</v>
+        <v>0.3349529949528069</v>
       </c>
       <c r="C9" t="n">
-        <v>10.26188971063529</v>
+        <v>0.5051309448553176</v>
       </c>
       <c r="D9" t="n">
-        <v>51.0353867030574</v>
+        <v>0.4666336772927184</v>
       </c>
       <c r="E9" t="n">
-        <v>27.26580294015222</v>
+        <v>0.7094459762006551</v>
       </c>
       <c r="F9" t="n">
-        <v>-2.84781681744809</v>
+        <v>0.498576091591276</v>
       </c>
       <c r="G9" t="n">
-        <v>-2.537019397298233</v>
+        <v>0.9319230264837087</v>
       </c>
       <c r="H9" t="n">
-        <v>15.32930368951794</v>
+        <v>0.1924764803095078</v>
       </c>
       <c r="I9" t="n">
-        <v>9.897513390586193</v>
+        <v>0.1161415668829011</v>
       </c>
       <c r="J9" t="n">
-        <v>9.313204647585749</v>
+        <v>0.04447160388952821</v>
       </c>
       <c r="K9" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="L9" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="M9" t="n">
-        <v>4.026354319180092</v>
+        <v>0.7938630683822473</v>
       </c>
       <c r="N9" t="n">
-        <v>-35.505615</v>
+        <v>0.9074186800851527</v>
       </c>
       <c r="O9" t="n">
-        <v>-11.589415</v>
+        <v>0.9076270133089607</v>
       </c>
       <c r="P9" t="n">
-        <v>-20.845243</v>
+        <v>0.8927633936894899</v>
       </c>
       <c r="Q9" t="n">
-        <v>-30.576</v>
+        <v>0.9571225219101468</v>
       </c>
       <c r="R9" t="n">
-        <v>-124.9</v>
+        <v>0.718589272593681</v>
       </c>
       <c r="S9" t="n">
-        <v>-14.10708087100158</v>
+        <v>0.9044149617100229</v>
       </c>
       <c r="T9" t="n">
-        <v>7.397879381596062</v>
+        <v>0.7058361191117127</v>
       </c>
       <c r="U9" t="n">
-        <v>14.74747741560568</v>
+        <v>0.6237069803983596</v>
       </c>
       <c r="V9" t="n">
-        <v>13.24433837017594</v>
+        <v>0.5409231120292544</v>
       </c>
       <c r="W9" t="n">
         <v>8</v>
       </c>
       <c r="X9" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Y9" t="n">
         <v>14</v>
@@ -1966,34 +1966,34 @@
         <v>10</v>
       </c>
       <c r="AQ9" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AR9" t="n">
-        <v>1</v>
+        <v>0.0625</v>
       </c>
       <c r="AS9" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AT9" t="n">
-        <v>7</v>
+        <v>0.3529411764705883</v>
       </c>
       <c r="AU9" t="n">
-        <v>10.68</v>
+        <v>1</v>
       </c>
       <c r="AV9" t="n">
-        <v>6.951999999999999</v>
+        <v>0.6216911764705882</v>
       </c>
       <c r="AW9" t="n">
         <v>2</v>
       </c>
       <c r="AX9" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AY9" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AZ9" t="n">
-        <v>7.333333333333333</v>
+        <v>6</v>
       </c>
       <c r="BA9" t="n">
         <v>2</v>
@@ -2006,73 +2006,73 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>16.20048775845504</v>
+        <v>0.3503515383403423</v>
       </c>
       <c r="C10" t="n">
-        <v>-27.1280671598897</v>
+        <v>0.4864359664200552</v>
       </c>
       <c r="D10" t="n">
-        <v>46.79879647539343</v>
+        <v>0.4164763654770263</v>
       </c>
       <c r="E10" t="n">
-        <v>5.240860219753799</v>
+        <v>0.2466709703812528</v>
       </c>
       <c r="F10" t="n">
-        <v>-9.269548997557875</v>
+        <v>0.495365225501221</v>
       </c>
       <c r="G10" t="n">
-        <v>-0.3842412451361868</v>
+        <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>26.1626150254086</v>
+        <v>0.344720922277624</v>
       </c>
       <c r="I10" t="n">
-        <v>18.28732316989424</v>
+        <v>0.2340465978070756</v>
       </c>
       <c r="J10" t="n">
-        <v>14.2470358351127</v>
+        <v>0.06736471109930955</v>
       </c>
       <c r="K10" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="L10" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="M10" t="n">
-        <v>-33.55317394888706</v>
+        <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>-31.74804</v>
+        <v>0.9176842936124422</v>
       </c>
       <c r="O10" t="n">
-        <v>-8.876296999999999</v>
+        <v>0.9319908288785386</v>
       </c>
       <c r="P10" t="n">
-        <v>-4.401658</v>
+        <v>0.9791519174402843</v>
       </c>
       <c r="Q10" t="n">
-        <v>-47.03</v>
+        <v>0.9329776326660628</v>
       </c>
       <c r="R10" t="n">
-        <v>-191.6</v>
+        <v>0.5552289982855743</v>
       </c>
       <c r="S10" t="n">
-        <v>-64.31920397517369</v>
+        <v>0.4564292193637743</v>
       </c>
       <c r="T10" t="n">
-        <v>2.022361540461676</v>
+        <v>0.4574418477836672</v>
       </c>
       <c r="U10" t="n">
-        <v>18.53138330286411</v>
+        <v>0.7017074223857528</v>
       </c>
       <c r="V10" t="n">
-        <v>4.661921586891281</v>
+        <v>0.4758176382354872</v>
       </c>
       <c r="W10" t="n">
         <v>6</v>
       </c>
       <c r="X10" t="n">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="Y10" t="n">
         <v>16</v>
@@ -2129,34 +2129,34 @@
         <v>6</v>
       </c>
       <c r="AQ10" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="AR10" t="n">
         <v>0</v>
       </c>
       <c r="AS10" t="n">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="AT10" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="AU10" t="n">
-        <v>7.880000000000001</v>
+        <v>0.5000000000000003</v>
       </c>
       <c r="AV10" t="n">
-        <v>5.882</v>
+        <v>0.425</v>
       </c>
       <c r="AW10" t="n">
         <v>2</v>
       </c>
       <c r="AX10" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="AY10" t="n">
         <v>14</v>
       </c>
       <c r="AZ10" t="n">
-        <v>12.66666666666667</v>
+        <v>10.66666666666667</v>
       </c>
       <c r="BA10" t="n">
         <v>2</v>
@@ -2169,76 +2169,76 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>14.02264177950645</v>
+        <v>0.3236838338185399</v>
       </c>
       <c r="C11" t="n">
-        <v>11.91454411631245</v>
+        <v>0.5059572720581562</v>
       </c>
       <c r="D11" t="n">
-        <v>96.08673552434298</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>16.26328032008724</v>
+        <v>0.478267510305577</v>
       </c>
       <c r="F11" t="n">
-        <v>-25.55775916127318</v>
+        <v>0.4872211204193634</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.5205439391723936</v>
+        <v>0.9956897207997103</v>
       </c>
       <c r="H11" t="n">
-        <v>51.99138858988159</v>
+        <v>0.7077020179114577</v>
       </c>
       <c r="I11" t="n">
-        <v>51.99138858988159</v>
+        <v>0.7077020179114577</v>
       </c>
       <c r="J11" t="n">
-        <v>45.94760462249834</v>
+        <v>0.2209068918986902</v>
       </c>
       <c r="K11" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="L11" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="M11" t="n">
-        <v>-2.333709923984806</v>
+        <v>0.6595074671311945</v>
       </c>
       <c r="N11" t="n">
-        <v>-70.519424</v>
+        <v>0.8168732644529859</v>
       </c>
       <c r="O11" t="n">
-        <v>-37.34028</v>
+        <v>0.7028571306857105</v>
       </c>
       <c r="P11" t="n">
-        <v>-21.954058</v>
+        <v>0.887587297793518</v>
       </c>
       <c r="Q11" t="n">
-        <v>-155.87</v>
+        <v>0.7729009560403463</v>
       </c>
       <c r="R11" t="n">
-        <v>-418.3</v>
+        <v>0</v>
       </c>
       <c r="S11" t="n">
-        <v>-30.41114133027265</v>
+        <v>0.758952348767895</v>
       </c>
       <c r="T11" t="n">
-        <v>-4.42230183609494</v>
+        <v>0.1596440335666644</v>
       </c>
       <c r="U11" t="n">
-        <v>5.012626262626263</v>
+        <v>0.4230353159231006</v>
       </c>
       <c r="V11" t="n">
-        <v>17.05137071206019</v>
+        <v>0.6142198864280667</v>
       </c>
       <c r="W11" t="n">
         <v>9</v>
       </c>
       <c r="X11" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="Y11" t="n">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="Z11" t="n">
         <v>16</v>
@@ -2292,34 +2292,34 @@
         <v>22</v>
       </c>
       <c r="AQ11" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AR11" t="n">
-        <v>1</v>
+        <v>0.0625</v>
       </c>
       <c r="AS11" t="n">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="AT11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU11" t="n">
-        <v>8.279999999999999</v>
+        <v>0.5714285714285715</v>
       </c>
       <c r="AV11" t="n">
-        <v>3.691999999999999</v>
+        <v>0.3044642857142857</v>
       </c>
       <c r="AW11" t="n">
         <v>-1</v>
       </c>
       <c r="AX11" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AY11" t="n">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="AZ11" t="n">
-        <v>15.16666666666667</v>
+        <v>12.16666666666667</v>
       </c>
       <c r="BA11" t="n">
         <v>15.5</v>
@@ -2332,67 +2332,67 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>11.66715316369267</v>
+        <v>0.294840896798119</v>
       </c>
       <c r="C12" t="n">
-        <v>8.743270751737576</v>
+        <v>0.5043716353758688</v>
       </c>
       <c r="D12" t="n">
-        <v>31.99493560177435</v>
+        <v>0.2412123380368131</v>
       </c>
       <c r="E12" t="n">
-        <v>31.99493560177435</v>
+        <v>0.8088117009058552</v>
       </c>
       <c r="F12" t="n">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>-13.17767825547195</v>
+        <v>0.5954351024696715</v>
       </c>
       <c r="H12" t="n">
-        <v>72.79053896859247</v>
+        <v>1</v>
       </c>
       <c r="I12" t="n">
-        <v>72.79053896859247</v>
+        <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>0.3705569817803875</v>
+        <v>0.0006882295048204959</v>
       </c>
       <c r="K12" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="L12" t="n">
-        <v>30</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="M12" t="n">
-        <v>4.884990898560315</v>
+        <v>0.8120016640737541</v>
       </c>
       <c r="N12" t="n">
-        <v>-18.703888</v>
+        <v>0.9512560223083806</v>
       </c>
       <c r="O12" t="n">
-        <v>-5.257813</v>
+        <v>0.9608223419004499</v>
       </c>
       <c r="P12" t="n">
-        <v>-2.5556931</v>
+        <v>0.9886857288235849</v>
       </c>
       <c r="Q12" t="n">
-        <v>-3.102</v>
+        <v>0.9954210175295394</v>
       </c>
       <c r="R12" t="n">
-        <v>-112.9</v>
+        <v>0.7479794268919912</v>
       </c>
       <c r="S12" t="n">
-        <v>-17.22958222926846</v>
+        <v>0.8765564287008077</v>
       </c>
       <c r="T12" t="n">
-        <v>-2.510308997620174</v>
+        <v>0.2479942319909259</v>
       </c>
       <c r="U12" t="n">
-        <v>-7.185100306134665</v>
+        <v>0.17159458458555</v>
       </c>
       <c r="V12" t="n">
-        <v>16.71516538989576</v>
+        <v>0.5446194726090305</v>
       </c>
       <c r="W12" t="n">
         <v>14</v>
@@ -2401,7 +2401,7 @@
         <v>15</v>
       </c>
       <c r="Y12" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="Z12" t="n">
         <v>4</v>
@@ -2455,31 +2455,31 @@
         <v>24</v>
       </c>
       <c r="AQ12" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AR12" t="n">
         <v>0</v>
       </c>
       <c r="AS12" t="n">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="AT12" t="n">
-        <v>7</v>
+        <v>0.3529411764705883</v>
       </c>
       <c r="AU12" t="n">
-        <v>6.879999999999999</v>
+        <v>0.3214285714285713</v>
       </c>
       <c r="AV12" t="n">
-        <v>4.082</v>
+        <v>0.3011554621848739</v>
       </c>
       <c r="AW12" t="n">
         <v>-2</v>
       </c>
       <c r="AX12" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AY12" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="AZ12" t="n">
         <v>16.16666666666667</v>
@@ -2495,76 +2495,76 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-3.386684400278661</v>
+        <v>0.1105067905501615</v>
       </c>
       <c r="C13" t="n">
-        <v>-11.99191965883707</v>
+        <v>0.4940040401705815</v>
       </c>
       <c r="D13" t="n">
-        <v>22.95481606960552</v>
+        <v>0.1341856798376465</v>
       </c>
       <c r="E13" t="n">
-        <v>22.95481606960552</v>
+        <v>0.6188660823307414</v>
       </c>
       <c r="F13" t="n">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>-28.07919931801043</v>
+        <v>0.1242065860951116</v>
       </c>
       <c r="H13" t="n">
-        <v>20.09313206214689</v>
+        <v>0.2594242832236522</v>
       </c>
       <c r="I13" t="n">
-        <v>20.09313206214689</v>
+        <v>0.2594242832236522</v>
       </c>
       <c r="J13" t="n">
-        <v>0.2907138303612626</v>
+        <v>1.28520998289116e-05</v>
       </c>
       <c r="K13" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="L13" t="n">
-        <v>20</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="M13" t="n">
-        <v>5.337563823861091</v>
+        <v>0.8215622133329979</v>
       </c>
       <c r="N13" t="n">
-        <v>-19.151106</v>
+        <v>0.9503545355619496</v>
       </c>
       <c r="O13" t="n">
-        <v>-4.397229</v>
+        <v>0.9679968082021196</v>
       </c>
       <c r="P13" t="n">
-        <v>-2.3133376</v>
+        <v>0.9900254640860363</v>
       </c>
       <c r="Q13" t="n">
-        <v>-0.36</v>
+        <v>0.9994496688769975</v>
       </c>
       <c r="R13" t="n">
-        <v>-140.2</v>
+        <v>0.6811168258633357</v>
       </c>
       <c r="S13" t="n">
-        <v>-36.1665165785675</v>
+        <v>0.7076036725181475</v>
       </c>
       <c r="T13" t="n">
-        <v>-1.640122866014468</v>
+        <v>0.2882041720316711</v>
       </c>
       <c r="U13" t="n">
-        <v>-9.254693191370132</v>
+        <v>0.1289325404988002</v>
       </c>
       <c r="V13" t="n">
-        <v>1.921076849380055</v>
+        <v>0.3498445995934407</v>
       </c>
       <c r="W13" t="n">
         <v>24</v>
       </c>
       <c r="X13" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="Y13" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="Z13" t="n">
         <v>11</v>
@@ -2576,10 +2576,10 @@
         <v>25</v>
       </c>
       <c r="AC13" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AD13" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AE13" t="n">
         <v>25</v>
@@ -2621,19 +2621,19 @@
         <v>25</v>
       </c>
       <c r="AR13" t="n">
-        <v>1</v>
+        <v>0.0625</v>
       </c>
       <c r="AS13" t="n">
         <v>0</v>
       </c>
       <c r="AT13" t="n">
-        <v>17</v>
+        <v>0.9411764705882353</v>
       </c>
       <c r="AU13" t="n">
-        <v>8.119999999999999</v>
+        <v>0.5428571428571429</v>
       </c>
       <c r="AV13" t="n">
-        <v>4.068</v>
+        <v>0.2413550420168067</v>
       </c>
       <c r="AW13" t="n">
         <v>-2</v>
@@ -2642,10 +2642,10 @@
         <v>25</v>
       </c>
       <c r="AY13" t="n">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="AZ13" t="n">
-        <v>22.5</v>
+        <v>23.5</v>
       </c>
       <c r="BA13" t="n">
         <v>21.5</v>
@@ -2658,76 +2658,76 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>13.95336514824015</v>
+        <v>0.3228355420886687</v>
       </c>
       <c r="C14" t="n">
-        <v>23.25859899737732</v>
+        <v>0.5116292994986886</v>
       </c>
       <c r="D14" t="n">
-        <v>78.80445363214076</v>
+        <v>0.7953937588550206</v>
       </c>
       <c r="E14" t="n">
-        <v>18.44433120665891</v>
+        <v>0.5240944552170304</v>
       </c>
       <c r="F14" t="n">
-        <v>18.45286708043346</v>
+        <v>0.5092264335402168</v>
       </c>
       <c r="G14" t="n">
-        <v>-3.36834094368341</v>
+        <v>0.9056342726518527</v>
       </c>
       <c r="H14" t="n">
-        <v>13.60366441658631</v>
+        <v>0.168225447545836</v>
       </c>
       <c r="I14" t="n">
-        <v>13.60366441658631</v>
+        <v>0.168225447545836</v>
       </c>
       <c r="J14" t="n">
-        <v>8.544378348743662</v>
+        <v>0.04009860023623095</v>
       </c>
       <c r="K14" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="L14" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="M14" t="n">
-        <v>-0</v>
+        <v>0.7088068119168219</v>
       </c>
       <c r="N14" t="n">
-        <v>-31.144402</v>
+        <v>0.9184448643899391</v>
       </c>
       <c r="O14" t="n">
-        <v>-10.250537</v>
+        <v>0.9201053320014679</v>
       </c>
       <c r="P14" t="n">
-        <v>-9.80471</v>
+        <v>0.9504446116931717</v>
       </c>
       <c r="Q14" t="n">
-        <v>-100</v>
+        <v>0.8576434167172677</v>
       </c>
       <c r="R14" t="n">
-        <v>-126</v>
+        <v>0.715895175116336</v>
       </c>
       <c r="S14" t="n">
-        <v>-24.35856634276198</v>
+        <v>0.8129526007242001</v>
       </c>
       <c r="T14" t="n">
-        <v>6.326099897180583</v>
+        <v>0.6563108655596659</v>
       </c>
       <c r="U14" t="n">
-        <v>16.04290514344792</v>
+        <v>0.6504105872916137</v>
       </c>
       <c r="V14" t="n">
-        <v>16.3239528247262</v>
+        <v>0.5441011829414165</v>
       </c>
       <c r="W14" t="n">
         <v>10</v>
       </c>
       <c r="X14" t="n">
+        <v>7</v>
+      </c>
+      <c r="Y14" t="n">
         <v>6</v>
-      </c>
-      <c r="Y14" t="n">
-        <v>5</v>
       </c>
       <c r="Z14" t="n">
         <v>15</v>
@@ -2775,40 +2775,40 @@
         <v>10</v>
       </c>
       <c r="AO14" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AP14" t="n">
         <v>7</v>
       </c>
       <c r="AQ14" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AR14" t="n">
-        <v>5</v>
+        <v>0.3125</v>
       </c>
       <c r="AS14" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AT14" t="n">
-        <v>9</v>
+        <v>0.4705882352941176</v>
       </c>
       <c r="AU14" t="n">
-        <v>9.800000000000001</v>
+        <v>0.8428571428571433</v>
       </c>
       <c r="AV14" t="n">
-        <v>8.32</v>
+        <v>0.6907668067226891</v>
       </c>
       <c r="AW14" t="n">
         <v>0</v>
       </c>
       <c r="AX14" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AY14" t="n">
         <v>4</v>
       </c>
       <c r="AZ14" t="n">
-        <v>8.166666666666666</v>
+        <v>8.5</v>
       </c>
       <c r="BA14" t="n">
         <v>12.5</v>
@@ -2821,76 +2821,76 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>22.16629605141325</v>
+        <v>0.4234028074971881</v>
       </c>
       <c r="C15" t="n">
-        <v>25.28545511629232</v>
+        <v>0.5126427275581461</v>
       </c>
       <c r="D15" t="n">
-        <v>56.68036836397422</v>
+        <v>0.5334650417026271</v>
       </c>
       <c r="E15" t="n">
-        <v>41.09419827457792</v>
+        <v>1</v>
       </c>
       <c r="F15" t="n">
-        <v>48.5481232847671</v>
+        <v>0.5242740616423835</v>
       </c>
       <c r="G15" t="n">
-        <v>-2.466956540075888</v>
+        <v>0.9341386134780356</v>
       </c>
       <c r="H15" t="n">
-        <v>23.59942059635386</v>
+        <v>0.3086994240110334</v>
       </c>
       <c r="I15" t="n">
-        <v>21.39969185176944</v>
+        <v>0.2777858404522399</v>
       </c>
       <c r="J15" t="n">
-        <v>4.182676905433154</v>
+        <v>0.01876346839951029</v>
       </c>
       <c r="K15" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="L15" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="M15" t="n">
-        <v>0.01089070040624085</v>
+        <v>0.7090368766685574</v>
       </c>
       <c r="N15" t="n">
-        <v>-30.338762</v>
+        <v>0.9195298945720963</v>
       </c>
       <c r="O15" t="n">
-        <v>-2.2724824</v>
+        <v>0.9849706967185791</v>
       </c>
       <c r="P15" t="n">
-        <v>-1.0544966</v>
+        <v>0.9965563787170277</v>
       </c>
       <c r="Q15" t="n">
-        <v>-1.386</v>
+        <v>0.9978697777202641</v>
       </c>
       <c r="R15" t="n">
-        <v>-119.9</v>
+        <v>0.7308351702179769</v>
       </c>
       <c r="S15" t="n">
-        <v>-23.6604978211487</v>
+        <v>0.8191806732598841</v>
       </c>
       <c r="T15" t="n">
-        <v>9.979384062921399</v>
+        <v>0.8251234125778297</v>
       </c>
       <c r="U15" t="n">
-        <v>15.7649198423799</v>
+        <v>0.6446802713177632</v>
       </c>
       <c r="V15" t="n">
-        <v>21.2269055030331</v>
+        <v>0.594135690571257</v>
       </c>
       <c r="W15" t="n">
         <v>3</v>
       </c>
       <c r="X15" t="n">
+        <v>5</v>
+      </c>
+      <c r="Y15" t="n">
         <v>4</v>
-      </c>
-      <c r="Y15" t="n">
-        <v>3</v>
       </c>
       <c r="Z15" t="n">
         <v>1</v>
@@ -2902,10 +2902,10 @@
         <v>10</v>
       </c>
       <c r="AC15" t="n">
+        <v>11</v>
+      </c>
+      <c r="AD15" t="n">
         <v>10</v>
-      </c>
-      <c r="AD15" t="n">
-        <v>9</v>
       </c>
       <c r="AE15" t="n">
         <v>16</v>
@@ -2944,34 +2944,34 @@
         <v>8</v>
       </c>
       <c r="AQ15" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AR15" t="n">
-        <v>1</v>
+        <v>0.0625</v>
       </c>
       <c r="AS15" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AT15" t="n">
-        <v>9</v>
+        <v>0.4705882352941176</v>
       </c>
       <c r="AU15" t="n">
-        <v>7.359999999999999</v>
+        <v>0.4071428571428572</v>
       </c>
       <c r="AV15" t="n">
-        <v>6.754</v>
+        <v>0.5504096638655462</v>
       </c>
       <c r="AW15" t="n">
         <v>1</v>
       </c>
       <c r="AX15" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AY15" t="n">
         <v>9</v>
       </c>
       <c r="AZ15" t="n">
-        <v>6.333333333333333</v>
+        <v>7</v>
       </c>
       <c r="BA15" t="n">
         <v>7</v>
@@ -2984,76 +2984,76 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>16.05940226852471</v>
+        <v>0.3486239477787765</v>
       </c>
       <c r="C16" t="n">
-        <v>23.4687255950446</v>
+        <v>0.5117343627975223</v>
       </c>
       <c r="D16" t="n">
-        <v>49.32098803723084</v>
+        <v>0.446336781950616</v>
       </c>
       <c r="E16" t="n">
-        <v>20.68978568312832</v>
+        <v>0.5712746100808583</v>
       </c>
       <c r="F16" t="n">
-        <v>19.77630767602709</v>
+        <v>0.5098881538380136</v>
       </c>
       <c r="G16" t="n">
-        <v>-9.484830837822649</v>
+        <v>0.7122134502982835</v>
       </c>
       <c r="H16" t="n">
-        <v>33.6678023621572</v>
+        <v>0.4501940341011496</v>
       </c>
       <c r="I16" t="n">
-        <v>26.36943414195747</v>
+        <v>0.3476274261166677</v>
       </c>
       <c r="J16" t="n">
-        <v>10.92217941192822</v>
+        <v>0.05246930830778347</v>
       </c>
       <c r="K16" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="L16" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="M16" t="n">
-        <v>2.549797772789864</v>
+        <v>0.7626709868266816</v>
       </c>
       <c r="N16" t="n">
-        <v>-50.22718</v>
+        <v>0.8682386314501559</v>
       </c>
       <c r="O16" t="n">
-        <v>-12.242119</v>
+        <v>0.9021391654960228</v>
       </c>
       <c r="P16" t="n">
-        <v>-24.086199</v>
+        <v>0.8751078106354089</v>
       </c>
       <c r="Q16" t="n">
-        <v>-37.983</v>
+        <v>0.9464770986884486</v>
       </c>
       <c r="R16" t="n">
-        <v>-69.89999999999999</v>
+        <v>0.8532941464609356</v>
       </c>
       <c r="S16" t="n">
-        <v>-24.9593083635035</v>
+        <v>0.8075928620100625</v>
       </c>
       <c r="T16" t="n">
-        <v>4.262112007122982</v>
+        <v>0.5609372135446673</v>
       </c>
       <c r="U16" t="n">
-        <v>12.65973531369487</v>
+        <v>0.5806708131265779</v>
       </c>
       <c r="V16" t="n">
-        <v>17.3577666158993</v>
+        <v>0.5413974289029981</v>
       </c>
       <c r="W16" t="n">
         <v>7</v>
       </c>
       <c r="X16" t="n">
+        <v>6</v>
+      </c>
+      <c r="Y16" t="n">
         <v>5</v>
-      </c>
-      <c r="Y16" t="n">
-        <v>4</v>
       </c>
       <c r="Z16" t="n">
         <v>13</v>
@@ -3086,7 +3086,7 @@
         <v>23</v>
       </c>
       <c r="AJ16" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AK16" t="n">
         <v>21</v>
@@ -3107,34 +3107,34 @@
         <v>15</v>
       </c>
       <c r="AQ16" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="AR16" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="AS16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AT16" t="n">
+        <v>0.1764705882352941</v>
+      </c>
+      <c r="AU16" t="n">
+        <v>0.7214285714285715</v>
+      </c>
+      <c r="AV16" t="n">
+        <v>0.8346848739495798</v>
+      </c>
+      <c r="AW16" t="n">
+        <v>1</v>
+      </c>
+      <c r="AX16" t="n">
         <v>10</v>
       </c>
-      <c r="AT16" t="n">
-        <v>4</v>
-      </c>
-      <c r="AU16" t="n">
-        <v>9.119999999999999</v>
-      </c>
-      <c r="AV16" t="n">
-        <v>10.768</v>
-      </c>
-      <c r="AW16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX16" t="n">
-        <v>5</v>
-      </c>
       <c r="AY16" t="n">
         <v>1</v>
       </c>
       <c r="AZ16" t="n">
-        <v>4.333333333333333</v>
+        <v>6</v>
       </c>
       <c r="BA16" t="n">
         <v>7</v>
@@ -3147,76 +3147,76 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>22.94648620989339</v>
+        <v>0.4329562290055406</v>
       </c>
       <c r="C17" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="D17" t="n">
-        <v>79.81214357042474</v>
+        <v>0.807323876173899</v>
       </c>
       <c r="E17" t="n">
-        <v>1.983874305637229</v>
+        <v>0.1782371181577432</v>
       </c>
       <c r="F17" t="n">
-        <v>52.58851909733733</v>
+        <v>0.5262942595486686</v>
       </c>
       <c r="G17" t="n">
-        <v>-0.4781248282375045</v>
+        <v>0.9970311338425727</v>
       </c>
       <c r="H17" t="n">
-        <v>59.58013810995384</v>
+        <v>0.8143494593167058</v>
       </c>
       <c r="I17" t="n">
-        <v>59.58013810995384</v>
+        <v>0.8143494593167058</v>
       </c>
       <c r="J17" t="n">
-        <v>203.9996630653805</v>
+        <v>1</v>
       </c>
       <c r="K17" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="L17" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="M17" t="n">
-        <v>-16.975624565597</v>
+        <v>0.3501987605006666</v>
       </c>
       <c r="N17" t="n">
-        <v>-379.34042</v>
+        <v>0</v>
       </c>
       <c r="O17" t="n">
-        <v>-122.933945</v>
+        <v>0</v>
       </c>
       <c r="P17" t="n">
-        <v>-71.315994</v>
+        <v>0.624896046892191</v>
       </c>
       <c r="Q17" t="n">
-        <v>-714.972</v>
+        <v>0</v>
       </c>
       <c r="R17" t="n">
-        <v>-259.2</v>
+        <v>0.3896644624050942</v>
       </c>
       <c r="S17" t="n">
-        <v>-103.4381263528082</v>
+        <v>0.1074155071817111</v>
       </c>
       <c r="T17" t="n">
-        <v>10.9081793642653</v>
+        <v>0.8680415906787035</v>
       </c>
       <c r="U17" t="n">
-        <v>24.96516584088794</v>
+        <v>0.8343317255711132</v>
       </c>
       <c r="V17" t="n">
-        <v>23.11117995228029</v>
+        <v>0.661047248771656</v>
       </c>
       <c r="W17" t="n">
         <v>2</v>
       </c>
       <c r="X17" t="n">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="Y17" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Z17" t="n">
         <v>24</v>
@@ -3273,19 +3273,19 @@
         <v>2</v>
       </c>
       <c r="AR17" t="n">
-        <v>1</v>
+        <v>0.0625</v>
       </c>
       <c r="AS17" t="n">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="AT17" t="n">
-        <v>5</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="AU17" t="n">
-        <v>5.08</v>
+        <v>0</v>
       </c>
       <c r="AV17" t="n">
-        <v>3.812</v>
+        <v>0.2540441176470588</v>
       </c>
       <c r="AW17" t="n">
         <v>0</v>
@@ -3310,76 +3310,76 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>16.73073889020138</v>
+        <v>0.3568444587031447</v>
       </c>
       <c r="C18" t="n">
-        <v>26.32491340254508</v>
+        <v>0.5131624567012725</v>
       </c>
       <c r="D18" t="n">
-        <v>79.10914688108713</v>
+        <v>0.7990010452514599</v>
       </c>
       <c r="E18" t="n">
-        <v>20.24923606082558</v>
+        <v>0.5620180432596393</v>
       </c>
       <c r="F18" t="n">
-        <v>-57.4751735329748</v>
+        <v>0.4712624132335126</v>
       </c>
       <c r="G18" t="n">
-        <v>-23.70628730068136</v>
+        <v>0.2624905125154006</v>
       </c>
       <c r="H18" t="n">
-        <v>11.53756968770043</v>
+        <v>0.1391898711371353</v>
       </c>
       <c r="I18" t="n">
-        <v>8.863112564577856</v>
+        <v>0.1016047579937056</v>
       </c>
       <c r="J18" t="n">
-        <v>7.610184785468961</v>
+        <v>0.03555299818989589</v>
       </c>
       <c r="K18" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="L18" t="n">
-        <v>30</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="M18" t="n">
-        <v>5.884215747237198</v>
+        <v>0.8331101702454101</v>
       </c>
       <c r="N18" t="n">
-        <v>-32.602825</v>
+        <v>0.9145602064012045</v>
       </c>
       <c r="O18" t="n">
-        <v>-12.435372</v>
+        <v>0.9022723472722985</v>
       </c>
       <c r="P18" t="n">
-        <v>-36.259144</v>
+        <v>0.8108944863018862</v>
       </c>
       <c r="Q18" t="n">
-        <v>-28.541</v>
+        <v>0.9595257766850158</v>
       </c>
       <c r="R18" t="n">
-        <v>-46.5</v>
+        <v>0.9106049473426402</v>
       </c>
       <c r="S18" t="n">
-        <v>-33.17948947479677</v>
+        <v>0.7342535226293433</v>
       </c>
       <c r="T18" t="n">
-        <v>-2.251289146019368</v>
+        <v>0.2599631341877612</v>
       </c>
       <c r="U18" t="n">
-        <v>8.326628895184136</v>
+        <v>0.4913492956542896</v>
       </c>
       <c r="V18" t="n">
-        <v>11.94022055861703</v>
+        <v>0.4738373711411129</v>
       </c>
       <c r="W18" t="n">
         <v>5</v>
       </c>
       <c r="X18" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Y18" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="Z18" t="n">
         <v>14</v>
@@ -3412,7 +3412,7 @@
         <v>17</v>
       </c>
       <c r="AJ18" t="n">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="AK18" t="n">
         <v>22</v>
@@ -3433,34 +3433,34 @@
         <v>21</v>
       </c>
       <c r="AQ18" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="AR18" t="n">
-        <v>1</v>
+        <v>0.0625</v>
       </c>
       <c r="AS18" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AT18" t="n">
-        <v>6</v>
+        <v>0.2941176470588235</v>
       </c>
       <c r="AU18" t="n">
-        <v>6.719999999999999</v>
+        <v>0.2928571428571428</v>
       </c>
       <c r="AV18" t="n">
-        <v>6.207999999999999</v>
+        <v>0.506796218487395</v>
       </c>
       <c r="AW18" t="n">
         <v>1</v>
       </c>
       <c r="AX18" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="AY18" t="n">
         <v>12</v>
       </c>
       <c r="AZ18" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="BA18" t="n">
         <v>7</v>
@@ -3473,76 +3473,76 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>13.31283352357027</v>
+        <v>0.3149922380769621</v>
       </c>
       <c r="C19" t="n">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>87.07532708005394</v>
+        <v>0.8933132545396089</v>
       </c>
       <c r="E19" t="n">
-        <v>23.00434684167584</v>
+        <v>0.6199067934746507</v>
       </c>
       <c r="F19" t="n">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>-1.066144208268331</v>
+        <v>0.9784362871226625</v>
       </c>
       <c r="H19" t="n">
-        <v>26.92139370476351</v>
+        <v>0.3553843134637498</v>
       </c>
       <c r="I19" t="n">
-        <v>23.53980811311227</v>
+        <v>0.3078616682257471</v>
       </c>
       <c r="J19" t="n">
-        <v>10.88205819350233</v>
+        <v>0.05151304988219139</v>
       </c>
       <c r="K19" t="n">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="L19" t="n">
-        <v>30</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="M19" t="n">
-        <v>-0.07760962359333323</v>
+        <v>0.707167317842221</v>
       </c>
       <c r="N19" t="n">
-        <v>-20.007193</v>
+        <v>0.9477418889322627</v>
       </c>
       <c r="O19" t="n">
-        <v>-8.432029999999999</v>
+        <v>0.9349409162618966</v>
       </c>
       <c r="P19" t="n">
-        <v>-5.6037455</v>
+        <v>0.9726056409760415</v>
       </c>
       <c r="Q19" t="n">
-        <v>-19.265</v>
+        <v>0.9726867961769763</v>
       </c>
       <c r="R19" t="n">
-        <v>-43.9</v>
+        <v>0.9169728141072739</v>
       </c>
       <c r="S19" t="n">
-        <v>-66.87507419383033</v>
+        <v>0.4336260924203046</v>
       </c>
       <c r="T19" t="n">
-        <v>0.1908295315356896</v>
+        <v>0.3728096184401299</v>
       </c>
       <c r="U19" t="n">
-        <v>9.197162061239732</v>
+        <v>0.5092942376639913</v>
       </c>
       <c r="V19" t="n">
-        <v>12.98702941412517</v>
+        <v>0.4386049770394332</v>
       </c>
       <c r="W19" t="n">
         <v>11</v>
       </c>
       <c r="X19" t="n">
-        <v>20.5</v>
+        <v>25.5</v>
       </c>
       <c r="Y19" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="Z19" t="n">
         <v>10</v>
@@ -3551,7 +3551,7 @@
         <v>2</v>
       </c>
       <c r="AB19" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AC19" t="n">
         <v>8</v>
@@ -3575,7 +3575,7 @@
         <v>8</v>
       </c>
       <c r="AJ19" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AK19" t="n">
         <v>11</v>
@@ -3596,34 +3596,34 @@
         <v>19</v>
       </c>
       <c r="AQ19" t="n">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="AR19" t="n">
-        <v>3</v>
+        <v>0.1875</v>
       </c>
       <c r="AS19" t="n">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="AT19" t="n">
-        <v>9</v>
+        <v>0.4705882352941176</v>
       </c>
       <c r="AU19" t="n">
-        <v>6.959999999999999</v>
+        <v>0.3357142857142857</v>
       </c>
       <c r="AV19" t="n">
-        <v>5.294</v>
+        <v>0.3771953781512605</v>
       </c>
       <c r="AW19" t="n">
         <v>-2</v>
       </c>
       <c r="AX19" t="n">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="AY19" t="n">
         <v>15</v>
       </c>
       <c r="AZ19" t="n">
-        <v>16.5</v>
+        <v>19.16666666666667</v>
       </c>
       <c r="BA19" t="n">
         <v>21.5</v>
@@ -3636,76 +3636,76 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>-3.127069384853576</v>
+        <v>0.113685774090642</v>
       </c>
       <c r="C20" t="n">
-        <v>14.47142425533319</v>
+        <v>0.5072357121276666</v>
       </c>
       <c r="D20" t="n">
-        <v>49.7413257607549</v>
+        <v>0.4513131920195029</v>
       </c>
       <c r="E20" t="n">
-        <v>15.3894231359842</v>
+        <v>0.4599065425340659</v>
       </c>
       <c r="F20" t="n">
-        <v>-12.1058808561454</v>
+        <v>0.4939470595719273</v>
       </c>
       <c r="G20" t="n">
-        <v>-10.37273590776588</v>
+        <v>0.684135364374381</v>
       </c>
       <c r="H20" t="n">
-        <v>4.942168202313272</v>
+        <v>0.04650230889826245</v>
       </c>
       <c r="I20" t="n">
-        <v>3.85414624583415</v>
+        <v>0.03121194287098504</v>
       </c>
       <c r="J20" t="n">
-        <v>1.098445183005373</v>
+        <v>0.00368898591762829</v>
       </c>
       <c r="K20" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="L20" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="M20" t="n">
-        <v>2.030008826125329</v>
+        <v>0.7516905071046697</v>
       </c>
       <c r="N20" t="n">
-        <v>-22.035713</v>
+        <v>0.9424678022651661</v>
       </c>
       <c r="O20" t="n">
-        <v>-3.8634846</v>
+        <v>0.9721045193332719</v>
       </c>
       <c r="P20" t="n">
-        <v>-2.0051274</v>
+        <v>0.9915700733365406</v>
       </c>
       <c r="Q20" t="n">
-        <v>-14.146</v>
+        <v>0.9795666462366311</v>
       </c>
       <c r="R20" t="n">
-        <v>-81.8</v>
+        <v>0.8241489101151114</v>
       </c>
       <c r="S20" t="n">
-        <v>-14.6143510056393</v>
+        <v>0.8998891664680193</v>
       </c>
       <c r="T20" t="n">
-        <v>4.23207808758245</v>
+        <v>0.5595493931002241</v>
       </c>
       <c r="U20" t="n">
-        <v>21.56525066972828</v>
+        <v>0.7642467673370593</v>
       </c>
       <c r="V20" t="n">
-        <v>8.642770463208505</v>
+        <v>0.4572878914140265</v>
       </c>
       <c r="W20" t="n">
         <v>23</v>
       </c>
       <c r="X20" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Y20" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="Z20" t="n">
         <v>18</v>
@@ -3759,31 +3759,31 @@
         <v>3</v>
       </c>
       <c r="AQ20" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AR20" t="n">
-        <v>3</v>
+        <v>0.1875</v>
       </c>
       <c r="AS20" t="n">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="AT20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AU20" t="n">
-        <v>7.92</v>
+        <v>0.5071428571428573</v>
       </c>
       <c r="AV20" t="n">
-        <v>4.238</v>
+        <v>0.3323214285714285</v>
       </c>
       <c r="AW20" t="n">
         <v>-2</v>
       </c>
       <c r="AX20" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AY20" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AZ20" t="n">
         <v>18.83333333333333</v>
@@ -3799,76 +3799,76 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>4.096755819215803</v>
+        <v>0.2021414490655427</v>
       </c>
       <c r="C21" t="n">
-        <v>-17.66846748285585</v>
+        <v>0.4911657662585721</v>
       </c>
       <c r="D21" t="n">
-        <v>15.85060415097002</v>
+        <v>0.05007837814936534</v>
       </c>
       <c r="E21" t="n">
-        <v>15.85060415097002</v>
+        <v>0.4695966039159827</v>
       </c>
       <c r="F21" t="n">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="G21" t="n">
-        <v>-16.09818886087115</v>
+        <v>0.5030802432668626</v>
       </c>
       <c r="H21" t="n">
-        <v>57.01102979074322</v>
+        <v>0.778244851013052</v>
       </c>
       <c r="I21" t="n">
-        <v>57.01102979074322</v>
+        <v>0.778244851013052</v>
       </c>
       <c r="J21" t="n">
-        <v>0.2366152385206008</v>
+        <v>0</v>
       </c>
       <c r="K21" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="L21" t="n">
-        <v>20</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="M21" t="n">
-        <v>6.473192326610921</v>
+        <v>0.8455522304855386</v>
       </c>
       <c r="N21" t="n">
-        <v>-14.171155</v>
+        <v>0.9632609613705454</v>
       </c>
       <c r="O21" t="n">
-        <v>-2.575629</v>
+        <v>0.982653942498781</v>
       </c>
       <c r="P21" t="n">
-        <v>-0.95275617</v>
+        <v>0.9971298983628701</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.073</v>
+        <v>1</v>
       </c>
       <c r="R21" t="n">
-        <v>-140</v>
+        <v>0.6816066617683075</v>
       </c>
       <c r="S21" t="n">
-        <v>-35.06301256914385</v>
+        <v>0.7174489854083855</v>
       </c>
       <c r="T21" t="n">
-        <v>-1.374915265762693</v>
+        <v>0.300459000415107</v>
       </c>
       <c r="U21" t="n">
-        <v>-15.50938337801609</v>
+        <v>0</v>
       </c>
       <c r="V21" t="n">
-        <v>6.681589930541358</v>
+        <v>0.4373181557965208</v>
       </c>
       <c r="W21" t="n">
         <v>19</v>
       </c>
       <c r="X21" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="Y21" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="Z21" t="n">
         <v>17</v>
@@ -3922,34 +3922,34 @@
         <v>26</v>
       </c>
       <c r="AQ21" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="AR21" t="n">
-        <v>5</v>
+        <v>0.3125</v>
       </c>
       <c r="AS21" t="n">
         <v>0</v>
       </c>
       <c r="AT21" t="n">
-        <v>12</v>
+        <v>0.6470588235294118</v>
       </c>
       <c r="AU21" t="n">
-        <v>8.92</v>
+        <v>0.6857142857142859</v>
       </c>
       <c r="AV21" t="n">
-        <v>4.638</v>
+        <v>0.2936659663865546</v>
       </c>
       <c r="AW21" t="n">
         <v>-2</v>
       </c>
       <c r="AX21" t="n">
+        <v>22</v>
+      </c>
+      <c r="AY21" t="n">
         <v>20</v>
       </c>
-      <c r="AY21" t="n">
-        <v>16</v>
-      </c>
       <c r="AZ21" t="n">
-        <v>19.16666666666667</v>
+        <v>21.16666666666667</v>
       </c>
       <c r="BA21" t="n">
         <v>21.5</v>
@@ -3962,76 +3962,76 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>-12.41133701893298</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>38.43620138437393</v>
+        <v>0.3174709703293532</v>
       </c>
       <c r="E22" t="n">
-        <v>-6.499000241838153</v>
+        <v>0</v>
       </c>
       <c r="F22" t="n">
-        <v>-10</v>
+        <v>0</v>
       </c>
       <c r="G22" t="n">
-        <v>-5.037876498438602</v>
+        <v>0.8528388057193081</v>
       </c>
       <c r="H22" t="n">
-        <v>13.26865922727528</v>
+        <v>0.1635174984689818</v>
       </c>
       <c r="I22" t="n">
-        <v>9.848595300846746</v>
+        <v>0.115454103277027</v>
       </c>
       <c r="J22" t="n">
-        <v>1.463938293126425</v>
+        <v>0.005523177627823206</v>
       </c>
       <c r="K22" t="n">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="L22" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="M22" t="n">
-        <v>-5.444690810544461</v>
+        <v>0.5937883656388702</v>
       </c>
       <c r="N22" t="n">
-        <v>-31.762783</v>
+        <v>0.9160074037932391</v>
       </c>
       <c r="O22" t="n">
-        <v>-2.7113304</v>
+        <v>0.9812122805696908</v>
       </c>
       <c r="P22" t="n">
-        <v>-1.3777176</v>
+        <v>0.9947898324937987</v>
       </c>
       <c r="Q22" t="n">
-        <v>-18.024</v>
+        <v>0.9729456082296545</v>
       </c>
       <c r="R22" t="n">
-        <v>-123</v>
+        <v>0.7232427136909134</v>
       </c>
       <c r="S22" t="n">
-        <v>-115.4777074378162</v>
+        <v>0</v>
       </c>
       <c r="T22" t="n">
-        <v>13.763900552205</v>
+        <v>1</v>
       </c>
       <c r="U22" t="n">
-        <v>-4.418852633823843</v>
+        <v>0.2286172874528176</v>
       </c>
       <c r="V22" t="n">
-        <v>-1.915161541857004</v>
+        <v>0.2314229632698124</v>
       </c>
       <c r="W22" t="n">
         <v>26</v>
       </c>
       <c r="X22" t="n">
-        <v>20.5</v>
+        <v>25.5</v>
       </c>
       <c r="Y22" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="Z22" t="n">
         <v>26</v>
@@ -4070,7 +4070,7 @@
         <v>4</v>
       </c>
       <c r="AL22" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="AM22" t="n">
         <v>15</v>
@@ -4094,13 +4094,13 @@
         <v>0</v>
       </c>
       <c r="AT22" t="n">
-        <v>9</v>
+        <v>0.4705882352941176</v>
       </c>
       <c r="AU22" t="n">
-        <v>7.080000000000001</v>
+        <v>0.3571428571428574</v>
       </c>
       <c r="AV22" t="n">
-        <v>2.412</v>
+        <v>0.1241596638655462</v>
       </c>
       <c r="AW22" t="n">
         <v>-2</v>
@@ -4125,73 +4125,73 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>5.311712171208316</v>
+        <v>0.217018578722556</v>
       </c>
       <c r="C23" t="n">
-        <v>33.89954720126429</v>
+        <v>0.5169497736006321</v>
       </c>
       <c r="D23" t="n">
-        <v>38.12531076736674</v>
+        <v>0.3137903128241781</v>
       </c>
       <c r="E23" t="n">
-        <v>9.979380903117223</v>
+        <v>0.3462339506194687</v>
       </c>
       <c r="F23" t="n">
-        <v>-4.647117234610764</v>
+        <v>0.4976764413826946</v>
       </c>
       <c r="G23" t="n">
-        <v>-2.456880076208734</v>
+        <v>0.9344572599503315</v>
       </c>
       <c r="H23" t="n">
-        <v>15.4830640456097</v>
+        <v>0.1946373301996476</v>
       </c>
       <c r="I23" t="n">
-        <v>15.04922521396774</v>
+        <v>0.1885404362048625</v>
       </c>
       <c r="J23" t="n">
-        <v>1.871579964907891</v>
+        <v>0.007464989376488444</v>
       </c>
       <c r="K23" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="L23" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="M23" t="n">
-        <v>12.83514240653122</v>
+        <v>0.97994766981392</v>
       </c>
       <c r="N23" t="n">
-        <v>-17.86221</v>
+        <v>0.953472163590055</v>
       </c>
       <c r="O23" t="n">
-        <v>-0.42557862</v>
+        <v>1</v>
       </c>
       <c r="P23" t="n">
-        <v>-0.40371707</v>
+        <v>1</v>
       </c>
       <c r="Q23" t="n">
-        <v>-15.904</v>
+        <v>0.9753261102965958</v>
       </c>
       <c r="R23" t="n">
-        <v>-10</v>
+        <v>1</v>
       </c>
       <c r="S23" t="n">
-        <v>-36.0547333105999</v>
+        <v>0.7086009876521535</v>
       </c>
       <c r="T23" t="n">
-        <v>1.851208301394448</v>
+        <v>0.4495331243155357</v>
       </c>
       <c r="U23" t="n">
-        <v>12.567078372749</v>
+        <v>0.5787608072854405</v>
       </c>
       <c r="V23" t="n">
-        <v>14.07464531357968</v>
+        <v>0.4958372626594436</v>
       </c>
       <c r="W23" t="n">
         <v>18</v>
       </c>
       <c r="X23" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y23" t="n">
         <v>15</v>
@@ -4248,34 +4248,34 @@
         <v>17</v>
       </c>
       <c r="AQ23" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="AR23" t="n">
-        <v>1</v>
+        <v>0.0625</v>
       </c>
       <c r="AS23" t="n">
         <v>0</v>
       </c>
       <c r="AT23" t="n">
-        <v>16</v>
+        <v>0.8823529411764706</v>
       </c>
       <c r="AU23" t="n">
-        <v>9.960000000000001</v>
+        <v>0.8714285714285719</v>
       </c>
       <c r="AV23" t="n">
-        <v>4.194</v>
+        <v>0.2818172268907564</v>
       </c>
       <c r="AW23" t="n">
         <v>0</v>
       </c>
       <c r="AX23" t="n">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="AY23" t="n">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="AZ23" t="n">
-        <v>13.83333333333333</v>
+        <v>16.5</v>
       </c>
       <c r="BA23" t="n">
         <v>12.5</v>
@@ -4288,76 +4288,76 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>-5.456505364521725</v>
+        <v>0.08516185136666882</v>
       </c>
       <c r="C24" t="n">
-        <v>-18.2924664115925</v>
+        <v>0.4908537667942038</v>
       </c>
       <c r="D24" t="n">
-        <v>59.35851003852313</v>
+        <v>0.565171763343964</v>
       </c>
       <c r="E24" t="n">
-        <v>20.81565396162424</v>
+        <v>0.5739192795382494</v>
       </c>
       <c r="F24" t="n">
-        <v>-30.69863332983753</v>
+        <v>0.4846506833350812</v>
       </c>
       <c r="G24" t="n">
-        <v>-2.507873873221591</v>
+        <v>0.9328446909240001</v>
       </c>
       <c r="H24" t="n">
-        <v>16.28204036447245</v>
+        <v>0.2058656333508742</v>
       </c>
       <c r="I24" t="n">
-        <v>11.2918334326833</v>
+        <v>0.1357364506771812</v>
       </c>
       <c r="J24" t="n">
-        <v>3.127922830386768</v>
+        <v>0.01353621374987976</v>
       </c>
       <c r="K24" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="L24" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="M24" t="n">
-        <v>-0.2904102817597565</v>
+        <v>0.7026719292295516</v>
       </c>
       <c r="N24" t="n">
-        <v>-9.404692000000001</v>
+        <v>0.9757567171855086</v>
       </c>
       <c r="O24" t="n">
-        <v>-1.9280291</v>
+        <v>0.987942429382592</v>
       </c>
       <c r="P24" t="n">
-        <v>-1.7894207</v>
+        <v>0.9927634082115141</v>
       </c>
       <c r="Q24" t="n">
-        <v>-6.662</v>
+        <v>0.9903372093519318</v>
       </c>
       <c r="R24" t="n">
-        <v>-62.6</v>
+        <v>0.8711731569924075</v>
       </c>
       <c r="S24" t="n">
-        <v>-31.43509248397971</v>
+        <v>0.7498167956512087</v>
       </c>
       <c r="T24" t="n">
-        <v>3.937306637090654</v>
+        <v>0.5459284654394633</v>
       </c>
       <c r="U24" t="n">
-        <v>13.50328947368421</v>
+        <v>0.5980596169921902</v>
       </c>
       <c r="V24" t="n">
-        <v>6.031961772324975</v>
+        <v>0.496206894603731</v>
       </c>
       <c r="W24" t="n">
         <v>25</v>
       </c>
       <c r="X24" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="Y24" t="n">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="Z24" t="n">
         <v>12</v>
@@ -4411,34 +4411,34 @@
         <v>12</v>
       </c>
       <c r="AQ24" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="AR24" t="n">
         <v>0</v>
       </c>
       <c r="AS24" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="AT24" t="n">
-        <v>5</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="AU24" t="n">
-        <v>7.759999999999999</v>
+        <v>0.4785714285714285</v>
       </c>
       <c r="AV24" t="n">
-        <v>5.914</v>
+        <v>0.5070798319327731</v>
       </c>
       <c r="AW24" t="n">
         <v>-2</v>
       </c>
       <c r="AX24" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="AY24" t="n">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="AZ24" t="n">
-        <v>18.5</v>
+        <v>15.5</v>
       </c>
       <c r="BA24" t="n">
         <v>21.5</v>
@@ -4451,67 +4451,67 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>6.544395463392694</v>
+        <v>0.2321127746035732</v>
       </c>
       <c r="C25" t="n">
-        <v>-8.468436040769767</v>
+        <v>0.4957657819796151</v>
       </c>
       <c r="D25" t="n">
-        <v>63.64475642761228</v>
+        <v>0.6159169582067138</v>
       </c>
       <c r="E25" t="n">
-        <v>30.74391359762542</v>
+        <v>0.7825259701051102</v>
       </c>
       <c r="F25" t="n">
-        <v>4.759229531829212</v>
+        <v>0.5023796147659146</v>
       </c>
       <c r="G25" t="n">
-        <v>-7.629676510426853</v>
+        <v>0.7708787112253882</v>
       </c>
       <c r="H25" t="n">
-        <v>1.633187042671735</v>
+        <v>0</v>
       </c>
       <c r="I25" t="n">
-        <v>1.633187042671735</v>
+        <v>0</v>
       </c>
       <c r="J25" t="n">
-        <v>2.072377747003896</v>
+        <v>0.008418416887212727</v>
       </c>
       <c r="K25" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="L25" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="M25" t="n">
-        <v>-1.327330652992109</v>
+        <v>0.6807671096239777</v>
       </c>
       <c r="N25" t="n">
-        <v>-38.603546</v>
+        <v>0.8993275595922393</v>
       </c>
       <c r="O25" t="n">
-        <v>-8.432829999999999</v>
+        <v>0.9352156928307442</v>
       </c>
       <c r="P25" t="n">
-        <v>-2.2554884</v>
+        <v>0.9902905427629883</v>
       </c>
       <c r="Q25" t="n">
-        <v>-18.443</v>
+        <v>0.9737732379805265</v>
       </c>
       <c r="R25" t="n">
-        <v>-94</v>
+        <v>0.7942689199118295</v>
       </c>
       <c r="S25" t="n">
-        <v>-22.30591767442485</v>
+        <v>0.8312660533450602</v>
       </c>
       <c r="T25" t="n">
-        <v>2.581220394797471</v>
+        <v>0.4832658413040146</v>
       </c>
       <c r="U25" t="n">
-        <v>15.19173494517928</v>
+        <v>0.6328647884135252</v>
       </c>
       <c r="V25" t="n">
-        <v>8.946967212645861</v>
+        <v>0.4981603003175227</v>
       </c>
       <c r="W25" t="n">
         <v>17</v>
@@ -4553,13 +4553,13 @@
         <v>21</v>
       </c>
       <c r="AJ25" t="n">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AK25" t="n">
         <v>7</v>
       </c>
       <c r="AL25" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AM25" t="n">
         <v>9</v>
@@ -4574,34 +4574,34 @@
         <v>9</v>
       </c>
       <c r="AQ25" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AR25" t="n">
-        <v>1</v>
+        <v>0.0625</v>
       </c>
       <c r="AS25" t="n">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="AT25" t="n">
-        <v>3</v>
+        <v>0.1176470588235294</v>
       </c>
       <c r="AU25" t="n">
-        <v>8.44</v>
+        <v>0.6000000000000001</v>
       </c>
       <c r="AV25" t="n">
-        <v>4.016</v>
+        <v>0.3263970588235294</v>
       </c>
       <c r="AW25" t="n">
         <v>-2</v>
       </c>
       <c r="AX25" t="n">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AY25" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="AZ25" t="n">
-        <v>19.83333333333333</v>
+        <v>16.83333333333333</v>
       </c>
       <c r="BA25" t="n">
         <v>21.5</v>
@@ -4614,67 +4614,67 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>1.949975333535692</v>
+        <v>0.1758541412307952</v>
       </c>
       <c r="C26" t="n">
-        <v>-0.6755970694940938</v>
+        <v>0.4996622014652529</v>
       </c>
       <c r="D26" t="n">
-        <v>11.62068113865888</v>
+        <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>8.81299274748751</v>
+        <v>0.3217264959413093</v>
       </c>
       <c r="F26" t="n">
-        <v>-11.77500069881041</v>
+        <v>0.4941124996505948</v>
       </c>
       <c r="G26" t="n">
-        <v>-32.00694773409127</v>
+        <v>0</v>
       </c>
       <c r="H26" t="n">
-        <v>11.25077239958805</v>
+        <v>0.1351594051297584</v>
       </c>
       <c r="I26" t="n">
-        <v>9.461894953656024</v>
+        <v>0.1100196634514233</v>
       </c>
       <c r="J26" t="n">
-        <v>3.509094495042173</v>
+        <v>0.01543089909934837</v>
       </c>
       <c r="K26" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="L26" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="M26" t="n">
-        <v>13.78437047756874</v>
+        <v>1</v>
       </c>
       <c r="N26" t="n">
-        <v>-17.303806</v>
+        <v>0.9549862332951745</v>
       </c>
       <c r="O26" t="n">
-        <v>-1.5806433</v>
+        <v>0.9906732482735996</v>
       </c>
       <c r="P26" t="n">
-        <v>-21.15654</v>
+        <v>0.8910425679458738</v>
       </c>
       <c r="Q26" t="n">
-        <v>-18.622</v>
+        <v>0.9733864419457549</v>
       </c>
       <c r="R26" t="n">
-        <v>-26.2</v>
+        <v>0.9603232916972814</v>
       </c>
       <c r="S26" t="n">
-        <v>-9.885073471050896</v>
+        <v>0.9420831382843193</v>
       </c>
       <c r="T26" t="n">
-        <v>2.941546649405757</v>
+        <v>0.4999159539255181</v>
       </c>
       <c r="U26" t="n">
-        <v>13.06596701649175</v>
+        <v>0.5890447667373551</v>
       </c>
       <c r="V26" t="n">
-        <v>4.243071781557444</v>
+        <v>0.3903181642401759</v>
       </c>
       <c r="W26" t="n">
         <v>21</v>
@@ -4683,7 +4683,7 @@
         <v>18</v>
       </c>
       <c r="Y26" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="Z26" t="n">
         <v>21</v>
@@ -4722,7 +4722,7 @@
         <v>19</v>
       </c>
       <c r="AL26" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AM26" t="n">
         <v>3</v>
@@ -4737,34 +4737,34 @@
         <v>14</v>
       </c>
       <c r="AQ26" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AR26" t="n">
         <v>0</v>
       </c>
       <c r="AS26" t="n">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="AT26" t="n">
-        <v>8</v>
+        <v>0.4117647058823529</v>
       </c>
       <c r="AU26" t="n">
-        <v>6.2</v>
+        <v>0.2000000000000001</v>
       </c>
       <c r="AV26" t="n">
-        <v>4.13</v>
+        <v>0.291764705882353</v>
       </c>
       <c r="AW26" t="n">
         <v>-2</v>
       </c>
       <c r="AX26" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AY26" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="AZ26" t="n">
-        <v>21.16666666666667</v>
+        <v>22.16666666666667</v>
       </c>
       <c r="BA26" t="n">
         <v>21.5</v>
@@ -4777,73 +4777,73 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.2369400972417335</v>
+        <v>0.1548780400930198</v>
       </c>
       <c r="C27" t="n">
-        <v>-22.78184174154354</v>
+        <v>0.4886090791292282</v>
       </c>
       <c r="D27" t="n">
-        <v>83.12431960843702</v>
+        <v>0.8465369785509608</v>
       </c>
       <c r="E27" t="n">
-        <v>-5.564784283049138</v>
+        <v>0.01962919047070939</v>
       </c>
       <c r="F27" t="n">
-        <v>1.985149015726884</v>
+        <v>0.5009925745078634</v>
       </c>
       <c r="G27" t="n">
-        <v>-7.443144048506335</v>
+        <v>0.7767773986759917</v>
       </c>
       <c r="H27" t="n">
-        <v>7.626313823827562</v>
+        <v>0.08422357801334494</v>
       </c>
       <c r="I27" t="n">
-        <v>5.163527717014352</v>
+        <v>0.04961315421093695</v>
       </c>
       <c r="J27" t="n">
-        <v>1.367606298185855</v>
+        <v>0.005024446549070471</v>
       </c>
       <c r="K27" t="n">
-        <v>30</v>
+        <v>0.5</v>
       </c>
       <c r="L27" t="n">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="M27" t="n">
-        <v>3.191954525579366</v>
+        <v>0.7762364719098203</v>
       </c>
       <c r="N27" t="n">
-        <v>-0.10475781</v>
+        <v>1</v>
       </c>
       <c r="O27" t="n">
-        <v>-3.3193715</v>
+        <v>0.9763364213360979</v>
       </c>
       <c r="P27" t="n">
-        <v>-189.10521</v>
+        <v>0</v>
       </c>
       <c r="Q27" t="n">
-        <v>-9.476000000000001</v>
+        <v>0.9863768161282571</v>
       </c>
       <c r="R27" t="n">
-        <v>-15.9</v>
+        <v>0.9855498408033309</v>
       </c>
       <c r="S27" t="n">
-        <v>-113.6662432659112</v>
+        <v>0.01616163730222851</v>
       </c>
       <c r="T27" t="n">
-        <v>5.93528961555606</v>
+        <v>0.6382521337313021</v>
       </c>
       <c r="U27" t="n">
-        <v>33.0019556714472</v>
+        <v>1</v>
       </c>
       <c r="V27" t="n">
-        <v>3.387334335792863</v>
+        <v>0.4274328096663137</v>
       </c>
       <c r="W27" t="n">
         <v>22</v>
       </c>
       <c r="X27" t="n">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="Y27" t="n">
         <v>12</v>
@@ -4894,40 +4894,40 @@
         <v>25</v>
       </c>
       <c r="AO27" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AP27" t="n">
         <v>1</v>
       </c>
       <c r="AQ27" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AR27" t="n">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="AS27" t="n">
-        <v>5</v>
+        <v>0.5</v>
       </c>
       <c r="AT27" t="n">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="AU27" t="n">
-        <v>8.120000000000001</v>
+        <v>0.5428571428571433</v>
       </c>
       <c r="AV27" t="n">
-        <v>10.718</v>
+        <v>0.7314285714285715</v>
       </c>
       <c r="AW27" t="n">
         <v>-2</v>
       </c>
       <c r="AX27" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="AY27" t="n">
         <v>2</v>
       </c>
       <c r="AZ27" t="n">
-        <v>15.83333333333333</v>
+        <v>15.5</v>
       </c>
       <c r="BA27" t="n">
         <v>21.5</v>

</xml_diff>

<commit_message>
Added figures and report with waterfall contributions of quant scores per stock
</commit_message>
<xml_diff>
--- a/output/stock_analysis_scores.xlsx
+++ b/output/stock_analysis_scores.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:BA27"/>
+  <dimension ref="A1:BU27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -646,50 +646,150 @@
       </c>
       <c r="AR1" s="1" t="inlineStr">
         <is>
+          <t>revenue_growth_contrib</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>eps_growth_contrib</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>fcf_growth_contrib</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>net_margin_avg_contrib</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
+        <is>
+          <t>gross_margin_avg_contrib</t>
+        </is>
+      </c>
+      <c r="AW1" s="1" t="inlineStr">
+        <is>
+          <t>d_e_ratio_contrib</t>
+        </is>
+      </c>
+      <c r="AX1" s="1" t="inlineStr">
+        <is>
+          <t>curr_ratio_contrib</t>
+        </is>
+      </c>
+      <c r="AY1" s="1" t="inlineStr">
+        <is>
+          <t>quick_ratio_contrib</t>
+        </is>
+      </c>
+      <c r="AZ1" s="1" t="inlineStr">
+        <is>
+          <t>z_score_contrib</t>
+        </is>
+      </c>
+      <c r="BA1" s="1" t="inlineStr">
+        <is>
+          <t>no_y_pos_eps_contrib</t>
+        </is>
+      </c>
+      <c r="BB1" s="1" t="inlineStr">
+        <is>
+          <t>no_y_pos_fcf_contrib</t>
+        </is>
+      </c>
+      <c r="BC1" s="1" t="inlineStr">
+        <is>
+          <t>shares_chg_contrib</t>
+        </is>
+      </c>
+      <c r="BD1" s="1" t="inlineStr">
+        <is>
+          <t>pe_ratio_contrib</t>
+        </is>
+      </c>
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>ps_ratio_contrib</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>pb_ratio_contrib</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>ev_ebitda_contrib</t>
+        </is>
+      </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>beta_contrib</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>scaled_vol_contrib</t>
+        </is>
+      </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>accrual_rat_contrib</t>
+        </is>
+      </c>
+      <c r="BK1" s="1" t="inlineStr">
+        <is>
+          <t>cash_conv_rat_contrib</t>
+        </is>
+      </c>
+      <c r="BL1" s="1" t="inlineStr">
+        <is>
           <t>MOAT_TEXT</t>
         </is>
       </c>
-      <c r="AS1" s="1" t="inlineStr">
+      <c r="BM1" s="1" t="inlineStr">
         <is>
           <t>MOAT_QUANT</t>
         </is>
       </c>
-      <c r="AT1" s="1" t="inlineStr">
+      <c r="BN1" s="1" t="inlineStr">
         <is>
           <t>MANAGEMENT</t>
         </is>
       </c>
-      <c r="AU1" s="1" t="inlineStr">
+      <c r="BO1" s="1" t="inlineStr">
         <is>
           <t>SENTIMENT</t>
         </is>
       </c>
-      <c r="AV1" s="1" t="inlineStr">
+      <c r="BP1" s="1" t="inlineStr">
         <is>
           <t>Qual Score</t>
         </is>
       </c>
-      <c r="AW1" s="1" t="inlineStr">
+      <c r="BQ1" s="1" t="inlineStr">
         <is>
           <t>External Rating Score</t>
         </is>
       </c>
-      <c r="AX1" s="1" t="inlineStr">
+      <c r="BR1" s="1" t="inlineStr">
         <is>
           <t>Quant Rank</t>
         </is>
       </c>
-      <c r="AY1" s="1" t="inlineStr">
+      <c r="BS1" s="1" t="inlineStr">
         <is>
           <t>Qual Rank</t>
         </is>
       </c>
-      <c r="AZ1" s="1" t="inlineStr">
+      <c r="BT1" s="1" t="inlineStr">
         <is>
           <t>Final Rank</t>
         </is>
       </c>
-      <c r="BA1" s="1" t="inlineStr">
+      <c r="BU1" s="1" t="inlineStr">
         <is>
           <t>External Rating Rank</t>
         </is>
@@ -726,7 +826,7 @@
         <v>0.1663195011416484</v>
       </c>
       <c r="J2" t="n">
-        <v>0.04717297044309587</v>
+        <v>0.04631651070770491</v>
       </c>
       <c r="K2" t="n">
         <v>1</v>
@@ -738,13 +838,13 @@
         <v>0.7265611810807434</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9109327977518669</v>
+        <v>0.9125860762637976</v>
       </c>
       <c r="O2" t="n">
-        <v>0.8943858253170122</v>
+        <v>0.8963287509250313</v>
       </c>
       <c r="P2" t="n">
-        <v>0.9441324103030683</v>
+        <v>0.9443308582661795</v>
       </c>
       <c r="Q2" t="n">
         <v>0.9652381284191277</v>
@@ -762,7 +862,7 @@
         <v>0.5953375612217265</v>
       </c>
       <c r="V2" t="n">
-        <v>0.5631956754380434</v>
+        <v>0.5824938246584986</v>
       </c>
       <c r="W2" t="n">
         <v>12</v>
@@ -801,7 +901,7 @@
         <v>15</v>
       </c>
       <c r="AI2" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AJ2" t="n">
         <v>22</v>
@@ -825,36 +925,96 @@
         <v>13</v>
       </c>
       <c r="AQ2" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AR2" t="n">
+        <v>0.03953269300078874</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>0.06579283354166217</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>0.02508006513551462</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>0.1144903052899215</v>
+      </c>
+      <c r="AV2" t="n">
+        <v>0.08857210900421632</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>0.04781848307341702</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>0.005017588659606384</v>
+      </c>
+      <c r="AY2" t="n">
+        <v>0.004989585034249453</v>
+      </c>
+      <c r="AZ2" t="n">
+        <v>0.004631651070770492</v>
+      </c>
+      <c r="BA2" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>0.01453122362161487</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>0.01825172152527595</v>
+      </c>
+      <c r="BE2" t="n">
+        <v>0.01792657501850062</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>0.01888661716532359</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>0.01930476256838256</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>0.01539554249326476</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>0.01796002986406243</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>0.0124052873674925</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>0.01190675122443453</v>
+      </c>
+      <c r="BL2" t="n">
         <v>0.1875</v>
       </c>
-      <c r="AS2" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT2" t="n">
+      <c r="BM2" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN2" t="n">
         <v>0.4117647058823529</v>
       </c>
-      <c r="AU2" t="n">
+      <c r="BO2" t="n">
         <v>0.5857142857142862</v>
       </c>
-      <c r="AV2" t="n">
+      <c r="BP2" t="n">
         <v>0.605871848739496</v>
       </c>
-      <c r="AW2" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX2" t="n">
-        <v>7</v>
-      </c>
-      <c r="AY2" t="n">
+      <c r="BQ2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR2" t="n">
+        <v>5</v>
+      </c>
+      <c r="BS2" t="n">
         <v>8</v>
       </c>
-      <c r="AZ2" t="n">
-        <v>9.166666666666666</v>
-      </c>
-      <c r="BA2" t="n">
+      <c r="BT2" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="BU2" t="n">
         <v>12.5</v>
       </c>
     </row>
@@ -889,7 +1049,7 @@
         <v>0.09312996144177385</v>
       </c>
       <c r="J3" t="n">
-        <v>0.04380607548732765</v>
+        <v>0.04314676143321022</v>
       </c>
       <c r="K3" t="n">
         <v>1</v>
@@ -901,13 +1061,13 @@
         <v>0.8805110616835674</v>
       </c>
       <c r="N3" t="n">
-        <v>0.9207813685041114</v>
+        <v>0.9219589828062312</v>
       </c>
       <c r="O3" t="n">
-        <v>0.929210906502052</v>
+        <v>0.9302312003183802</v>
       </c>
       <c r="P3" t="n">
-        <v>0.7030576364069231</v>
+        <v>0.7030609047385677</v>
       </c>
       <c r="Q3" t="n">
         <v>0.9618053136105278</v>
@@ -925,7 +1085,7 @@
         <v>0.5797619250522088</v>
       </c>
       <c r="V3" t="n">
-        <v>0.468088314943601</v>
+        <v>0.4691472031616153</v>
       </c>
       <c r="W3" t="n">
         <v>20</v>
@@ -988,36 +1148,96 @@
         <v>16</v>
       </c>
       <c r="AQ3" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="AR3" t="n">
+        <v>0.02333385975346928</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>0.06516396550623677</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>0.02513474031700482</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>0.08566306021106798</v>
+      </c>
+      <c r="AV3" t="n">
+        <v>0.05067936756099503</v>
+      </c>
+      <c r="AW3" t="n">
+        <v>0.02100339152802092</v>
+      </c>
+      <c r="AX3" t="n">
+        <v>0.002968044143912823</v>
+      </c>
+      <c r="AY3" t="n">
+        <v>0.002793898843253215</v>
+      </c>
+      <c r="AZ3" t="n">
+        <v>0.004314676143321023</v>
+      </c>
+      <c r="BA3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BB3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BC3" t="n">
+        <v>0.01761022123367135</v>
+      </c>
+      <c r="BD3" t="n">
+        <v>0.01843917965612462</v>
+      </c>
+      <c r="BE3" t="n">
+        <v>0.0186046240063676</v>
+      </c>
+      <c r="BF3" t="n">
+        <v>0.01406121809477136</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>0.01923610627221056</v>
+      </c>
+      <c r="BH3" t="n">
+        <v>0.01505755571883419</v>
+      </c>
+      <c r="BI3" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BJ3" t="n">
+        <v>0.01348805567130955</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>0.01159523850104418</v>
+      </c>
+      <c r="BL3" t="n">
         <v>0.0625</v>
       </c>
-      <c r="AS3" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT3" t="n">
+      <c r="BM3" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN3" t="n">
         <v>0.4117647058823529</v>
       </c>
-      <c r="AU3" t="n">
+      <c r="BO3" t="n">
         <v>0.4071428571428572</v>
       </c>
-      <c r="AV3" t="n">
+      <c r="BP3" t="n">
         <v>0.5415861344537816</v>
       </c>
-      <c r="AW3" t="n">
+      <c r="BQ3" t="n">
         <v>-1</v>
       </c>
-      <c r="AX3" t="n">
-        <v>18</v>
-      </c>
-      <c r="AY3" t="n">
+      <c r="BR3" t="n">
+        <v>16</v>
+      </c>
+      <c r="BS3" t="n">
         <v>10</v>
       </c>
-      <c r="AZ3" t="n">
-        <v>14.5</v>
-      </c>
-      <c r="BA3" t="n">
+      <c r="BT3" t="n">
+        <v>13.83333333333333</v>
+      </c>
+      <c r="BU3" t="n">
         <v>15.5</v>
       </c>
     </row>
@@ -1052,7 +1272,7 @@
         <v>0.3058218618737277</v>
       </c>
       <c r="J4" t="n">
-        <v>0.09369783883611271</v>
+        <v>0.09181796522047064</v>
       </c>
       <c r="K4" t="n">
         <v>1</v>
@@ -1064,13 +1284,13 @@
         <v>0.8723889815444184</v>
       </c>
       <c r="N4" t="n">
-        <v>0.9280590770221323</v>
+        <v>0.9295556091552033</v>
       </c>
       <c r="O4" t="n">
-        <v>0.9381715388346016</v>
+        <v>0.9394440814048761</v>
       </c>
       <c r="P4" t="n">
-        <v>0.9588308050046499</v>
+        <v>0.9590708869069868</v>
       </c>
       <c r="Q4" t="n">
         <v>0.9702095951013421</v>
@@ -1088,7 +1308,7 @@
         <v>0.5776900013729086</v>
       </c>
       <c r="V4" t="n">
-        <v>0.5646952859791136</v>
+        <v>0.5496010605547099</v>
       </c>
       <c r="W4" t="n">
         <v>15</v>
@@ -1115,7 +1335,7 @@
         <v>9</v>
       </c>
       <c r="AE4" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AF4" t="n">
         <v>11</v>
@@ -1151,36 +1371,96 @@
         <v>18</v>
       </c>
       <c r="AQ4" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AR4" t="n">
+        <v>0.0368762404782183</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>0.06581932532592692</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>0.02506957522992934</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>0.08495924603996494</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>0.06943449985166603</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>0.04877549549279664</v>
+      </c>
+      <c r="AX4" t="n">
+        <v>0.009337090815433959</v>
+      </c>
+      <c r="AY4" t="n">
+        <v>0.009174655856211829</v>
+      </c>
+      <c r="AZ4" t="n">
+        <v>0.009181796522047064</v>
+      </c>
+      <c r="BA4" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BB4" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BC4" t="n">
+        <v>0.01744777963088837</v>
+      </c>
+      <c r="BD4" t="n">
+        <v>0.01859111218310407</v>
+      </c>
+      <c r="BE4" t="n">
+        <v>0.01878888162809752</v>
+      </c>
+      <c r="BF4" t="n">
+        <v>0.01918141773813974</v>
+      </c>
+      <c r="BG4" t="n">
+        <v>0.01940419190202684</v>
+      </c>
+      <c r="BH4" t="n">
+        <v>0.01553759490570659</v>
+      </c>
+      <c r="BI4" t="n">
+        <v>0.01681738005113619</v>
+      </c>
+      <c r="BJ4" t="n">
+        <v>0.01365097687595733</v>
+      </c>
+      <c r="BK4" t="n">
+        <v>0.01155380002745817</v>
+      </c>
+      <c r="BL4" t="n">
         <v>0.5</v>
       </c>
-      <c r="AS4" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT4" t="n">
+      <c r="BM4" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN4" t="n">
         <v>0.3529411764705883</v>
       </c>
-      <c r="AU4" t="n">
+      <c r="BO4" t="n">
         <v>0.7428571428571432</v>
       </c>
-      <c r="AV4" t="n">
+      <c r="BP4" t="n">
         <v>0.7143697478991597</v>
       </c>
-      <c r="AW4" t="n">
+      <c r="BQ4" t="n">
         <v>2</v>
       </c>
-      <c r="AX4" t="n">
-        <v>6</v>
-      </c>
-      <c r="AY4" t="n">
+      <c r="BR4" t="n">
+        <v>7</v>
+      </c>
+      <c r="BS4" t="n">
         <v>3</v>
       </c>
-      <c r="AZ4" t="n">
-        <v>3.666666666666667</v>
-      </c>
-      <c r="BA4" t="n">
+      <c r="BT4" t="n">
+        <v>4</v>
+      </c>
+      <c r="BU4" t="n">
         <v>2</v>
       </c>
     </row>
@@ -1215,7 +1495,7 @@
         <v>0.09974170517994529</v>
       </c>
       <c r="J5" t="n">
-        <v>0.02739625053119859</v>
+        <v>0.02698096420277992</v>
       </c>
       <c r="K5" t="n">
         <v>0.5</v>
@@ -1227,13 +1507,13 @@
         <v>0.6351202205493853</v>
       </c>
       <c r="N5" t="n">
-        <v>0.9065269436419175</v>
+        <v>0.9079201618741175</v>
       </c>
       <c r="O5" t="n">
-        <v>0.9750716264593272</v>
+        <v>0.9754074478848008</v>
       </c>
       <c r="P5" t="n">
-        <v>0.9651841491541497</v>
+        <v>0.965165271125231</v>
       </c>
       <c r="Q5" t="n">
         <v>0.9741884749002081</v>
@@ -1251,7 +1531,7 @@
         <v>0.722868999856208</v>
       </c>
       <c r="V5" t="n">
-        <v>0.4394651701670539</v>
+        <v>0.4485299070093264</v>
       </c>
       <c r="W5" t="n">
         <v>16</v>
@@ -1314,36 +1594,96 @@
         <v>5</v>
       </c>
       <c r="AQ5" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AR5" t="n">
+        <v>0.03684610410124924</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>0.06628219215316969</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>0.03054508974476772</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>0.0537548144911516</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>0.04337001407447085</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>0.003796161931970406</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>0.002992251155398359</v>
+      </c>
+      <c r="AZ5" t="n">
+        <v>0.002698096420277992</v>
+      </c>
+      <c r="BA5" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BB5" t="n">
+        <v>0.006666666666666666</v>
+      </c>
+      <c r="BC5" t="n">
+        <v>0.01270240441098771</v>
+      </c>
+      <c r="BD5" t="n">
+        <v>0.01815840323748235</v>
+      </c>
+      <c r="BE5" t="n">
+        <v>0.01950814895769602</v>
+      </c>
+      <c r="BF5" t="n">
+        <v>0.01930330542250462</v>
+      </c>
+      <c r="BG5" t="n">
+        <v>0.01948376949800416</v>
+      </c>
+      <c r="BH5" t="n">
+        <v>0.01407788390889052</v>
+      </c>
+      <c r="BI5" t="n">
+        <v>0.008232406711175</v>
+      </c>
+      <c r="BJ5" t="n">
+        <v>0.01565481412633928</v>
+      </c>
+      <c r="BK5" t="n">
+        <v>0.01445737999712416</v>
+      </c>
+      <c r="BL5" t="n">
         <v>0.375</v>
       </c>
-      <c r="AS5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT5" t="n">
+      <c r="BM5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN5" t="n">
         <v>0.2941176470588235</v>
       </c>
-      <c r="AU5" t="n">
+      <c r="BO5" t="n">
         <v>0.35</v>
       </c>
-      <c r="AV5" t="n">
+      <c r="BP5" t="n">
         <v>0.6091176470588234</v>
       </c>
-      <c r="AW5" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX5" t="n">
-        <v>20</v>
-      </c>
-      <c r="AY5" t="n">
+      <c r="BQ5" t="n">
+        <v>1</v>
+      </c>
+      <c r="BR5" t="n">
+        <v>21</v>
+      </c>
+      <c r="BS5" t="n">
         <v>6</v>
       </c>
-      <c r="AZ5" t="n">
-        <v>11</v>
-      </c>
-      <c r="BA5" t="n">
+      <c r="BT5" t="n">
+        <v>11.33333333333333</v>
+      </c>
+      <c r="BU5" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1378,7 +1718,7 @@
         <v>0.2030205917768616</v>
       </c>
       <c r="J6" t="n">
-        <v>0.09584913851042939</v>
+        <v>0.09162820374614881</v>
       </c>
       <c r="K6" t="n">
         <v>1</v>
@@ -1390,13 +1730,13 @@
         <v>0.5253294730906513</v>
       </c>
       <c r="N6" t="n">
-        <v>0.6424594952765212</v>
+        <v>0.6589894922898327</v>
       </c>
       <c r="O6" t="n">
-        <v>0.8747767539664674</v>
+        <v>0.8806468182784555</v>
       </c>
       <c r="P6" t="n">
-        <v>0.9051464262448219</v>
+        <v>0.9082165811103071</v>
       </c>
       <c r="Q6" t="n">
         <v>0.8251625041061528</v>
@@ -1414,7 +1754,7 @@
         <v>0.7511492748871105</v>
       </c>
       <c r="V6" t="n">
-        <v>0.4969180586672016</v>
+        <v>0.4507780253214322</v>
       </c>
       <c r="W6" t="n">
         <v>4</v>
@@ -1441,7 +1781,7 @@
         <v>13</v>
       </c>
       <c r="AE6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AF6" t="n">
         <v>11</v>
@@ -1477,36 +1817,96 @@
         <v>4</v>
       </c>
       <c r="AQ6" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="AR6" t="n">
-        <v>0</v>
+        <v>0.05474824231084491</v>
       </c>
       <c r="AS6" t="n">
-        <v>0</v>
+        <v>0.06539288620578035</v>
       </c>
       <c r="AT6" t="n">
-        <v>0</v>
+        <v>0.02502323068530539</v>
       </c>
       <c r="AU6" t="n">
+        <v>0.05257305030049449</v>
+      </c>
+      <c r="AV6" t="n">
+        <v>0.01377369399887991</v>
+      </c>
+      <c r="AW6" t="n">
+        <v>0.04765334783785795</v>
+      </c>
+      <c r="AX6" t="n">
+        <v>0.007848494789161822</v>
+      </c>
+      <c r="AY6" t="n">
+        <v>0.006090617753305849</v>
+      </c>
+      <c r="AZ6" t="n">
+        <v>0.009162820374614881</v>
+      </c>
+      <c r="BA6" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BB6" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BC6" t="n">
+        <v>0.01050658946181303</v>
+      </c>
+      <c r="BD6" t="n">
+        <v>0.01317978984579665</v>
+      </c>
+      <c r="BE6" t="n">
+        <v>0.01761293636556911</v>
+      </c>
+      <c r="BF6" t="n">
+        <v>0.01816433162220614</v>
+      </c>
+      <c r="BG6" t="n">
+        <v>0.01650325008212306</v>
+      </c>
+      <c r="BH6" t="n">
+        <v>0.01037472446730345</v>
+      </c>
+      <c r="BI6" t="n">
+        <v>0.01396726818515696</v>
+      </c>
+      <c r="BJ6" t="n">
+        <v>0.01317976553747598</v>
+      </c>
+      <c r="BK6" t="n">
+        <v>0.01502298549774221</v>
+      </c>
+      <c r="BL6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN6" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO6" t="n">
         <v>0.5928571428571431</v>
       </c>
-      <c r="AV6" t="n">
+      <c r="BP6" t="n">
         <v>0.08892857142857145</v>
       </c>
-      <c r="AW6" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX6" t="n">
-        <v>13</v>
-      </c>
-      <c r="AY6" t="n">
+      <c r="BQ6" t="n">
+        <v>1</v>
+      </c>
+      <c r="BR6" t="n">
+        <v>20</v>
+      </c>
+      <c r="BS6" t="n">
         <v>26</v>
       </c>
-      <c r="AZ6" t="n">
-        <v>15.33333333333333</v>
-      </c>
-      <c r="BA6" t="n">
+      <c r="BT6" t="n">
+        <v>17.66666666666667</v>
+      </c>
+      <c r="BU6" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1541,7 +1941,7 @@
         <v>0.5225027503283737</v>
       </c>
       <c r="J7" t="n">
-        <v>0.4141298953939992</v>
+        <v>0.4135619898282562</v>
       </c>
       <c r="K7" t="n">
         <v>1</v>
@@ -1553,13 +1953,13 @@
         <v>0.7430839628232666</v>
       </c>
       <c r="N7" t="n">
-        <v>0.8878134281190538</v>
+        <v>0.8878664081781904</v>
       </c>
       <c r="O7" t="n">
-        <v>0.7921107719388552</v>
+        <v>0.792120394861284</v>
       </c>
       <c r="P7" t="n">
-        <v>0.7761404879876588</v>
+        <v>0.7728439550497633</v>
       </c>
       <c r="Q7" t="n">
         <v>0.9382932340556843</v>
@@ -1577,7 +1977,7 @@
         <v>0.5009788316709686</v>
       </c>
       <c r="V7" t="n">
-        <v>0.7172734282580814</v>
+        <v>0.7141806300031365</v>
       </c>
       <c r="W7" t="n">
         <v>1</v>
@@ -1643,33 +2043,93 @@
         <v>1</v>
       </c>
       <c r="AR7" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>0.07127732438526745</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>0.02738991770064862</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>0.1278222362308842</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>0.087098128534546</v>
+      </c>
+      <c r="AW7" t="n">
+        <v>0.04856052813819937</v>
+      </c>
+      <c r="AX7" t="n">
+        <v>0.01802989857906338</v>
+      </c>
+      <c r="AY7" t="n">
+        <v>0.01567508250985121</v>
+      </c>
+      <c r="AZ7" t="n">
+        <v>0.04135619898282562</v>
+      </c>
+      <c r="BA7" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BB7" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BC7" t="n">
+        <v>0.01486167925646533</v>
+      </c>
+      <c r="BD7" t="n">
+        <v>0.01775732816356381</v>
+      </c>
+      <c r="BE7" t="n">
+        <v>0.01584240789722568</v>
+      </c>
+      <c r="BF7" t="n">
+        <v>0.01545687910099527</v>
+      </c>
+      <c r="BG7" t="n">
+        <v>0.01876586468111369</v>
+      </c>
+      <c r="BH7" t="n">
+        <v>0.01019348518246388</v>
+      </c>
+      <c r="BI7" t="n">
+        <v>0.004074094026603713</v>
+      </c>
+      <c r="BJ7" t="n">
+        <v>0</v>
+      </c>
+      <c r="BK7" t="n">
+        <v>0.01001957663341937</v>
+      </c>
+      <c r="BL7" t="n">
         <v>0.0625</v>
       </c>
-      <c r="AS7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT7" t="n">
+      <c r="BM7" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN7" t="n">
         <v>0.4117647058823529</v>
       </c>
-      <c r="AU7" t="n">
+      <c r="BO7" t="n">
         <v>0.03571428571428576</v>
       </c>
-      <c r="AV7" t="n">
+      <c r="BP7" t="n">
         <v>0.4858718487394958</v>
       </c>
-      <c r="AW7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX7" t="n">
-        <v>1</v>
-      </c>
-      <c r="AY7" t="n">
+      <c r="BQ7" t="n">
+        <v>1</v>
+      </c>
+      <c r="BR7" t="n">
+        <v>1</v>
+      </c>
+      <c r="BS7" t="n">
         <v>13</v>
       </c>
-      <c r="AZ7" t="n">
+      <c r="BT7" t="n">
         <v>7</v>
       </c>
-      <c r="BA7" t="n">
+      <c r="BU7" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1704,7 +2164,7 @@
         <v>0.3955410778355132</v>
       </c>
       <c r="J8" t="n">
-        <v>0.06917132465993209</v>
+        <v>0.06773128912413094</v>
       </c>
       <c r="K8" t="n">
         <v>1</v>
@@ -1716,13 +2176,13 @@
         <v>0.9196804035152566</v>
       </c>
       <c r="N8" t="n">
-        <v>0.9215579366909874</v>
+        <v>0.9232540004524955</v>
       </c>
       <c r="O8" t="n">
-        <v>0.9168614577123432</v>
+        <v>0.9186494941246219</v>
       </c>
       <c r="P8" t="n">
-        <v>0.9505942384385307</v>
+        <v>0.9509273129395278</v>
       </c>
       <c r="Q8" t="n">
         <v>0.9709874533036222</v>
@@ -1740,7 +2200,7 @@
         <v>0.6216004218447548</v>
       </c>
       <c r="V8" t="n">
-        <v>0.602203408587734</v>
+        <v>0.6008512042081281</v>
       </c>
       <c r="W8" t="n">
         <v>13</v>
@@ -1785,7 +2245,7 @@
         <v>18</v>
       </c>
       <c r="AK8" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AL8" t="n">
         <v>14</v>
@@ -1806,33 +2266,93 @@
         <v>4</v>
       </c>
       <c r="AR8" t="n">
+        <v>0.03843461910030711</v>
+      </c>
+      <c r="AS8" t="n">
+        <v>0.06634653632660778</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>0.02528784486687893</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>0.09677065516054695</v>
+      </c>
+      <c r="AV8" t="n">
+        <v>0.1056360535018922</v>
+      </c>
+      <c r="AW8" t="n">
+        <v>0.04636027131031541</v>
+      </c>
+      <c r="AX8" t="n">
+        <v>0.0118662323350654</v>
+      </c>
+      <c r="AY8" t="n">
+        <v>0.0118662323350654</v>
+      </c>
+      <c r="AZ8" t="n">
+        <v>0.006773128912413095</v>
+      </c>
+      <c r="BA8" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BB8" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BC8" t="n">
+        <v>0.01839360807030513</v>
+      </c>
+      <c r="BD8" t="n">
+        <v>0.01846508000904991</v>
+      </c>
+      <c r="BE8" t="n">
+        <v>0.01837298988249244</v>
+      </c>
+      <c r="BF8" t="n">
+        <v>0.01901854625879056</v>
+      </c>
+      <c r="BG8" t="n">
+        <v>0.01941974906607245</v>
+      </c>
+      <c r="BH8" t="n">
+        <v>0.01440607396522165</v>
+      </c>
+      <c r="BI8" t="n">
+        <v>0.01402388498748666</v>
+      </c>
+      <c r="BJ8" t="n">
+        <v>0.01697768968272208</v>
+      </c>
+      <c r="BK8" t="n">
+        <v>0.0124320084368951</v>
+      </c>
+      <c r="BL8" t="n">
         <v>0.0625</v>
       </c>
-      <c r="AS8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT8" t="n">
+      <c r="BM8" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN8" t="n">
         <v>0.5294117647058824</v>
       </c>
-      <c r="AU8" t="n">
+      <c r="BO8" t="n">
         <v>0.7285714285714289</v>
       </c>
-      <c r="AV8" t="n">
+      <c r="BP8" t="n">
         <v>0.6074474789915967</v>
       </c>
-      <c r="AW8" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX8" t="n">
+      <c r="BQ8" t="n">
+        <v>1</v>
+      </c>
+      <c r="BR8" t="n">
         <v>4</v>
       </c>
-      <c r="AY8" t="n">
+      <c r="BS8" t="n">
         <v>7</v>
       </c>
-      <c r="AZ8" t="n">
+      <c r="BT8" t="n">
         <v>6</v>
       </c>
-      <c r="BA8" t="n">
+      <c r="BU8" t="n">
         <v>7</v>
       </c>
     </row>
@@ -1867,7 +2387,7 @@
         <v>0.1161415668829011</v>
       </c>
       <c r="J9" t="n">
-        <v>0.04447160388952821</v>
+        <v>0.04386488727486224</v>
       </c>
       <c r="K9" t="n">
         <v>1</v>
@@ -1879,13 +2399,13 @@
         <v>0.7938630683822473</v>
       </c>
       <c r="N9" t="n">
-        <v>0.9074186800851527</v>
+        <v>0.9086396166946782</v>
       </c>
       <c r="O9" t="n">
-        <v>0.9076270133089607</v>
+        <v>0.9088096621213055</v>
       </c>
       <c r="P9" t="n">
-        <v>0.8927633936894899</v>
+        <v>0.8925639074385167</v>
       </c>
       <c r="Q9" t="n">
         <v>0.9571225219101468</v>
@@ -1903,7 +2423,7 @@
         <v>0.6237069803983596</v>
       </c>
       <c r="V9" t="n">
-        <v>0.5409231120292544</v>
+        <v>0.5355421753834159</v>
       </c>
       <c r="W9" t="n">
         <v>8</v>
@@ -1966,36 +2486,96 @@
         <v>10</v>
       </c>
       <c r="AQ9" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="AR9" t="n">
+        <v>0.0435438893438649</v>
+      </c>
+      <c r="AS9" t="n">
+        <v>0.06566702283119129</v>
+      </c>
+      <c r="AT9" t="n">
+        <v>0.0249288045795638</v>
+      </c>
+      <c r="AU9" t="n">
+        <v>0.09222797690608517</v>
+      </c>
+      <c r="AV9" t="n">
+        <v>0.06066237804805339</v>
+      </c>
+      <c r="AW9" t="n">
+        <v>0.04659615132418544</v>
+      </c>
+      <c r="AX9" t="n">
+        <v>0.005774294409285235</v>
+      </c>
+      <c r="AY9" t="n">
+        <v>0.003484247006487034</v>
+      </c>
+      <c r="AZ9" t="n">
+        <v>0.004386488727486224</v>
+      </c>
+      <c r="BA9" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BB9" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BC9" t="n">
+        <v>0.01587726136764495</v>
+      </c>
+      <c r="BD9" t="n">
+        <v>0.01817279233389357</v>
+      </c>
+      <c r="BE9" t="n">
+        <v>0.01817619324242611</v>
+      </c>
+      <c r="BF9" t="n">
+        <v>0.01785127814877033</v>
+      </c>
+      <c r="BG9" t="n">
+        <v>0.01914245043820294</v>
+      </c>
+      <c r="BH9" t="n">
+        <v>0.01437178545187362</v>
+      </c>
+      <c r="BI9" t="n">
+        <v>0.01808829923420046</v>
+      </c>
+      <c r="BJ9" t="n">
+        <v>0.01411672238223425</v>
+      </c>
+      <c r="BK9" t="n">
+        <v>0.01247413960796719</v>
+      </c>
+      <c r="BL9" t="n">
         <v>0.0625</v>
       </c>
-      <c r="AS9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT9" t="n">
+      <c r="BM9" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN9" t="n">
         <v>0.3529411764705883</v>
       </c>
-      <c r="AU9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AV9" t="n">
+      <c r="BO9" t="n">
+        <v>1</v>
+      </c>
+      <c r="BP9" t="n">
         <v>0.6216911764705882</v>
       </c>
-      <c r="AW9" t="n">
+      <c r="BQ9" t="n">
         <v>2</v>
       </c>
-      <c r="AX9" t="n">
-        <v>11</v>
-      </c>
-      <c r="AY9" t="n">
+      <c r="BR9" t="n">
+        <v>9</v>
+      </c>
+      <c r="BS9" t="n">
         <v>5</v>
       </c>
-      <c r="AZ9" t="n">
-        <v>6</v>
-      </c>
-      <c r="BA9" t="n">
+      <c r="BT9" t="n">
+        <v>5.333333333333333</v>
+      </c>
+      <c r="BU9" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2030,7 +2610,7 @@
         <v>0.2340465978070756</v>
       </c>
       <c r="J10" t="n">
-        <v>0.06736471109930955</v>
+        <v>0.06588726112203129</v>
       </c>
       <c r="K10" t="n">
         <v>1</v>
@@ -2042,13 +2622,13 @@
         <v>0</v>
       </c>
       <c r="N10" t="n">
-        <v>0.9176842936124422</v>
+        <v>0.9195056912923397</v>
       </c>
       <c r="O10" t="n">
-        <v>0.9319908288785386</v>
+        <v>0.9334868991119403</v>
       </c>
       <c r="P10" t="n">
-        <v>0.9791519174402843</v>
+        <v>0.9792990287312365</v>
       </c>
       <c r="Q10" t="n">
         <v>0.9329776326660628</v>
@@ -2066,7 +2646,7 @@
         <v>0.7017074223857528</v>
       </c>
       <c r="V10" t="n">
-        <v>0.4758176382354872</v>
+        <v>0.4524330770626401</v>
       </c>
       <c r="W10" t="n">
         <v>6</v>
@@ -2129,36 +2709,96 @@
         <v>6</v>
       </c>
       <c r="AQ10" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="AR10" t="n">
-        <v>0</v>
+        <v>0.04554569998424451</v>
       </c>
       <c r="AS10" t="n">
+        <v>0.06323667563460718</v>
+      </c>
+      <c r="AT10" t="n">
+        <v>0.02476826127506105</v>
+      </c>
+      <c r="AU10" t="n">
+        <v>0.03206722614956286</v>
+      </c>
+      <c r="AV10" t="n">
+        <v>0.05414192751201342</v>
+      </c>
+      <c r="AW10" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="AX10" t="n">
+        <v>0.01034162766832872</v>
+      </c>
+      <c r="AY10" t="n">
+        <v>0.007021397934212269</v>
+      </c>
+      <c r="AZ10" t="n">
+        <v>0.006588726112203129</v>
+      </c>
+      <c r="BA10" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BB10" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BC10" t="n">
+        <v>0</v>
+      </c>
+      <c r="BD10" t="n">
+        <v>0.01839011382584679</v>
+      </c>
+      <c r="BE10" t="n">
+        <v>0.01866973798223881</v>
+      </c>
+      <c r="BF10" t="n">
+        <v>0.01958598057462473</v>
+      </c>
+      <c r="BG10" t="n">
+        <v>0.01865955265332126</v>
+      </c>
+      <c r="BH10" t="n">
+        <v>0.01110457996571148</v>
+      </c>
+      <c r="BI10" t="n">
+        <v>0.009128584387275486</v>
+      </c>
+      <c r="BJ10" t="n">
+        <v>0.009148836955673345</v>
+      </c>
+      <c r="BK10" t="n">
+        <v>0.01403414844771506</v>
+      </c>
+      <c r="BL10" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM10" t="n">
         <v>0.5</v>
       </c>
-      <c r="AT10" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU10" t="n">
+      <c r="BN10" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO10" t="n">
         <v>0.5000000000000003</v>
       </c>
-      <c r="AV10" t="n">
+      <c r="BP10" t="n">
         <v>0.425</v>
       </c>
-      <c r="AW10" t="n">
+      <c r="BQ10" t="n">
         <v>2</v>
       </c>
-      <c r="AX10" t="n">
-        <v>16</v>
-      </c>
-      <c r="AY10" t="n">
+      <c r="BR10" t="n">
+        <v>19</v>
+      </c>
+      <c r="BS10" t="n">
         <v>14</v>
       </c>
-      <c r="AZ10" t="n">
-        <v>10.66666666666667</v>
-      </c>
-      <c r="BA10" t="n">
+      <c r="BT10" t="n">
+        <v>11.66666666666667</v>
+      </c>
+      <c r="BU10" t="n">
         <v>2</v>
       </c>
     </row>
@@ -2193,7 +2833,7 @@
         <v>0.7077020179114577</v>
       </c>
       <c r="J11" t="n">
-        <v>0.2209068918986902</v>
+        <v>0.2113121860790065</v>
       </c>
       <c r="K11" t="n">
         <v>1</v>
@@ -2205,13 +2845,13 @@
         <v>0.6595074671311945</v>
       </c>
       <c r="N11" t="n">
-        <v>0.8168732644529859</v>
+        <v>0.8250084760791984</v>
       </c>
       <c r="O11" t="n">
-        <v>0.7028571306857105</v>
+        <v>0.7161331333534163</v>
       </c>
       <c r="P11" t="n">
-        <v>0.887587297793518</v>
+        <v>0.8910050252129752</v>
       </c>
       <c r="Q11" t="n">
         <v>0.7729009560403463</v>
@@ -2229,7 +2869,7 @@
         <v>0.4230353159231006</v>
       </c>
       <c r="V11" t="n">
-        <v>0.6142198864280667</v>
+        <v>0.5818907369687332</v>
       </c>
       <c r="W11" t="n">
         <v>9</v>
@@ -2292,36 +2932,96 @@
         <v>22</v>
       </c>
       <c r="AQ11" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AR11" t="n">
+        <v>0.04207889839641019</v>
+      </c>
+      <c r="AS11" t="n">
+        <v>0.06577444536756032</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>0.02436105602096817</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>0.06217477633972501</v>
+      </c>
+      <c r="AV11" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="AW11" t="n">
+        <v>0.04978448603998552</v>
+      </c>
+      <c r="AX11" t="n">
+        <v>0.02123106053734373</v>
+      </c>
+      <c r="AY11" t="n">
+        <v>0.02123106053734373</v>
+      </c>
+      <c r="AZ11" t="n">
+        <v>0.02113121860790065</v>
+      </c>
+      <c r="BA11" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BB11" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BC11" t="n">
+        <v>0.01319014934262389</v>
+      </c>
+      <c r="BD11" t="n">
+        <v>0.01650016952158397</v>
+      </c>
+      <c r="BE11" t="n">
+        <v>0.01432266266706833</v>
+      </c>
+      <c r="BF11" t="n">
+        <v>0.0178201005042595</v>
+      </c>
+      <c r="BG11" t="n">
+        <v>0.01545801912080693</v>
+      </c>
+      <c r="BH11" t="n">
+        <v>0</v>
+      </c>
+      <c r="BI11" t="n">
+        <v>0.0151790469753579</v>
+      </c>
+      <c r="BJ11" t="n">
+        <v>0.003192880671333288</v>
+      </c>
+      <c r="BK11" t="n">
+        <v>0.008460706318462012</v>
+      </c>
+      <c r="BL11" t="n">
         <v>0.0625</v>
       </c>
-      <c r="AS11" t="n">
+      <c r="BM11" t="n">
         <v>0.5</v>
       </c>
-      <c r="AT11" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU11" t="n">
+      <c r="BN11" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO11" t="n">
         <v>0.5714285714285715</v>
       </c>
-      <c r="AV11" t="n">
+      <c r="BP11" t="n">
         <v>0.3044642857142857</v>
       </c>
-      <c r="AW11" t="n">
+      <c r="BQ11" t="n">
         <v>-1</v>
       </c>
-      <c r="AX11" t="n">
-        <v>3</v>
-      </c>
-      <c r="AY11" t="n">
+      <c r="BR11" t="n">
+        <v>6</v>
+      </c>
+      <c r="BS11" t="n">
         <v>18</v>
       </c>
-      <c r="AZ11" t="n">
-        <v>12.16666666666667</v>
-      </c>
-      <c r="BA11" t="n">
+      <c r="BT11" t="n">
+        <v>13.16666666666667</v>
+      </c>
+      <c r="BU11" t="n">
         <v>15.5</v>
       </c>
     </row>
@@ -2356,7 +3056,7 @@
         <v>1</v>
       </c>
       <c r="J12" t="n">
-        <v>0.0006882295048204959</v>
+        <v>0.0006779517030470306</v>
       </c>
       <c r="K12" t="n">
         <v>1</v>
@@ -2368,13 +3068,13 @@
         <v>0.8120016640737541</v>
       </c>
       <c r="N12" t="n">
-        <v>0.9512560223083806</v>
+        <v>0.9519264594580706</v>
       </c>
       <c r="O12" t="n">
-        <v>0.9608223419004499</v>
+        <v>0.9613229311699134</v>
       </c>
       <c r="P12" t="n">
-        <v>0.9886857288235849</v>
+        <v>0.9886481756773893</v>
       </c>
       <c r="Q12" t="n">
         <v>0.9954210175295394</v>
@@ -2392,7 +3092,7 @@
         <v>0.17159458458555</v>
       </c>
       <c r="V12" t="n">
-        <v>0.5446194726090305</v>
+        <v>0.4986425362738459</v>
       </c>
       <c r="W12" t="n">
         <v>14</v>
@@ -2455,36 +3155,96 @@
         <v>24</v>
       </c>
       <c r="AQ12" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="AR12" t="n">
-        <v>0</v>
+        <v>0.03832931658375547</v>
       </c>
       <c r="AS12" t="n">
+        <v>0.06556831259886295</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU12" t="n">
+        <v>0.1051455211177612</v>
+      </c>
+      <c r="AV12" t="n">
+        <v>0.03135760394478571</v>
+      </c>
+      <c r="AW12" t="n">
+        <v>0.02977175512348357</v>
+      </c>
+      <c r="AX12" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AY12" t="n">
+        <v>0.03</v>
+      </c>
+      <c r="AZ12" t="n">
+        <v>6.779517030470306e-05</v>
+      </c>
+      <c r="BA12" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BB12" t="n">
+        <v>0.01333333333333333</v>
+      </c>
+      <c r="BC12" t="n">
+        <v>0.01624003328147508</v>
+      </c>
+      <c r="BD12" t="n">
+        <v>0.01903852918916141</v>
+      </c>
+      <c r="BE12" t="n">
+        <v>0.01922645862339827</v>
+      </c>
+      <c r="BF12" t="n">
+        <v>0.01977296351354779</v>
+      </c>
+      <c r="BG12" t="n">
+        <v>0.01990842035059079</v>
+      </c>
+      <c r="BH12" t="n">
+        <v>0.01495958853783982</v>
+      </c>
+      <c r="BI12" t="n">
+        <v>0.01753112857401615</v>
+      </c>
+      <c r="BJ12" t="n">
+        <v>0.004959884639818518</v>
+      </c>
+      <c r="BK12" t="n">
+        <v>0.003431891691711</v>
+      </c>
+      <c r="BL12" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM12" t="n">
         <v>0.5</v>
       </c>
-      <c r="AT12" t="n">
+      <c r="BN12" t="n">
         <v>0.3529411764705883</v>
       </c>
-      <c r="AU12" t="n">
+      <c r="BO12" t="n">
         <v>0.3214285714285713</v>
       </c>
-      <c r="AV12" t="n">
+      <c r="BP12" t="n">
         <v>0.3011554621848739</v>
       </c>
-      <c r="AW12" t="n">
+      <c r="BQ12" t="n">
         <v>-2</v>
       </c>
-      <c r="AX12" t="n">
-        <v>8</v>
-      </c>
-      <c r="AY12" t="n">
+      <c r="BR12" t="n">
+        <v>13</v>
+      </c>
+      <c r="BS12" t="n">
         <v>19</v>
       </c>
-      <c r="AZ12" t="n">
-        <v>16.16666666666667</v>
-      </c>
-      <c r="BA12" t="n">
+      <c r="BT12" t="n">
+        <v>17.83333333333333</v>
+      </c>
+      <c r="BU12" t="n">
         <v>21.5</v>
       </c>
     </row>
@@ -2519,7 +3279,7 @@
         <v>0.2594242832236522</v>
       </c>
       <c r="J13" t="n">
-        <v>1.28520998289116e-05</v>
+        <v>1.365039350338893e-05</v>
       </c>
       <c r="K13" t="n">
         <v>1</v>
@@ -2531,13 +3291,13 @@
         <v>0.8215622133329979</v>
       </c>
       <c r="N13" t="n">
-        <v>0.9503545355619496</v>
+        <v>0.9509383873501193</v>
       </c>
       <c r="O13" t="n">
-        <v>0.9679968082021196</v>
+        <v>0.9683277090261213</v>
       </c>
       <c r="P13" t="n">
-        <v>0.9900254640860363</v>
+        <v>0.9899649466584611</v>
       </c>
       <c r="Q13" t="n">
         <v>0.9994496688769975</v>
@@ -2555,7 +3315,7 @@
         <v>0.1289325404988002</v>
       </c>
       <c r="V13" t="n">
-        <v>0.3498445995934407</v>
+        <v>0.3556489578029118</v>
       </c>
       <c r="W13" t="n">
         <v>24</v>
@@ -2621,33 +3381,93 @@
         <v>25</v>
       </c>
       <c r="AR13" t="n">
+        <v>0.01436588277152099</v>
+      </c>
+      <c r="AS13" t="n">
+        <v>0.0642205252221756</v>
+      </c>
+      <c r="AT13" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU13" t="n">
+        <v>0.08045259070299637</v>
+      </c>
+      <c r="AV13" t="n">
+        <v>0.01744413837889404</v>
+      </c>
+      <c r="AW13" t="n">
+        <v>0.006210329304755579</v>
+      </c>
+      <c r="AX13" t="n">
+        <v>0.007782728496709567</v>
+      </c>
+      <c r="AY13" t="n">
+        <v>0.007782728496709567</v>
+      </c>
+      <c r="AZ13" t="n">
+        <v>1.365039350338893e-06</v>
+      </c>
+      <c r="BA13" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BB13" t="n">
+        <v>0.006666666666666666</v>
+      </c>
+      <c r="BC13" t="n">
+        <v>0.01643124426665996</v>
+      </c>
+      <c r="BD13" t="n">
+        <v>0.01901876774700239</v>
+      </c>
+      <c r="BE13" t="n">
+        <v>0.01936655418052243</v>
+      </c>
+      <c r="BF13" t="n">
+        <v>0.01979929893316922</v>
+      </c>
+      <c r="BG13" t="n">
+        <v>0.01998899337753995</v>
+      </c>
+      <c r="BH13" t="n">
+        <v>0.01362233651726671</v>
+      </c>
+      <c r="BI13" t="n">
+        <v>0.01415207345036295</v>
+      </c>
+      <c r="BJ13" t="n">
+        <v>0.005764083440633423</v>
+      </c>
+      <c r="BK13" t="n">
+        <v>0.002578650809976005</v>
+      </c>
+      <c r="BL13" t="n">
         <v>0.0625</v>
       </c>
-      <c r="AS13" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT13" t="n">
+      <c r="BM13" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN13" t="n">
         <v>0.9411764705882353</v>
       </c>
-      <c r="AU13" t="n">
+      <c r="BO13" t="n">
         <v>0.5428571428571429</v>
       </c>
-      <c r="AV13" t="n">
+      <c r="BP13" t="n">
         <v>0.2413550420168067</v>
       </c>
-      <c r="AW13" t="n">
+      <c r="BQ13" t="n">
         <v>-2</v>
       </c>
-      <c r="AX13" t="n">
+      <c r="BR13" t="n">
         <v>25</v>
       </c>
-      <c r="AY13" t="n">
+      <c r="BS13" t="n">
         <v>24</v>
       </c>
-      <c r="AZ13" t="n">
+      <c r="BT13" t="n">
         <v>23.5</v>
       </c>
-      <c r="BA13" t="n">
+      <c r="BU13" t="n">
         <v>21.5</v>
       </c>
     </row>
@@ -2682,7 +3502,7 @@
         <v>0.168225447545836</v>
       </c>
       <c r="J14" t="n">
-        <v>0.04009860023623095</v>
+        <v>0.03904987923984332</v>
       </c>
       <c r="K14" t="n">
         <v>1</v>
@@ -2694,13 +3514,13 @@
         <v>0.7088068119168219</v>
       </c>
       <c r="N14" t="n">
-        <v>0.9184448643899391</v>
+        <v>0.9207666479717697</v>
       </c>
       <c r="O14" t="n">
-        <v>0.9201053320014679</v>
+        <v>0.9223920087155701</v>
       </c>
       <c r="P14" t="n">
-        <v>0.9504446116931717</v>
+        <v>0.9511367057108948</v>
       </c>
       <c r="Q14" t="n">
         <v>0.8576434167172677</v>
@@ -2718,7 +3538,7 @@
         <v>0.6504105872916137</v>
       </c>
       <c r="V14" t="n">
-        <v>0.5441011829414165</v>
+        <v>0.5486817437165438</v>
       </c>
       <c r="W14" t="n">
         <v>10</v>
@@ -2763,7 +3583,7 @@
         <v>17</v>
       </c>
       <c r="AK14" t="n">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="AL14" t="n">
         <v>23</v>
@@ -2781,36 +3601,96 @@
         <v>7</v>
       </c>
       <c r="AQ14" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AR14" t="n">
+        <v>0.04196862047152693</v>
+      </c>
+      <c r="AS14" t="n">
+        <v>0.06651180893482952</v>
+      </c>
+      <c r="AT14" t="n">
+        <v>0.02546132167701084</v>
+      </c>
+      <c r="AU14" t="n">
+        <v>0.06813227917821395</v>
+      </c>
+      <c r="AV14" t="n">
+        <v>0.1034011886511527</v>
+      </c>
+      <c r="AW14" t="n">
+        <v>0.04528171363259264</v>
+      </c>
+      <c r="AX14" t="n">
+        <v>0.00504676342637508</v>
+      </c>
+      <c r="AY14" t="n">
+        <v>0.00504676342637508</v>
+      </c>
+      <c r="AZ14" t="n">
+        <v>0.003904987923984332</v>
+      </c>
+      <c r="BA14" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BB14" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BC14" t="n">
+        <v>0.01417613623833644</v>
+      </c>
+      <c r="BD14" t="n">
+        <v>0.0184153329594354</v>
+      </c>
+      <c r="BE14" t="n">
+        <v>0.0184478401743114</v>
+      </c>
+      <c r="BF14" t="n">
+        <v>0.0190227341142179</v>
+      </c>
+      <c r="BG14" t="n">
+        <v>0.01715286833434536</v>
+      </c>
+      <c r="BH14" t="n">
+        <v>0.01431790350232672</v>
+      </c>
+      <c r="BI14" t="n">
+        <v>0.016259052014484</v>
+      </c>
+      <c r="BJ14" t="n">
+        <v>0.01312621731119332</v>
+      </c>
+      <c r="BK14" t="n">
+        <v>0.01300821174583227</v>
+      </c>
+      <c r="BL14" t="n">
         <v>0.3125</v>
       </c>
-      <c r="AS14" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT14" t="n">
+      <c r="BM14" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN14" t="n">
         <v>0.4705882352941176</v>
       </c>
-      <c r="AU14" t="n">
+      <c r="BO14" t="n">
         <v>0.8428571428571433</v>
       </c>
-      <c r="AV14" t="n">
+      <c r="BP14" t="n">
         <v>0.6907668067226891</v>
       </c>
-      <c r="AW14" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX14" t="n">
-        <v>9</v>
-      </c>
-      <c r="AY14" t="n">
+      <c r="BQ14" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR14" t="n">
+        <v>8</v>
+      </c>
+      <c r="BS14" t="n">
         <v>4</v>
       </c>
-      <c r="AZ14" t="n">
-        <v>8.5</v>
-      </c>
-      <c r="BA14" t="n">
+      <c r="BT14" t="n">
+        <v>8.166666666666666</v>
+      </c>
+      <c r="BU14" t="n">
         <v>12.5</v>
       </c>
     </row>
@@ -2845,7 +3725,7 @@
         <v>0.2777858404522399</v>
       </c>
       <c r="J15" t="n">
-        <v>0.01876346839951029</v>
+        <v>0.01834502080384879</v>
       </c>
       <c r="K15" t="n">
         <v>1</v>
@@ -2857,13 +3737,13 @@
         <v>0.7090368766685574</v>
       </c>
       <c r="N15" t="n">
-        <v>0.9195298945720963</v>
+        <v>0.9218417896824113</v>
       </c>
       <c r="O15" t="n">
-        <v>0.9849706967185791</v>
+        <v>0.9854131257221024</v>
       </c>
       <c r="P15" t="n">
-        <v>0.9965563787170277</v>
+        <v>0.9966112405889642</v>
       </c>
       <c r="Q15" t="n">
         <v>0.9978697777202641</v>
@@ -2881,7 +3761,7 @@
         <v>0.6446802713177632</v>
       </c>
       <c r="V15" t="n">
-        <v>0.594135690571257</v>
+        <v>0.605997915503954</v>
       </c>
       <c r="W15" t="n">
         <v>3</v>
@@ -2944,36 +3824,96 @@
         <v>8</v>
       </c>
       <c r="AQ15" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AR15" t="n">
+        <v>0.05504236497463445</v>
+      </c>
+      <c r="AS15" t="n">
+        <v>0.06664355458255899</v>
+      </c>
+      <c r="AT15" t="n">
+        <v>0.02621370308211918</v>
+      </c>
+      <c r="AU15" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="AV15" t="n">
+        <v>0.06935045542134152</v>
+      </c>
+      <c r="AW15" t="n">
+        <v>0.04670693067390178</v>
+      </c>
+      <c r="AX15" t="n">
+        <v>0.009260982720331002</v>
+      </c>
+      <c r="AY15" t="n">
+        <v>0.008333575213567196</v>
+      </c>
+      <c r="AZ15" t="n">
+        <v>0.001834502080384879</v>
+      </c>
+      <c r="BA15" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BB15" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BC15" t="n">
+        <v>0.01418073753337115</v>
+      </c>
+      <c r="BD15" t="n">
+        <v>0.01843683579364823</v>
+      </c>
+      <c r="BE15" t="n">
+        <v>0.01970826251444205</v>
+      </c>
+      <c r="BF15" t="n">
+        <v>0.01993222481177928</v>
+      </c>
+      <c r="BG15" t="n">
+        <v>0.01995739555440528</v>
+      </c>
+      <c r="BH15" t="n">
+        <v>0.01461670340435954</v>
+      </c>
+      <c r="BI15" t="n">
+        <v>0.01638361346519768</v>
+      </c>
+      <c r="BJ15" t="n">
+        <v>0.01650246825155659</v>
+      </c>
+      <c r="BK15" t="n">
+        <v>0.01289360542635526</v>
+      </c>
+      <c r="BL15" t="n">
         <v>0.0625</v>
       </c>
-      <c r="AS15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT15" t="n">
+      <c r="BM15" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN15" t="n">
         <v>0.4705882352941176</v>
       </c>
-      <c r="AU15" t="n">
+      <c r="BO15" t="n">
         <v>0.4071428571428572</v>
       </c>
-      <c r="AV15" t="n">
+      <c r="BP15" t="n">
         <v>0.5504096638655462</v>
       </c>
-      <c r="AW15" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX15" t="n">
-        <v>5</v>
-      </c>
-      <c r="AY15" t="n">
+      <c r="BQ15" t="n">
+        <v>1</v>
+      </c>
+      <c r="BR15" t="n">
+        <v>3</v>
+      </c>
+      <c r="BS15" t="n">
         <v>9</v>
       </c>
-      <c r="AZ15" t="n">
-        <v>7</v>
-      </c>
-      <c r="BA15" t="n">
+      <c r="BT15" t="n">
+        <v>6.333333333333333</v>
+      </c>
+      <c r="BU15" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3008,7 +3948,7 @@
         <v>0.3476274261166677</v>
       </c>
       <c r="J16" t="n">
-        <v>0.05246930830778347</v>
+        <v>0.05093344298721163</v>
       </c>
       <c r="K16" t="n">
         <v>1</v>
@@ -3020,13 +3960,13 @@
         <v>0.7626709868266816</v>
       </c>
       <c r="N16" t="n">
-        <v>0.8682386314501559</v>
+        <v>0.8725029897966433</v>
       </c>
       <c r="O16" t="n">
-        <v>0.9021391654960228</v>
+        <v>0.9053336666766214</v>
       </c>
       <c r="P16" t="n">
-        <v>0.8751078106354089</v>
+        <v>0.8773467980136157</v>
       </c>
       <c r="Q16" t="n">
         <v>0.9464770986884486</v>
@@ -3044,7 +3984,7 @@
         <v>0.5806708131265779</v>
       </c>
       <c r="V16" t="n">
-        <v>0.5413974289029981</v>
+        <v>0.5176056611539661</v>
       </c>
       <c r="W16" t="n">
         <v>7</v>
@@ -3107,36 +4047,96 @@
         <v>15</v>
       </c>
       <c r="AQ16" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AR16" t="n">
-        <v>1</v>
+        <v>0.04532111321124094</v>
       </c>
       <c r="AS16" t="n">
-        <v>1</v>
+        <v>0.0665254671636779</v>
       </c>
       <c r="AT16" t="n">
+        <v>0.02549440769190068</v>
+      </c>
+      <c r="AU16" t="n">
+        <v>0.07426569931051159</v>
+      </c>
+      <c r="AV16" t="n">
+        <v>0.05802378165358008</v>
+      </c>
+      <c r="AW16" t="n">
+        <v>0.03561067251491418</v>
+      </c>
+      <c r="AX16" t="n">
+        <v>0.01350582102303449</v>
+      </c>
+      <c r="AY16" t="n">
+        <v>0.01042882278350003</v>
+      </c>
+      <c r="AZ16" t="n">
+        <v>0.005093344298721164</v>
+      </c>
+      <c r="BA16" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BB16" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BC16" t="n">
+        <v>0.01525341973653363</v>
+      </c>
+      <c r="BD16" t="n">
+        <v>0.01745005979593287</v>
+      </c>
+      <c r="BE16" t="n">
+        <v>0.01810667333353243</v>
+      </c>
+      <c r="BF16" t="n">
+        <v>0.01754693596027232</v>
+      </c>
+      <c r="BG16" t="n">
+        <v>0.01892954197376897</v>
+      </c>
+      <c r="BH16" t="n">
+        <v>0.01706588292921871</v>
+      </c>
+      <c r="BI16" t="n">
+        <v>0.01615185724020125</v>
+      </c>
+      <c r="BJ16" t="n">
+        <v>0.01121874427089335</v>
+      </c>
+      <c r="BK16" t="n">
+        <v>0.01161341626253156</v>
+      </c>
+      <c r="BL16" t="n">
+        <v>1</v>
+      </c>
+      <c r="BM16" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN16" t="n">
         <v>0.1764705882352941</v>
       </c>
-      <c r="AU16" t="n">
-        <v>0.7214285714285715</v>
-      </c>
-      <c r="AV16" t="n">
-        <v>0.8346848739495798</v>
-      </c>
-      <c r="AW16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX16" t="n">
-        <v>10</v>
-      </c>
-      <c r="AY16" t="n">
-        <v>1</v>
-      </c>
-      <c r="AZ16" t="n">
-        <v>6</v>
-      </c>
-      <c r="BA16" t="n">
+      <c r="BO16" t="n">
+        <v>0.7214285714285719</v>
+      </c>
+      <c r="BP16" t="n">
+        <v>0.8346848739495799</v>
+      </c>
+      <c r="BQ16" t="n">
+        <v>1</v>
+      </c>
+      <c r="BR16" t="n">
+        <v>11</v>
+      </c>
+      <c r="BS16" t="n">
+        <v>1</v>
+      </c>
+      <c r="BT16" t="n">
+        <v>6.333333333333333</v>
+      </c>
+      <c r="BU16" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3189,7 +4189,7 @@
         <v>0</v>
       </c>
       <c r="P17" t="n">
-        <v>0.624896046892191</v>
+        <v>0.6192162929935138</v>
       </c>
       <c r="Q17" t="n">
         <v>0</v>
@@ -3207,7 +4207,7 @@
         <v>0.8343317255711132</v>
       </c>
       <c r="V17" t="n">
-        <v>0.661047248771656</v>
+        <v>0.6228118430490143</v>
       </c>
       <c r="W17" t="n">
         <v>2</v>
@@ -3273,33 +4273,93 @@
         <v>2</v>
       </c>
       <c r="AR17" t="n">
+        <v>0.05628430977072028</v>
+      </c>
+      <c r="AS17" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="AT17" t="n">
+        <v>0.02631471297743343</v>
+      </c>
+      <c r="AU17" t="n">
+        <v>0.02317082536050662</v>
+      </c>
+      <c r="AV17" t="n">
+        <v>0.1049521039026069</v>
+      </c>
+      <c r="AW17" t="n">
+        <v>0.04985155669212864</v>
+      </c>
+      <c r="AX17" t="n">
+        <v>0.02443048377950117</v>
+      </c>
+      <c r="AY17" t="n">
+        <v>0.02443048377950117</v>
+      </c>
+      <c r="AZ17" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="BA17" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB17" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BC17" t="n">
+        <v>0.007003975210013331</v>
+      </c>
+      <c r="BD17" t="n">
+        <v>0</v>
+      </c>
+      <c r="BE17" t="n">
+        <v>0</v>
+      </c>
+      <c r="BF17" t="n">
+        <v>0.01238432585987028</v>
+      </c>
+      <c r="BG17" t="n">
+        <v>0</v>
+      </c>
+      <c r="BH17" t="n">
+        <v>0.007793289248101885</v>
+      </c>
+      <c r="BI17" t="n">
+        <v>0.002148310143634222</v>
+      </c>
+      <c r="BJ17" t="n">
+        <v>0.01736083181357407</v>
+      </c>
+      <c r="BK17" t="n">
+        <v>0.01668663451142226</v>
+      </c>
+      <c r="BL17" t="n">
         <v>0.0625</v>
       </c>
-      <c r="AS17" t="n">
+      <c r="BM17" t="n">
         <v>0.5</v>
       </c>
-      <c r="AT17" t="n">
+      <c r="BN17" t="n">
         <v>0.2352941176470588</v>
       </c>
-      <c r="AU17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AV17" t="n">
+      <c r="BO17" t="n">
+        <v>0</v>
+      </c>
+      <c r="BP17" t="n">
         <v>0.2540441176470588</v>
       </c>
-      <c r="AW17" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX17" t="n">
+      <c r="BQ17" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR17" t="n">
         <v>2</v>
       </c>
-      <c r="AY17" t="n">
+      <c r="BS17" t="n">
         <v>23</v>
       </c>
-      <c r="AZ17" t="n">
+      <c r="BT17" t="n">
         <v>12.5</v>
       </c>
-      <c r="BA17" t="n">
+      <c r="BU17" t="n">
         <v>12.5</v>
       </c>
     </row>
@@ -3334,7 +4394,7 @@
         <v>0.1016047579937056</v>
       </c>
       <c r="J18" t="n">
-        <v>0.03555299818989589</v>
+        <v>0.03410880900291786</v>
       </c>
       <c r="K18" t="n">
         <v>1</v>
@@ -3346,13 +4406,13 @@
         <v>0.8331101702454101</v>
       </c>
       <c r="N18" t="n">
-        <v>0.9145602064012045</v>
+        <v>0.9184146219953763</v>
       </c>
       <c r="O18" t="n">
-        <v>0.9022723472722985</v>
+        <v>0.906746479773536</v>
       </c>
       <c r="P18" t="n">
-        <v>0.8108944863018862</v>
+        <v>0.8167399307629344</v>
       </c>
       <c r="Q18" t="n">
         <v>0.9595257766850158</v>
@@ -3370,7 +4430,7 @@
         <v>0.4913492956542896</v>
       </c>
       <c r="V18" t="n">
-        <v>0.4738373711411129</v>
+        <v>0.5073032374895393</v>
       </c>
       <c r="W18" t="n">
         <v>5</v>
@@ -3409,7 +4469,7 @@
         <v>7</v>
       </c>
       <c r="AI18" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AJ18" t="n">
         <v>20</v>
@@ -3433,36 +4493,96 @@
         <v>21</v>
       </c>
       <c r="AQ18" t="n">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="AR18" t="n">
+        <v>0.04638977963140882</v>
+      </c>
+      <c r="AS18" t="n">
+        <v>0.06671111937116542</v>
+      </c>
+      <c r="AT18" t="n">
+        <v>0.02356312066167563</v>
+      </c>
+      <c r="AU18" t="n">
+        <v>0.07306234562375312</v>
+      </c>
+      <c r="AV18" t="n">
+        <v>0.1038701358826898</v>
+      </c>
+      <c r="AW18" t="n">
+        <v>0.01312452562577003</v>
+      </c>
+      <c r="AX18" t="n">
+        <v>0.004175696134114059</v>
+      </c>
+      <c r="AY18" t="n">
+        <v>0.00304814273981117</v>
+      </c>
+      <c r="AZ18" t="n">
+        <v>0.003410880900291787</v>
+      </c>
+      <c r="BA18" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BB18" t="n">
+        <v>0.01333333333333333</v>
+      </c>
+      <c r="BC18" t="n">
+        <v>0.0166622034049082</v>
+      </c>
+      <c r="BD18" t="n">
+        <v>0.01836829243990752</v>
+      </c>
+      <c r="BE18" t="n">
+        <v>0.01813492959547072</v>
+      </c>
+      <c r="BF18" t="n">
+        <v>0.01633479861525869</v>
+      </c>
+      <c r="BG18" t="n">
+        <v>0.01919051553370032</v>
+      </c>
+      <c r="BH18" t="n">
+        <v>0.0182120989468528</v>
+      </c>
+      <c r="BI18" t="n">
+        <v>0.01468507045258687</v>
+      </c>
+      <c r="BJ18" t="n">
+        <v>0.005199262683755224</v>
+      </c>
+      <c r="BK18" t="n">
+        <v>0.009826985913085793</v>
+      </c>
+      <c r="BL18" t="n">
         <v>0.0625</v>
       </c>
-      <c r="AS18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AT18" t="n">
+      <c r="BM18" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN18" t="n">
         <v>0.2941176470588235</v>
       </c>
-      <c r="AU18" t="n">
+      <c r="BO18" t="n">
         <v>0.2928571428571428</v>
       </c>
-      <c r="AV18" t="n">
+      <c r="BP18" t="n">
         <v>0.506796218487395</v>
       </c>
-      <c r="AW18" t="n">
-        <v>1</v>
-      </c>
-      <c r="AX18" t="n">
-        <v>17</v>
-      </c>
-      <c r="AY18" t="n">
+      <c r="BQ18" t="n">
+        <v>1</v>
+      </c>
+      <c r="BR18" t="n">
         <v>12</v>
       </c>
-      <c r="AZ18" t="n">
+      <c r="BS18" t="n">
         <v>12</v>
       </c>
-      <c r="BA18" t="n">
+      <c r="BT18" t="n">
+        <v>10.33333333333333</v>
+      </c>
+      <c r="BU18" t="n">
         <v>7</v>
       </c>
     </row>
@@ -3497,7 +4617,7 @@
         <v>0.3078616682257471</v>
       </c>
       <c r="J19" t="n">
-        <v>0.05151304988219139</v>
+        <v>0.05085725226374337</v>
       </c>
       <c r="K19" t="n">
         <v>0.5</v>
@@ -3509,13 +4629,13 @@
         <v>0.707167317842221</v>
       </c>
       <c r="N19" t="n">
-        <v>0.9477418889322627</v>
+        <v>0.9483873812150783</v>
       </c>
       <c r="O19" t="n">
-        <v>0.9349409162618966</v>
+        <v>0.9357041989836253</v>
       </c>
       <c r="P19" t="n">
-        <v>0.9726056409760415</v>
+        <v>0.9725097039554158</v>
       </c>
       <c r="Q19" t="n">
         <v>0.9726867961769763</v>
@@ -3533,7 +4653,7 @@
         <v>0.5092942376639913</v>
       </c>
       <c r="V19" t="n">
-        <v>0.4386049770394332</v>
+        <v>0.4702890127744849</v>
       </c>
       <c r="W19" t="n">
         <v>11</v>
@@ -3596,36 +4716,96 @@
         <v>19</v>
       </c>
       <c r="AQ19" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="AR19" t="n">
+        <v>0.04094899095000507</v>
+      </c>
+      <c r="AS19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT19" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU19" t="n">
+        <v>0.08058788315170459</v>
+      </c>
+      <c r="AV19" t="n">
+        <v>0.1161307230901492</v>
+      </c>
+      <c r="AW19" t="n">
+        <v>0.04892181435613313</v>
+      </c>
+      <c r="AX19" t="n">
+        <v>0.01066152940391249</v>
+      </c>
+      <c r="AY19" t="n">
+        <v>0.009235850046772413</v>
+      </c>
+      <c r="AZ19" t="n">
+        <v>0.005085725226374338</v>
+      </c>
+      <c r="BA19" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BB19" t="n">
+        <v>0.01333333333333333</v>
+      </c>
+      <c r="BC19" t="n">
+        <v>0.01414334635684442</v>
+      </c>
+      <c r="BD19" t="n">
+        <v>0.01896774762430157</v>
+      </c>
+      <c r="BE19" t="n">
+        <v>0.01871408397967251</v>
+      </c>
+      <c r="BF19" t="n">
+        <v>0.01945019407910832</v>
+      </c>
+      <c r="BG19" t="n">
+        <v>0.01945373592353953</v>
+      </c>
+      <c r="BH19" t="n">
+        <v>0.01833945628214548</v>
+      </c>
+      <c r="BI19" t="n">
+        <v>0.008672521848406093</v>
+      </c>
+      <c r="BJ19" t="n">
+        <v>0.007456192368802599</v>
+      </c>
+      <c r="BK19" t="n">
+        <v>0.01018588475327983</v>
+      </c>
+      <c r="BL19" t="n">
         <v>0.1875</v>
       </c>
-      <c r="AS19" t="n">
+      <c r="BM19" t="n">
         <v>0.5</v>
       </c>
-      <c r="AT19" t="n">
+      <c r="BN19" t="n">
         <v>0.4705882352941176</v>
       </c>
-      <c r="AU19" t="n">
+      <c r="BO19" t="n">
         <v>0.3357142857142857</v>
       </c>
-      <c r="AV19" t="n">
+      <c r="BP19" t="n">
         <v>0.3771953781512605</v>
       </c>
-      <c r="AW19" t="n">
+      <c r="BQ19" t="n">
         <v>-2</v>
       </c>
-      <c r="AX19" t="n">
-        <v>21</v>
-      </c>
-      <c r="AY19" t="n">
+      <c r="BR19" t="n">
         <v>15</v>
       </c>
-      <c r="AZ19" t="n">
-        <v>19.16666666666667</v>
-      </c>
-      <c r="BA19" t="n">
+      <c r="BS19" t="n">
+        <v>15</v>
+      </c>
+      <c r="BT19" t="n">
+        <v>17.16666666666667</v>
+      </c>
+      <c r="BU19" t="n">
         <v>21.5</v>
       </c>
     </row>
@@ -3660,7 +4840,7 @@
         <v>0.03121194287098504</v>
       </c>
       <c r="J20" t="n">
-        <v>0.00368898591762829</v>
+        <v>0.003671172695361119</v>
       </c>
       <c r="K20" t="n">
         <v>1</v>
@@ -3672,13 +4852,13 @@
         <v>0.7516905071046697</v>
       </c>
       <c r="N20" t="n">
-        <v>0.9424678022651661</v>
+        <v>0.9428556565295528</v>
       </c>
       <c r="O20" t="n">
-        <v>0.9721045193332719</v>
+        <v>0.9722299165549803</v>
       </c>
       <c r="P20" t="n">
-        <v>0.9915700733365406</v>
+        <v>0.9914607377034723</v>
       </c>
       <c r="Q20" t="n">
         <v>0.9795666462366311</v>
@@ -3696,7 +4876,7 @@
         <v>0.7642467673370593</v>
       </c>
       <c r="V20" t="n">
-        <v>0.4572878914140265</v>
+        <v>0.4544937787432675</v>
       </c>
       <c r="W20" t="n">
         <v>23</v>
@@ -3759,36 +4939,96 @@
         <v>3</v>
       </c>
       <c r="AQ20" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="AR20" t="n">
+        <v>0.01477915063178347</v>
+      </c>
+      <c r="AS20" t="n">
+        <v>0.06594064257659667</v>
+      </c>
+      <c r="AT20" t="n">
+        <v>0.02469735297859637</v>
+      </c>
+      <c r="AU20" t="n">
+        <v>0.05978785052942857</v>
+      </c>
+      <c r="AV20" t="n">
+        <v>0.05867071496253538</v>
+      </c>
+      <c r="AW20" t="n">
+        <v>0.03420676821871906</v>
+      </c>
+      <c r="AX20" t="n">
+        <v>0.001395069266947873</v>
+      </c>
+      <c r="AY20" t="n">
+        <v>0.000936358286129551</v>
+      </c>
+      <c r="AZ20" t="n">
+        <v>0.0003671172695361119</v>
+      </c>
+      <c r="BA20" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BB20" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BC20" t="n">
+        <v>0.01503381014209339</v>
+      </c>
+      <c r="BD20" t="n">
+        <v>0.01885711313059106</v>
+      </c>
+      <c r="BE20" t="n">
+        <v>0.01944459833109961</v>
+      </c>
+      <c r="BF20" t="n">
+        <v>0.01982921475406945</v>
+      </c>
+      <c r="BG20" t="n">
+        <v>0.01959133292473262</v>
+      </c>
+      <c r="BH20" t="n">
+        <v>0.01648297820230223</v>
+      </c>
+      <c r="BI20" t="n">
+        <v>0.01799778332936039</v>
+      </c>
+      <c r="BJ20" t="n">
+        <v>0.01119098786200448</v>
+      </c>
+      <c r="BK20" t="n">
+        <v>0.01528493534674119</v>
+      </c>
+      <c r="BL20" t="n">
         <v>0.1875</v>
       </c>
-      <c r="AS20" t="n">
+      <c r="BM20" t="n">
         <v>0.5</v>
       </c>
-      <c r="AT20" t="n">
-        <v>0</v>
-      </c>
-      <c r="AU20" t="n">
+      <c r="BN20" t="n">
+        <v>0</v>
+      </c>
+      <c r="BO20" t="n">
         <v>0.5071428571428573</v>
       </c>
-      <c r="AV20" t="n">
+      <c r="BP20" t="n">
         <v>0.3323214285714285</v>
       </c>
-      <c r="AW20" t="n">
+      <c r="BQ20" t="n">
         <v>-2</v>
       </c>
-      <c r="AX20" t="n">
-        <v>19</v>
-      </c>
-      <c r="AY20" t="n">
+      <c r="BR20" t="n">
+        <v>18</v>
+      </c>
+      <c r="BS20" t="n">
         <v>16</v>
       </c>
-      <c r="AZ20" t="n">
-        <v>18.83333333333333</v>
-      </c>
-      <c r="BA20" t="n">
+      <c r="BT20" t="n">
+        <v>18.5</v>
+      </c>
+      <c r="BU20" t="n">
         <v>21.5</v>
       </c>
     </row>
@@ -3835,13 +5075,13 @@
         <v>0.8455522304855386</v>
       </c>
       <c r="N21" t="n">
-        <v>0.9632609613705454</v>
+        <v>0.9637234925860685</v>
       </c>
       <c r="O21" t="n">
-        <v>0.982653942498781</v>
+        <v>0.9828282441498101</v>
       </c>
       <c r="P21" t="n">
-        <v>0.9971298983628701</v>
+        <v>0.9970952075673054</v>
       </c>
       <c r="Q21" t="n">
         <v>1</v>
@@ -3859,7 +5099,7 @@
         <v>0</v>
       </c>
       <c r="V21" t="n">
-        <v>0.4373181557965208</v>
+        <v>0.3859773319990336</v>
       </c>
       <c r="W21" t="n">
         <v>19</v>
@@ -3922,36 +5162,96 @@
         <v>26</v>
       </c>
       <c r="AQ21" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AR21" t="n">
+        <v>0.02627838837852055</v>
+      </c>
+      <c r="AS21" t="n">
+        <v>0.06385154961361438</v>
+      </c>
+      <c r="AT21" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU21" t="n">
+        <v>0.06104755850907776</v>
+      </c>
+      <c r="AV21" t="n">
+        <v>0.006510189159417494</v>
+      </c>
+      <c r="AW21" t="n">
+        <v>0.02515401216334313</v>
+      </c>
+      <c r="AX21" t="n">
+        <v>0.02334734553039156</v>
+      </c>
+      <c r="AY21" t="n">
+        <v>0.02334734553039156</v>
+      </c>
+      <c r="AZ21" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA21" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BB21" t="n">
+        <v>0.006666666666666666</v>
+      </c>
+      <c r="BC21" t="n">
+        <v>0.01691104460971077</v>
+      </c>
+      <c r="BD21" t="n">
+        <v>0.01927446985172137</v>
+      </c>
+      <c r="BE21" t="n">
+        <v>0.0196565648829962</v>
+      </c>
+      <c r="BF21" t="n">
+        <v>0.01994190415134611</v>
+      </c>
+      <c r="BG21" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BH21" t="n">
+        <v>0.01363213323536615</v>
+      </c>
+      <c r="BI21" t="n">
+        <v>0.01434897970816771</v>
+      </c>
+      <c r="BJ21" t="n">
+        <v>0.00600918000830214</v>
+      </c>
+      <c r="BK21" t="n">
+        <v>0</v>
+      </c>
+      <c r="BL21" t="n">
         <v>0.3125</v>
       </c>
-      <c r="AS21" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT21" t="n">
+      <c r="BM21" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN21" t="n">
         <v>0.6470588235294118</v>
       </c>
-      <c r="AU21" t="n">
+      <c r="BO21" t="n">
         <v>0.6857142857142859</v>
       </c>
-      <c r="AV21" t="n">
+      <c r="BP21" t="n">
         <v>0.2936659663865546</v>
       </c>
-      <c r="AW21" t="n">
+      <c r="BQ21" t="n">
         <v>-2</v>
       </c>
-      <c r="AX21" t="n">
-        <v>22</v>
-      </c>
-      <c r="AY21" t="n">
+      <c r="BR21" t="n">
+        <v>23</v>
+      </c>
+      <c r="BS21" t="n">
         <v>20</v>
       </c>
-      <c r="AZ21" t="n">
-        <v>21.16666666666667</v>
-      </c>
-      <c r="BA21" t="n">
+      <c r="BT21" t="n">
+        <v>21.5</v>
+      </c>
+      <c r="BU21" t="n">
         <v>21.5</v>
       </c>
     </row>
@@ -3986,7 +5286,7 @@
         <v>0.115454103277027</v>
       </c>
       <c r="J22" t="n">
-        <v>0.005523177627823206</v>
+        <v>0.005710230171261709</v>
       </c>
       <c r="K22" t="n">
         <v>0.5</v>
@@ -3998,13 +5298,13 @@
         <v>0.5937883656388702</v>
       </c>
       <c r="N22" t="n">
-        <v>0.9160074037932391</v>
+        <v>0.9123644506386244</v>
       </c>
       <c r="O22" t="n">
-        <v>0.9812122805696908</v>
+        <v>0.9801627136956182</v>
       </c>
       <c r="P22" t="n">
-        <v>0.9947898324937987</v>
+        <v>0.994334806954243</v>
       </c>
       <c r="Q22" t="n">
         <v>0.9729456082296545</v>
@@ -4022,7 +5322,7 @@
         <v>0.2286172874528176</v>
       </c>
       <c r="V22" t="n">
-        <v>0.2314229632698124</v>
+        <v>0.2309624564243025</v>
       </c>
       <c r="W22" t="n">
         <v>26</v>
@@ -4061,7 +5361,7 @@
         <v>23</v>
       </c>
       <c r="AI22" t="n">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="AJ22" t="n">
         <v>6</v>
@@ -4094,27 +5394,87 @@
         <v>0</v>
       </c>
       <c r="AT22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AU22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AV22" t="n">
+        <v>0.04127122614281591</v>
+      </c>
+      <c r="AW22" t="n">
+        <v>0.04264194028596541</v>
+      </c>
+      <c r="AX22" t="n">
+        <v>0.004905524954069453</v>
+      </c>
+      <c r="AY22" t="n">
+        <v>0.00346362309831081</v>
+      </c>
+      <c r="AZ22" t="n">
+        <v>0.000571023017126171</v>
+      </c>
+      <c r="BA22" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BB22" t="n">
+        <v>0</v>
+      </c>
+      <c r="BC22" t="n">
+        <v>0.0118757673127774</v>
+      </c>
+      <c r="BD22" t="n">
+        <v>0.01824728901277249</v>
+      </c>
+      <c r="BE22" t="n">
+        <v>0.01960325427391237</v>
+      </c>
+      <c r="BF22" t="n">
+        <v>0.01988669613908486</v>
+      </c>
+      <c r="BG22" t="n">
+        <v>0.01945891216459309</v>
+      </c>
+      <c r="BH22" t="n">
+        <v>0.01446485427381827</v>
+      </c>
+      <c r="BI22" t="n">
+        <v>0</v>
+      </c>
+      <c r="BJ22" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BK22" t="n">
+        <v>0.004572345749056353</v>
+      </c>
+      <c r="BL22" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM22" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN22" t="n">
         <v>0.4705882352941176</v>
       </c>
-      <c r="AU22" t="n">
+      <c r="BO22" t="n">
         <v>0.3571428571428574</v>
       </c>
-      <c r="AV22" t="n">
+      <c r="BP22" t="n">
         <v>0.1241596638655462</v>
       </c>
-      <c r="AW22" t="n">
+      <c r="BQ22" t="n">
         <v>-2</v>
       </c>
-      <c r="AX22" t="n">
+      <c r="BR22" t="n">
         <v>26</v>
       </c>
-      <c r="AY22" t="n">
+      <c r="BS22" t="n">
         <v>25</v>
       </c>
-      <c r="AZ22" t="n">
+      <c r="BT22" t="n">
         <v>24.16666666666667</v>
       </c>
-      <c r="BA22" t="n">
+      <c r="BU22" t="n">
         <v>21.5</v>
       </c>
     </row>
@@ -4149,7 +5509,7 @@
         <v>0.1885404362048625</v>
       </c>
       <c r="J23" t="n">
-        <v>0.007464989376488444</v>
+        <v>0.007328725160485975</v>
       </c>
       <c r="K23" t="n">
         <v>1</v>
@@ -4161,7 +5521,7 @@
         <v>0.97994766981392</v>
       </c>
       <c r="N23" t="n">
-        <v>0.953472163590055</v>
+        <v>0.9546745594885025</v>
       </c>
       <c r="O23" t="n">
         <v>1</v>
@@ -4185,7 +5545,7 @@
         <v>0.5787608072854405</v>
       </c>
       <c r="V23" t="n">
-        <v>0.4958372626594436</v>
+        <v>0.4579907958015668</v>
       </c>
       <c r="W23" t="n">
         <v>18</v>
@@ -4248,36 +5608,96 @@
         <v>17</v>
       </c>
       <c r="AQ23" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AR23" t="n">
+        <v>0.02821241523393228</v>
+      </c>
+      <c r="AS23" t="n">
+        <v>0.06720347056808218</v>
+      </c>
+      <c r="AT23" t="n">
+        <v>0.02488382206913473</v>
+      </c>
+      <c r="AU23" t="n">
+        <v>0.04501041358053093</v>
+      </c>
+      <c r="AV23" t="n">
+        <v>0.04079274066714316</v>
+      </c>
+      <c r="AW23" t="n">
+        <v>0.04672286299751657</v>
+      </c>
+      <c r="AX23" t="n">
+        <v>0.005839119905989427</v>
+      </c>
+      <c r="AY23" t="n">
+        <v>0.005656213086145874</v>
+      </c>
+      <c r="AZ23" t="n">
+        <v>0.0007328725160485975</v>
+      </c>
+      <c r="BA23" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BB23" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BC23" t="n">
+        <v>0.0195989533962784</v>
+      </c>
+      <c r="BD23" t="n">
+        <v>0.01909349118977005</v>
+      </c>
+      <c r="BE23" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BF23" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BG23" t="n">
+        <v>0.01950652220593192</v>
+      </c>
+      <c r="BH23" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BI23" t="n">
+        <v>0.01417201975304307</v>
+      </c>
+      <c r="BJ23" t="n">
+        <v>0.008990662486310714</v>
+      </c>
+      <c r="BK23" t="n">
+        <v>0.01157521614570881</v>
+      </c>
+      <c r="BL23" t="n">
         <v>0.0625</v>
       </c>
-      <c r="AS23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AT23" t="n">
+      <c r="BM23" t="n">
+        <v>0</v>
+      </c>
+      <c r="BN23" t="n">
         <v>0.8823529411764706</v>
       </c>
-      <c r="AU23" t="n">
+      <c r="BO23" t="n">
         <v>0.8714285714285719</v>
       </c>
-      <c r="AV23" t="n">
+      <c r="BP23" t="n">
         <v>0.2818172268907564</v>
       </c>
-      <c r="AW23" t="n">
-        <v>0</v>
-      </c>
-      <c r="AX23" t="n">
-        <v>15</v>
-      </c>
-      <c r="AY23" t="n">
+      <c r="BQ23" t="n">
+        <v>0</v>
+      </c>
+      <c r="BR23" t="n">
+        <v>17</v>
+      </c>
+      <c r="BS23" t="n">
         <v>22</v>
       </c>
-      <c r="AZ23" t="n">
-        <v>16.5</v>
-      </c>
-      <c r="BA23" t="n">
+      <c r="BT23" t="n">
+        <v>17.16666666666667</v>
+      </c>
+      <c r="BU23" t="n">
         <v>12.5</v>
       </c>
     </row>
@@ -4312,7 +5732,7 @@
         <v>0.1357364506771812</v>
       </c>
       <c r="J24" t="n">
-        <v>0.01353621374987976</v>
+        <v>0.01351120465779231</v>
       </c>
       <c r="K24" t="n">
         <v>1</v>
@@ -4324,13 +5744,13 @@
         <v>0.7026719292295516</v>
       </c>
       <c r="N24" t="n">
-        <v>0.9757567171855086</v>
+        <v>0.9754486248117293</v>
       </c>
       <c r="O24" t="n">
-        <v>0.987942429382592</v>
+        <v>0.9876611422165285</v>
       </c>
       <c r="P24" t="n">
-        <v>0.9927634082115141</v>
+        <v>0.9924815859637466</v>
       </c>
       <c r="Q24" t="n">
         <v>0.9903372093519318</v>
@@ -4348,7 +5768,7 @@
         <v>0.5980596169921902</v>
       </c>
       <c r="V24" t="n">
-        <v>0.496206894603731</v>
+        <v>0.4937093881681514</v>
       </c>
       <c r="W24" t="n">
         <v>25</v>
@@ -4414,33 +5834,93 @@
         <v>14</v>
       </c>
       <c r="AR24" t="n">
-        <v>0</v>
+        <v>0.01107104067766695</v>
       </c>
       <c r="AS24" t="n">
-        <v>1</v>
+        <v>0.0638109896832465</v>
       </c>
       <c r="AT24" t="n">
+        <v>0.02423253416675406</v>
+      </c>
+      <c r="AU24" t="n">
+        <v>0.07460950633997242</v>
+      </c>
+      <c r="AV24" t="n">
+        <v>0.07347232923471532</v>
+      </c>
+      <c r="AW24" t="n">
+        <v>0.04664223454620001</v>
+      </c>
+      <c r="AX24" t="n">
+        <v>0.006175969000526225</v>
+      </c>
+      <c r="AY24" t="n">
+        <v>0.004072093520315436</v>
+      </c>
+      <c r="AZ24" t="n">
+        <v>0.001351120465779232</v>
+      </c>
+      <c r="BA24" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BB24" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BC24" t="n">
+        <v>0.01405343858459103</v>
+      </c>
+      <c r="BD24" t="n">
+        <v>0.01950897249623459</v>
+      </c>
+      <c r="BE24" t="n">
+        <v>0.01975322284433057</v>
+      </c>
+      <c r="BF24" t="n">
+        <v>0.01984963171927493</v>
+      </c>
+      <c r="BG24" t="n">
+        <v>0.01980674418703864</v>
+      </c>
+      <c r="BH24" t="n">
+        <v>0.01742346313984815</v>
+      </c>
+      <c r="BI24" t="n">
+        <v>0.01499633591302417</v>
+      </c>
+      <c r="BJ24" t="n">
+        <v>0.01091856930878927</v>
+      </c>
+      <c r="BK24" t="n">
+        <v>0.0119611923398438</v>
+      </c>
+      <c r="BL24" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM24" t="n">
+        <v>1</v>
+      </c>
+      <c r="BN24" t="n">
         <v>0.2352941176470588</v>
       </c>
-      <c r="AU24" t="n">
+      <c r="BO24" t="n">
         <v>0.4785714285714285</v>
       </c>
-      <c r="AV24" t="n">
+      <c r="BP24" t="n">
         <v>0.5070798319327731</v>
       </c>
-      <c r="AW24" t="n">
+      <c r="BQ24" t="n">
         <v>-2</v>
       </c>
-      <c r="AX24" t="n">
+      <c r="BR24" t="n">
         <v>14</v>
       </c>
-      <c r="AY24" t="n">
+      <c r="BS24" t="n">
         <v>11</v>
       </c>
-      <c r="AZ24" t="n">
+      <c r="BT24" t="n">
         <v>15.5</v>
       </c>
-      <c r="BA24" t="n">
+      <c r="BU24" t="n">
         <v>21.5</v>
       </c>
     </row>
@@ -4475,7 +5955,7 @@
         <v>0</v>
       </c>
       <c r="J25" t="n">
-        <v>0.008418416887212727</v>
+        <v>0.008133979942392271</v>
       </c>
       <c r="K25" t="n">
         <v>1</v>
@@ -4487,13 +5967,13 @@
         <v>0.6807671096239777</v>
       </c>
       <c r="N25" t="n">
-        <v>0.8993275595922393</v>
+        <v>0.9027940688251688</v>
       </c>
       <c r="O25" t="n">
-        <v>0.9352156928307442</v>
+        <v>0.937478257430821</v>
       </c>
       <c r="P25" t="n">
-        <v>0.9902905427629883</v>
+        <v>0.9905022639348643</v>
       </c>
       <c r="Q25" t="n">
         <v>0.9737732379805265</v>
@@ -4511,7 +5991,7 @@
         <v>0.6328647884135252</v>
       </c>
       <c r="V25" t="n">
-        <v>0.4981603003175227</v>
+        <v>0.5254377181455517</v>
       </c>
       <c r="W25" t="n">
         <v>17</v>
@@ -4574,36 +6054,96 @@
         <v>9</v>
       </c>
       <c r="AQ25" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="AR25" t="n">
+        <v>0.03017466069846451</v>
+      </c>
+      <c r="AS25" t="n">
+        <v>0.06444955165734997</v>
+      </c>
+      <c r="AT25" t="n">
+        <v>0.02511898073829573</v>
+      </c>
+      <c r="AU25" t="n">
+        <v>0.1017283761136643</v>
+      </c>
+      <c r="AV25" t="n">
+        <v>0.08006920456687279</v>
+      </c>
+      <c r="AW25" t="n">
+        <v>0.03854393556126941</v>
+      </c>
+      <c r="AX25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AZ25" t="n">
+        <v>0.0008133979942392272</v>
+      </c>
+      <c r="BA25" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BB25" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BC25" t="n">
+        <v>0.01361534219247955</v>
+      </c>
+      <c r="BD25" t="n">
+        <v>0.01805588137650338</v>
+      </c>
+      <c r="BE25" t="n">
+        <v>0.01874956514861642</v>
+      </c>
+      <c r="BF25" t="n">
+        <v>0.01981004527869729</v>
+      </c>
+      <c r="BG25" t="n">
+        <v>0.01947546475961053</v>
+      </c>
+      <c r="BH25" t="n">
+        <v>0.01588537839823659</v>
+      </c>
+      <c r="BI25" t="n">
+        <v>0.01662532106690121</v>
+      </c>
+      <c r="BJ25" t="n">
+        <v>0.009665316826080291</v>
+      </c>
+      <c r="BK25" t="n">
+        <v>0.01265729576827051</v>
+      </c>
+      <c r="BL25" t="n">
         <v>0.0625</v>
       </c>
-      <c r="AS25" t="n">
+      <c r="BM25" t="n">
         <v>0.5</v>
       </c>
-      <c r="AT25" t="n">
+      <c r="BN25" t="n">
         <v>0.1176470588235294</v>
       </c>
-      <c r="AU25" t="n">
+      <c r="BO25" t="n">
         <v>0.6000000000000001</v>
       </c>
-      <c r="AV25" t="n">
+      <c r="BP25" t="n">
         <v>0.3263970588235294</v>
       </c>
-      <c r="AW25" t="n">
+      <c r="BQ25" t="n">
         <v>-2</v>
       </c>
-      <c r="AX25" t="n">
-        <v>12</v>
-      </c>
-      <c r="AY25" t="n">
+      <c r="BR25" t="n">
+        <v>10</v>
+      </c>
+      <c r="BS25" t="n">
         <v>17</v>
       </c>
-      <c r="AZ25" t="n">
-        <v>16.83333333333333</v>
-      </c>
-      <c r="BA25" t="n">
+      <c r="BT25" t="n">
+        <v>16.16666666666667</v>
+      </c>
+      <c r="BU25" t="n">
         <v>21.5</v>
       </c>
     </row>
@@ -4638,7 +6178,7 @@
         <v>0.1100196634514233</v>
       </c>
       <c r="J26" t="n">
-        <v>0.01543089909934837</v>
+        <v>0.01518707855031575</v>
       </c>
       <c r="K26" t="n">
         <v>1</v>
@@ -4650,13 +6190,13 @@
         <v>1</v>
       </c>
       <c r="N26" t="n">
-        <v>0.9549862332951745</v>
+        <v>0.9556932086453609</v>
       </c>
       <c r="O26" t="n">
-        <v>0.9906732482735996</v>
+        <v>0.9907853992293019</v>
       </c>
       <c r="P26" t="n">
-        <v>0.8910425679458738</v>
+        <v>0.8911230427774736</v>
       </c>
       <c r="Q26" t="n">
         <v>0.9733864419457549</v>
@@ -4674,7 +6214,7 @@
         <v>0.5890447667373551</v>
       </c>
       <c r="V26" t="n">
-        <v>0.3903181642401759</v>
+        <v>0.3592683787827005</v>
       </c>
       <c r="W26" t="n">
         <v>21</v>
@@ -4740,33 +6280,93 @@
         <v>24</v>
       </c>
       <c r="AR26" t="n">
-        <v>0</v>
+        <v>0.02286103836000338</v>
       </c>
       <c r="AS26" t="n">
+        <v>0.06495608619048288</v>
+      </c>
+      <c r="AT26" t="n">
+        <v>0.02470562498252974</v>
+      </c>
+      <c r="AU26" t="n">
+        <v>0.04182444447237021</v>
+      </c>
+      <c r="AV26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AW26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AX26" t="n">
+        <v>0.004054782153892753</v>
+      </c>
+      <c r="AY26" t="n">
+        <v>0.0033005899035427</v>
+      </c>
+      <c r="AZ26" t="n">
+        <v>0.001518707855031575</v>
+      </c>
+      <c r="BA26" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BB26" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BC26" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BD26" t="n">
+        <v>0.01911386417290722</v>
+      </c>
+      <c r="BE26" t="n">
+        <v>0.01981570798458604</v>
+      </c>
+      <c r="BF26" t="n">
+        <v>0.01782246085554947</v>
+      </c>
+      <c r="BG26" t="n">
+        <v>0.0194677288389151</v>
+      </c>
+      <c r="BH26" t="n">
+        <v>0.01920646583394563</v>
+      </c>
+      <c r="BI26" t="n">
+        <v>0.01884166276568639</v>
+      </c>
+      <c r="BJ26" t="n">
+        <v>0.009998319078510363</v>
+      </c>
+      <c r="BK26" t="n">
+        <v>0.0117808953347471</v>
+      </c>
+      <c r="BL26" t="n">
+        <v>0</v>
+      </c>
+      <c r="BM26" t="n">
         <v>0.5</v>
       </c>
-      <c r="AT26" t="n">
+      <c r="BN26" t="n">
         <v>0.4117647058823529</v>
       </c>
-      <c r="AU26" t="n">
+      <c r="BO26" t="n">
         <v>0.2000000000000001</v>
       </c>
-      <c r="AV26" t="n">
+      <c r="BP26" t="n">
         <v>0.291764705882353</v>
       </c>
-      <c r="AW26" t="n">
+      <c r="BQ26" t="n">
         <v>-2</v>
       </c>
-      <c r="AX26" t="n">
+      <c r="BR26" t="n">
         <v>24</v>
       </c>
-      <c r="AY26" t="n">
+      <c r="BS26" t="n">
         <v>21</v>
       </c>
-      <c r="AZ26" t="n">
+      <c r="BT26" t="n">
         <v>22.16666666666667</v>
       </c>
-      <c r="BA26" t="n">
+      <c r="BU26" t="n">
         <v>21.5</v>
       </c>
     </row>
@@ -4801,7 +6401,7 @@
         <v>0.04961315421093695</v>
       </c>
       <c r="J27" t="n">
-        <v>0.005024446549070471</v>
+        <v>0.004947929937497759</v>
       </c>
       <c r="K27" t="n">
         <v>0.5</v>
@@ -4816,7 +6416,7 @@
         <v>1</v>
       </c>
       <c r="O27" t="n">
-        <v>0.9763364213360979</v>
+        <v>0.976650427011825</v>
       </c>
       <c r="P27" t="n">
         <v>0</v>
@@ -4837,7 +6437,7 @@
         <v>1</v>
       </c>
       <c r="V27" t="n">
-        <v>0.4274328096663137</v>
+        <v>0.4222378676291156</v>
       </c>
       <c r="W27" t="n">
         <v>22</v>
@@ -4900,36 +6500,96 @@
         <v>1</v>
       </c>
       <c r="AQ27" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AR27" t="n">
-        <v>1</v>
+        <v>0.02013414521209257</v>
       </c>
       <c r="AS27" t="n">
+        <v>0.06351918028679968</v>
+      </c>
+      <c r="AT27" t="n">
+        <v>0.02504962872539317</v>
+      </c>
+      <c r="AU27" t="n">
+        <v>0.002551794761192221</v>
+      </c>
+      <c r="AV27" t="n">
+        <v>0.1100498072116249</v>
+      </c>
+      <c r="AW27" t="n">
+        <v>0.03883886993379959</v>
+      </c>
+      <c r="AX27" t="n">
+        <v>0.002526707340400348</v>
+      </c>
+      <c r="AY27" t="n">
+        <v>0.001488394626328108</v>
+      </c>
+      <c r="AZ27" t="n">
+        <v>0.0004947929937497759</v>
+      </c>
+      <c r="BA27" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="BB27" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BC27" t="n">
+        <v>0.01552472943819641</v>
+      </c>
+      <c r="BD27" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BE27" t="n">
+        <v>0.0195330085402365</v>
+      </c>
+      <c r="BF27" t="n">
+        <v>0</v>
+      </c>
+      <c r="BG27" t="n">
+        <v>0.01972753632256514</v>
+      </c>
+      <c r="BH27" t="n">
+        <v>0.01971099681606662</v>
+      </c>
+      <c r="BI27" t="n">
+        <v>0.0003232327460445701</v>
+      </c>
+      <c r="BJ27" t="n">
+        <v>0.01276504267462604</v>
+      </c>
+      <c r="BK27" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="BL27" t="n">
+        <v>1</v>
+      </c>
+      <c r="BM27" t="n">
         <v>0.5</v>
       </c>
-      <c r="AT27" t="n">
-        <v>1</v>
-      </c>
-      <c r="AU27" t="n">
+      <c r="BN27" t="n">
+        <v>1</v>
+      </c>
+      <c r="BO27" t="n">
         <v>0.5428571428571433</v>
       </c>
-      <c r="AV27" t="n">
+      <c r="BP27" t="n">
         <v>0.7314285714285715</v>
       </c>
-      <c r="AW27" t="n">
+      <c r="BQ27" t="n">
         <v>-2</v>
       </c>
-      <c r="AX27" t="n">
-        <v>23</v>
-      </c>
-      <c r="AY27" t="n">
+      <c r="BR27" t="n">
+        <v>22</v>
+      </c>
+      <c r="BS27" t="n">
         <v>2</v>
       </c>
-      <c r="AZ27" t="n">
-        <v>15.5</v>
-      </c>
-      <c r="BA27" t="n">
+      <c r="BT27" t="n">
+        <v>15.16666666666667</v>
+      </c>
+      <c r="BU27" t="n">
         <v>21.5</v>
       </c>
     </row>

</xml_diff>